<commit_message>
Arquivo:03 - Formatação Condicional
</commit_message>
<xml_diff>
--- a/03-Meteora_Ecommerce-Graficos-Formatos.xlsx
+++ b/03-Meteora_Ecommerce-Graficos-Formatos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafae\Meu Drive (mz.tears.of.time@gmail.com)\Dev\Cursos\Curso-003\001 - Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BC63186-1A15-41E8-A47B-9886677F4D1E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ADFB8CA-4776-490A-A51D-A71529BA5786}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="17280" windowHeight="7800" firstSheet="2" activeTab="3" xr2:uid="{F6D97A53-F63B-4272-A181-44B26E0B790F}"/>
+    <workbookView xWindow="930" yWindow="0" windowWidth="23070" windowHeight="11505" firstSheet="2" activeTab="2" xr2:uid="{F6D97A53-F63B-4272-A181-44B26E0B790F}"/>
   </bookViews>
   <sheets>
     <sheet name="Meu Gráfico" sheetId="6" state="hidden" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="90">
   <si>
     <t>Produtos</t>
   </si>
@@ -307,6 +307,9 @@
   </si>
   <si>
     <t>Estoque</t>
+  </si>
+  <si>
+    <t>Situação</t>
   </si>
 </sst>
 </file>
@@ -777,7 +780,116 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Título Meteora" xfId="2" xr:uid="{52F1EA3C-B23E-4AE6-AE73-27AD9F7C9021}"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="25">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -812,40 +924,6 @@
           <bgColor theme="1"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
@@ -885,7 +963,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[03-Meteora_Ecommerce-AULA_INICIAL.xlsx]Planilha3!Tabela dinâmica85</c:name>
+    <c:name>[03-Meteora_Ecommerce-Graficos-Formatos.xlsx]Planilha3!Tabela dinâmica85</c:name>
     <c:fmtId val="1"/>
   </c:pivotSource>
   <c:chart>
@@ -2099,7 +2177,7 @@
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Office Resolve Testes" refreshedDate="45091.695904398148" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="39" xr:uid="{D9D057AD-0FAE-4908-B186-309A9CA94BEA}">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A3:G42" sheet="Produtos"/>
+    <worksheetSource ref="A3:H42" sheet="Produtos"/>
   </cacheSource>
   <cacheFields count="7">
     <cacheField name="Produtos" numFmtId="0">
@@ -2682,36 +2760,37 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{40AC111B-A369-4C0B-9503-7C5B9442DAEA}" name="TB_Produtos" displayName="TB_Produtos" ref="A3:F42" totalsRowShown="0" headerRowDxfId="14">
-  <autoFilter ref="A3:F42" xr:uid="{40AC111B-A369-4C0B-9503-7C5B9442DAEA}"/>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{2F8ED5FF-48A1-488E-9DF1-FE060F71A415}" name="Código"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{40AC111B-A369-4C0B-9503-7C5B9442DAEA}" name="TB_Produtos" displayName="TB_Produtos" ref="A3:G42" headerRowDxfId="12">
+  <autoFilter ref="A3:G42" xr:uid="{40AC111B-A369-4C0B-9503-7C5B9442DAEA}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{2F8ED5FF-48A1-488E-9DF1-FE060F71A415}" name="Código" totalsRowLabel="Total"/>
     <tableColumn id="2" xr3:uid="{E100D4E2-C3A0-43FF-A1D9-90A4BC2A9918}" name="Produtos"/>
-    <tableColumn id="3" xr3:uid="{2EF7FEE0-6B6F-4534-86A0-46B6555B7BEF}" name="Tamanho" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{2EF7FEE0-6B6F-4534-86A0-46B6555B7BEF}" name="Tamanho" dataDxfId="10" totalsRowDxfId="11"/>
     <tableColumn id="4" xr3:uid="{4435A4B8-E7F0-4D66-A4F8-6A9FEAA36D5A}" name="Categoria"/>
-    <tableColumn id="6" xr3:uid="{15F9CACC-A558-4A20-80CF-C2ADA2603221}" name="Estoque" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{CA8AD0DE-58EC-4839-85FB-1DD75DA28087}" name="Preço Unitário" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{15F9CACC-A558-4A20-80CF-C2ADA2603221}" name="Estoque" dataDxfId="8" totalsRowDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{3D723964-A53C-4456-A86F-04BE235E4F0C}" name="Situação" dataDxfId="6" totalsRowDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{CA8AD0DE-58EC-4839-85FB-1DD75DA28087}" name="Preço Unitário" totalsRowFunction="sum" dataDxfId="4" totalsRowDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{AD739091-30BD-4C30-BDDA-7504C0C4B6E2}" name="TB_Vendas" displayName="TB_Vendas" ref="A2:H61" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8" headerRowCellStyle="Cabeçalho Meteora">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{AD739091-30BD-4C30-BDDA-7504C0C4B6E2}" name="TB_Vendas" displayName="TB_Vendas" ref="A2:H61" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23" headerRowCellStyle="Cabeçalho Meteora">
   <autoFilter ref="A2:H61" xr:uid="{AD739091-30BD-4C30-BDDA-7504C0C4B6E2}"/>
   <tableColumns count="8">
-    <tableColumn id="7" xr3:uid="{5E8DE7C3-CDB6-4314-A5CC-C44D3C21973F}" name="Mês" dataDxfId="7">
+    <tableColumn id="7" xr3:uid="{5E8DE7C3-CDB6-4314-A5CC-C44D3C21973F}" name="Mês" dataDxfId="22">
       <calculatedColumnFormula>MONTH(TB_Vendas[[#This Row],[Data]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{43632F1F-6978-4CE7-BB13-7CCE587D6821}" name="Data" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{49DF5362-33BE-4541-BD47-0B512249381E}" name="Código" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{B3C718A1-FEFF-4C65-9CA1-DF94EF755918}" name="Tamanho" dataDxfId="4">
+    <tableColumn id="1" xr3:uid="{43632F1F-6978-4CE7-BB13-7CCE587D6821}" name="Data" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{49DF5362-33BE-4541-BD47-0B512249381E}" name="Código" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{B3C718A1-FEFF-4C65-9CA1-DF94EF755918}" name="Tamanho" dataDxfId="19">
       <calculatedColumnFormula>_xlfn.XLOOKUP(C3,TB_Produtos[Código],TB_Produtos[Tamanho])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{1F3EAF93-84E7-4086-BE54-3AB7D71B21A8}" name="Categoria" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{7DC2ADED-AF8A-4BC8-A38E-FEF676FE49C9}" name="Qtd" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{9459B662-6A4F-4486-82B1-12F67B8F842E}" name="Total" dataDxfId="1"/>
-    <tableColumn id="8" xr3:uid="{192FEBCA-1287-48A6-9BE6-69528F71C305}" name="Vendedor" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{1F3EAF93-84E7-4086-BE54-3AB7D71B21A8}" name="Categoria" dataDxfId="18"/>
+    <tableColumn id="5" xr3:uid="{7DC2ADED-AF8A-4BC8-A38E-FEF676FE49C9}" name="Qtd" dataDxfId="17"/>
+    <tableColumn id="6" xr3:uid="{9459B662-6A4F-4486-82B1-12F67B8F842E}" name="Total" dataDxfId="16"/>
+    <tableColumn id="8" xr3:uid="{192FEBCA-1287-48A6-9BE6-69528F71C305}" name="Vendedor" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3185,10 +3264,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8ADA2D8-DE9E-4ACF-B5A7-8907124C5CF1}">
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3197,11 +3276,11 @@
     <col min="2" max="2" width="15.5703125" customWidth="1"/>
     <col min="3" max="3" width="11.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1"/>
-    <col min="6" max="6" width="21.7109375" customWidth="1"/>
+    <col min="5" max="6" width="12.28515625" customWidth="1"/>
+    <col min="7" max="7" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="33" t="s">
         <v>15</v>
       </c>
@@ -3210,16 +3289,18 @@
       <c r="D1" s="33"/>
       <c r="E1" s="33"/>
       <c r="F1" s="33"/>
-    </row>
-    <row r="2" spans="1:6" ht="4.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G1" s="33"/>
+    </row>
+    <row r="2" spans="1:7" ht="4.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="1:6" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="27" t="s">
         <v>41</v>
       </c>
@@ -3236,10 +3317,13 @@
         <v>88</v>
       </c>
       <c r="F3" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="G3" s="27" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -3255,11 +3339,15 @@
       <c r="E4" s="1">
         <v>12</v>
       </c>
-      <c r="F4" s="28">
+      <c r="F4" s="1">
+        <f>TB_Produtos[[#This Row],[Estoque]]</f>
+        <v>12</v>
+      </c>
+      <c r="G4" s="28">
         <v>65.900000000000006</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -3275,11 +3363,15 @@
       <c r="E5" s="1">
         <v>15</v>
       </c>
-      <c r="F5" s="28">
+      <c r="F5" s="1">
+        <f>TB_Produtos[[#This Row],[Estoque]]</f>
+        <v>15</v>
+      </c>
+      <c r="G5" s="28">
         <v>69.900000000000006</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>45</v>
       </c>
@@ -3295,11 +3387,15 @@
       <c r="E6" s="1">
         <v>5</v>
       </c>
-      <c r="F6" s="28">
+      <c r="F6" s="1">
+        <f>TB_Produtos[[#This Row],[Estoque]]</f>
+        <v>5</v>
+      </c>
+      <c r="G6" s="28">
         <v>70.900000000000006</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>46</v>
       </c>
@@ -3315,11 +3411,15 @@
       <c r="E7" s="1">
         <v>2</v>
       </c>
-      <c r="F7" s="28">
+      <c r="F7" s="1">
+        <f>TB_Produtos[[#This Row],[Estoque]]</f>
+        <v>2</v>
+      </c>
+      <c r="G7" s="28">
         <v>145</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>47</v>
       </c>
@@ -3335,11 +3435,15 @@
       <c r="E8" s="1">
         <v>1</v>
       </c>
-      <c r="F8" s="28">
+      <c r="F8" s="1">
+        <f>TB_Produtos[[#This Row],[Estoque]]</f>
+        <v>1</v>
+      </c>
+      <c r="G8" s="28">
         <v>259.89999999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>48</v>
       </c>
@@ -3355,11 +3459,15 @@
       <c r="E9" s="1">
         <v>11</v>
       </c>
-      <c r="F9" s="28">
+      <c r="F9" s="1">
+        <f>TB_Produtos[[#This Row],[Estoque]]</f>
+        <v>11</v>
+      </c>
+      <c r="G9" s="28">
         <v>39.9</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>49</v>
       </c>
@@ -3375,11 +3483,15 @@
       <c r="E10" s="1">
         <v>6</v>
       </c>
-      <c r="F10" s="28">
+      <c r="F10" s="1">
+        <f>TB_Produtos[[#This Row],[Estoque]]</f>
+        <v>6</v>
+      </c>
+      <c r="G10" s="28">
         <v>85.9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>50</v>
       </c>
@@ -3395,11 +3507,15 @@
       <c r="E11" s="1">
         <v>5</v>
       </c>
-      <c r="F11" s="28">
+      <c r="F11" s="1">
+        <f>TB_Produtos[[#This Row],[Estoque]]</f>
+        <v>5</v>
+      </c>
+      <c r="G11" s="28">
         <v>89.9</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>51</v>
       </c>
@@ -3415,11 +3531,15 @@
       <c r="E12" s="1">
         <v>8</v>
       </c>
-      <c r="F12" s="28">
+      <c r="F12" s="1">
+        <f>TB_Produtos[[#This Row],[Estoque]]</f>
+        <v>8</v>
+      </c>
+      <c r="G12" s="28">
         <v>92.9</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>52</v>
       </c>
@@ -3435,11 +3555,15 @@
       <c r="E13" s="1">
         <v>2</v>
       </c>
-      <c r="F13" s="28">
+      <c r="F13" s="1">
+        <f>TB_Produtos[[#This Row],[Estoque]]</f>
+        <v>2</v>
+      </c>
+      <c r="G13" s="28">
         <v>44.9</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>53</v>
       </c>
@@ -3455,11 +3579,15 @@
       <c r="E14" s="1">
         <v>3</v>
       </c>
-      <c r="F14" s="28">
+      <c r="F14" s="1">
+        <f>TB_Produtos[[#This Row],[Estoque]]</f>
+        <v>3</v>
+      </c>
+      <c r="G14" s="28">
         <v>46.9</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>54</v>
       </c>
@@ -3475,11 +3603,15 @@
       <c r="E15" s="1">
         <v>5</v>
       </c>
-      <c r="F15" s="28">
+      <c r="F15" s="1">
+        <f>TB_Produtos[[#This Row],[Estoque]]</f>
+        <v>5</v>
+      </c>
+      <c r="G15" s="28">
         <v>48.9</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>55</v>
       </c>
@@ -3495,11 +3627,15 @@
       <c r="E16" s="1">
         <v>6</v>
       </c>
-      <c r="F16" s="28">
+      <c r="F16" s="1">
+        <f>TB_Produtos[[#This Row],[Estoque]]</f>
+        <v>6</v>
+      </c>
+      <c r="G16" s="28">
         <v>39.9</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>56</v>
       </c>
@@ -3515,11 +3651,15 @@
       <c r="E17" s="1">
         <v>10</v>
       </c>
-      <c r="F17" s="28">
+      <c r="F17" s="1">
+        <f>TB_Produtos[[#This Row],[Estoque]]</f>
+        <v>10</v>
+      </c>
+      <c r="G17" s="28">
         <v>39.9</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>57</v>
       </c>
@@ -3535,11 +3675,15 @@
       <c r="E18" s="1">
         <v>12</v>
       </c>
-      <c r="F18" s="28">
+      <c r="F18" s="1">
+        <f>TB_Produtos[[#This Row],[Estoque]]</f>
+        <v>12</v>
+      </c>
+      <c r="G18" s="28">
         <v>42.5</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>58</v>
       </c>
@@ -3555,11 +3699,15 @@
       <c r="E19" s="1">
         <v>6</v>
       </c>
-      <c r="F19" s="28">
+      <c r="F19" s="1">
+        <f>TB_Produtos[[#This Row],[Estoque]]</f>
+        <v>6</v>
+      </c>
+      <c r="G19" s="28">
         <v>25.9</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>59</v>
       </c>
@@ -3575,11 +3723,15 @@
       <c r="E20" s="1">
         <v>10</v>
       </c>
-      <c r="F20" s="28">
+      <c r="F20" s="1">
+        <f>TB_Produtos[[#This Row],[Estoque]]</f>
+        <v>10</v>
+      </c>
+      <c r="G20" s="28">
         <v>29.9</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>60</v>
       </c>
@@ -3595,11 +3747,15 @@
       <c r="E21" s="1">
         <v>12</v>
       </c>
-      <c r="F21" s="28">
+      <c r="F21" s="1">
+        <f>TB_Produtos[[#This Row],[Estoque]]</f>
+        <v>12</v>
+      </c>
+      <c r="G21" s="28">
         <v>32.9</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>61</v>
       </c>
@@ -3615,11 +3771,15 @@
       <c r="E22" s="1">
         <v>21</v>
       </c>
-      <c r="F22" s="28">
+      <c r="F22" s="1">
+        <f>TB_Produtos[[#This Row],[Estoque]]</f>
+        <v>21</v>
+      </c>
+      <c r="G22" s="28">
         <v>49.9</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>62</v>
       </c>
@@ -3635,11 +3795,15 @@
       <c r="E23" s="1">
         <v>5</v>
       </c>
-      <c r="F23" s="28">
+      <c r="F23" s="1">
+        <f>TB_Produtos[[#This Row],[Estoque]]</f>
+        <v>5</v>
+      </c>
+      <c r="G23" s="28">
         <v>299.89999999999998</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>63</v>
       </c>
@@ -3655,11 +3819,15 @@
       <c r="E24" s="1">
         <v>5</v>
       </c>
-      <c r="F24" s="28">
+      <c r="F24" s="1">
+        <f>TB_Produtos[[#This Row],[Estoque]]</f>
+        <v>5</v>
+      </c>
+      <c r="G24" s="28">
         <v>302.89999999999998</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>64</v>
       </c>
@@ -3675,11 +3843,15 @@
       <c r="E25" s="1">
         <v>5</v>
       </c>
-      <c r="F25" s="28">
+      <c r="F25" s="1">
+        <f>TB_Produtos[[#This Row],[Estoque]]</f>
+        <v>5</v>
+      </c>
+      <c r="G25" s="28">
         <v>300</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>65</v>
       </c>
@@ -3695,11 +3867,15 @@
       <c r="E26" s="1">
         <v>5</v>
       </c>
-      <c r="F26" s="28">
+      <c r="F26" s="1">
+        <f>TB_Produtos[[#This Row],[Estoque]]</f>
+        <v>5</v>
+      </c>
+      <c r="G26" s="28">
         <v>249.9</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>66</v>
       </c>
@@ -3715,11 +3891,15 @@
       <c r="E27" s="1">
         <v>5</v>
       </c>
-      <c r="F27" s="28">
+      <c r="F27" s="1">
+        <f>TB_Produtos[[#This Row],[Estoque]]</f>
+        <v>5</v>
+      </c>
+      <c r="G27" s="28">
         <v>259.89999999999998</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>67</v>
       </c>
@@ -3735,11 +3915,15 @@
       <c r="E28" s="1">
         <v>5</v>
       </c>
-      <c r="F28" s="28">
+      <c r="F28" s="1">
+        <f>TB_Produtos[[#This Row],[Estoque]]</f>
+        <v>5</v>
+      </c>
+      <c r="G28" s="28">
         <v>299.89999999999998</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>68</v>
       </c>
@@ -3755,11 +3939,15 @@
       <c r="E29" s="1">
         <v>3</v>
       </c>
-      <c r="F29" s="28">
+      <c r="F29" s="1">
+        <f>TB_Produtos[[#This Row],[Estoque]]</f>
+        <v>3</v>
+      </c>
+      <c r="G29" s="28">
         <v>349.9</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>69</v>
       </c>
@@ -3775,11 +3963,15 @@
       <c r="E30" s="1">
         <v>3</v>
       </c>
-      <c r="F30" s="28">
+      <c r="F30" s="1">
+        <f>TB_Produtos[[#This Row],[Estoque]]</f>
+        <v>3</v>
+      </c>
+      <c r="G30" s="28">
         <v>399.9</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>70</v>
       </c>
@@ -3795,11 +3987,15 @@
       <c r="E31" s="1">
         <v>5</v>
       </c>
-      <c r="F31" s="28">
+      <c r="F31" s="1">
+        <f>TB_Produtos[[#This Row],[Estoque]]</f>
+        <v>5</v>
+      </c>
+      <c r="G31" s="28">
         <v>249.9</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>71</v>
       </c>
@@ -3815,11 +4011,15 @@
       <c r="E32" s="1">
         <v>3</v>
       </c>
-      <c r="F32" s="28">
+      <c r="F32" s="1">
+        <f>TB_Produtos[[#This Row],[Estoque]]</f>
+        <v>3</v>
+      </c>
+      <c r="G32" s="28">
         <v>255</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>72</v>
       </c>
@@ -3835,11 +4035,15 @@
       <c r="E33" s="1">
         <v>5</v>
       </c>
-      <c r="F33" s="28">
+      <c r="F33" s="1">
+        <f>TB_Produtos[[#This Row],[Estoque]]</f>
+        <v>5</v>
+      </c>
+      <c r="G33" s="28">
         <v>259.89999999999998</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>73</v>
       </c>
@@ -3855,11 +4059,15 @@
       <c r="E34" s="1">
         <v>5</v>
       </c>
-      <c r="F34" s="28">
+      <c r="F34" s="1">
+        <f>TB_Produtos[[#This Row],[Estoque]]</f>
+        <v>5</v>
+      </c>
+      <c r="G34" s="28">
         <v>199.9</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>74</v>
       </c>
@@ -3875,11 +4083,15 @@
       <c r="E35" s="1">
         <v>5</v>
       </c>
-      <c r="F35" s="28">
+      <c r="F35" s="1">
+        <f>TB_Produtos[[#This Row],[Estoque]]</f>
+        <v>5</v>
+      </c>
+      <c r="G35" s="28">
         <v>249.9</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>75</v>
       </c>
@@ -3895,11 +4107,15 @@
       <c r="E36" s="1">
         <v>5</v>
       </c>
-      <c r="F36" s="28">
+      <c r="F36" s="1">
+        <f>TB_Produtos[[#This Row],[Estoque]]</f>
+        <v>5</v>
+      </c>
+      <c r="G36" s="28">
         <v>259.89999999999998</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>76</v>
       </c>
@@ -3915,11 +4131,15 @@
       <c r="E37" s="1">
         <v>3</v>
       </c>
-      <c r="F37" s="28">
+      <c r="F37" s="1">
+        <f>TB_Produtos[[#This Row],[Estoque]]</f>
+        <v>3</v>
+      </c>
+      <c r="G37" s="28">
         <v>89.9</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>77</v>
       </c>
@@ -3935,11 +4155,15 @@
       <c r="E38" s="1">
         <v>3</v>
       </c>
-      <c r="F38" s="28">
+      <c r="F38" s="1">
+        <f>TB_Produtos[[#This Row],[Estoque]]</f>
+        <v>3</v>
+      </c>
+      <c r="G38" s="28">
         <v>91.4</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>78</v>
       </c>
@@ -3955,11 +4179,15 @@
       <c r="E39" s="1">
         <v>3</v>
       </c>
-      <c r="F39" s="28">
+      <c r="F39" s="1">
+        <f>TB_Produtos[[#This Row],[Estoque]]</f>
+        <v>3</v>
+      </c>
+      <c r="G39" s="28">
         <v>93.5</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>79</v>
       </c>
@@ -3975,11 +4203,15 @@
       <c r="E40" s="1">
         <v>2</v>
       </c>
-      <c r="F40" s="28">
+      <c r="F40" s="1">
+        <f>TB_Produtos[[#This Row],[Estoque]]</f>
+        <v>2</v>
+      </c>
+      <c r="G40" s="28">
         <v>140</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>80</v>
       </c>
@@ -3995,11 +4227,15 @@
       <c r="E41" s="1">
         <v>2</v>
       </c>
-      <c r="F41" s="28">
+      <c r="F41" s="1">
+        <f>TB_Produtos[[#This Row],[Estoque]]</f>
+        <v>2</v>
+      </c>
+      <c r="G41" s="28">
         <v>142.9</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>81</v>
       </c>
@@ -4015,18 +4251,65 @@
       <c r="E42" s="1">
         <v>2</v>
       </c>
-      <c r="F42" s="28">
+      <c r="F42" s="1">
+        <f>TB_Produtos[[#This Row],[Estoque]]</f>
+        <v>2</v>
+      </c>
+      <c r="G42" s="28">
         <v>146</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A1:G1"/>
   </mergeCells>
+  <conditionalFormatting sqref="F4:F42">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="lessThan">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="iconSet" priority="2">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="3"/>
+        <cfvo type="num" val="10" gte="0"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G4:G42">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFDAFF01"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{288B949B-9CE8-47BA-A0AE-8CCE5611B9F9}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{288B949B-9CE8-47BA-A0AE-8CCE5611B9F9}">
+            <x14:dataBar minLength="0" maxLength="100" direction="rightToLeft">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>G4:G42</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4034,8 +4317,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BF34D44-0E29-4A7F-B47B-66AF094D5F9D}">
   <dimension ref="A1:H61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5745,7 +6028,7 @@
     <mergeCell ref="A1:H1"/>
   </mergeCells>
   <conditionalFormatting sqref="F2">
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Arquivo:03 - Formatação e modelo para Dashboard
</commit_message>
<xml_diff>
--- a/03-Meteora_Ecommerce-Graficos-Formatos.xlsx
+++ b/03-Meteora_Ecommerce-Graficos-Formatos.xlsx
@@ -8,28 +8,29 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafae\Meu Drive (mz.tears.of.time@gmail.com)\Dev\Cursos\Curso-003\001 - Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ADFB8CA-4776-490A-A51D-A71529BA5786}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36EF3DD9-40B9-4769-B864-2E012969786A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="23070" windowHeight="11505" firstSheet="2" activeTab="2" xr2:uid="{F6D97A53-F63B-4272-A181-44B26E0B790F}"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="23070" windowHeight="11505" firstSheet="2" activeTab="3" xr2:uid="{F6D97A53-F63B-4272-A181-44B26E0B790F}"/>
   </bookViews>
   <sheets>
     <sheet name="Meu Gráfico" sheetId="6" state="hidden" r:id="rId1"/>
     <sheet name="Planilha3" sheetId="5" state="hidden" r:id="rId2"/>
     <sheet name="Produtos" sheetId="17" r:id="rId3"/>
-    <sheet name="Vendas" sheetId="16" r:id="rId4"/>
-    <sheet name="Meus Números (Tabela)" sheetId="12" state="hidden" r:id="rId5"/>
-    <sheet name="Filtro Avançado" sheetId="9" state="hidden" r:id="rId6"/>
+    <sheet name="Dashboard" sheetId="18" r:id="rId4"/>
+    <sheet name="Vendas" sheetId="16" r:id="rId5"/>
+    <sheet name="Meus Números (Tabela)" sheetId="12" state="hidden" r:id="rId6"/>
+    <sheet name="Filtro Avançado" sheetId="9" state="hidden" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Vendas!$B$2:$F$61</definedName>
-    <definedName name="_xlnm.Extract" localSheetId="5">'Filtro Avançado'!$B$6:$H$6</definedName>
-    <definedName name="_xlnm.Criteria" localSheetId="5">'Filtro Avançado'!$B$2:$C$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Vendas!$B$2:$F$61</definedName>
+    <definedName name="_xlnm.Extract" localSheetId="6">'Filtro Avançado'!$B$6:$H$6</definedName>
+    <definedName name="_xlnm.Criteria" localSheetId="6">'Filtro Avançado'!$B$2:$C$3</definedName>
     <definedName name="Int_Nome_Produtos">#REF!</definedName>
     <definedName name="Int_Quantidade">#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId7"/>
+    <pivotCache cacheId="0" r:id="rId8"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -780,52 +781,50 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Título Meteora" xfId="2" xr:uid="{52F1EA3C-B23E-4AE6-AE73-27AD9F7C9021}"/>
   </cellStyles>
-  <dxfs count="25">
+  <dxfs count="21">
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
-          <bgColor theme="8" tint="-0.24994659260841701"/>
+          <bgColor theme="1"/>
         </patternFill>
       </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
+        <color rgb="FF9C0006"/>
       </font>
       <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="8" tint="-0.24994659260841701"/>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -870,61 +869,15 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <b/>
         <i val="0"/>
         <color theme="1"/>
       </font>
       <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
+        <patternFill patternType="solid">
+          <bgColor theme="8" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2760,37 +2713,37 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{40AC111B-A369-4C0B-9503-7C5B9442DAEA}" name="TB_Produtos" displayName="TB_Produtos" ref="A3:G42" headerRowDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{40AC111B-A369-4C0B-9503-7C5B9442DAEA}" name="TB_Produtos" displayName="TB_Produtos" ref="A3:G42" headerRowDxfId="19">
   <autoFilter ref="A3:G42" xr:uid="{40AC111B-A369-4C0B-9503-7C5B9442DAEA}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{2F8ED5FF-48A1-488E-9DF1-FE060F71A415}" name="Código" totalsRowLabel="Total"/>
     <tableColumn id="2" xr3:uid="{E100D4E2-C3A0-43FF-A1D9-90A4BC2A9918}" name="Produtos"/>
-    <tableColumn id="3" xr3:uid="{2EF7FEE0-6B6F-4534-86A0-46B6555B7BEF}" name="Tamanho" dataDxfId="10" totalsRowDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{2EF7FEE0-6B6F-4534-86A0-46B6555B7BEF}" name="Tamanho" dataDxfId="18" totalsRowDxfId="17"/>
     <tableColumn id="4" xr3:uid="{4435A4B8-E7F0-4D66-A4F8-6A9FEAA36D5A}" name="Categoria"/>
-    <tableColumn id="6" xr3:uid="{15F9CACC-A558-4A20-80CF-C2ADA2603221}" name="Estoque" dataDxfId="8" totalsRowDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{3D723964-A53C-4456-A86F-04BE235E4F0C}" name="Situação" dataDxfId="6" totalsRowDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{CA8AD0DE-58EC-4839-85FB-1DD75DA28087}" name="Preço Unitário" totalsRowFunction="sum" dataDxfId="4" totalsRowDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{15F9CACC-A558-4A20-80CF-C2ADA2603221}" name="Estoque" dataDxfId="16" totalsRowDxfId="15"/>
+    <tableColumn id="7" xr3:uid="{3D723964-A53C-4456-A86F-04BE235E4F0C}" name="Situação" dataDxfId="14" totalsRowDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{CA8AD0DE-58EC-4839-85FB-1DD75DA28087}" name="Preço Unitário" totalsRowFunction="sum" dataDxfId="12" totalsRowDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{AD739091-30BD-4C30-BDDA-7504C0C4B6E2}" name="TB_Vendas" displayName="TB_Vendas" ref="A2:H61" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23" headerRowCellStyle="Cabeçalho Meteora">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{AD739091-30BD-4C30-BDDA-7504C0C4B6E2}" name="TB_Vendas" displayName="TB_Vendas" ref="A2:H61" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8" headerRowCellStyle="Cabeçalho Meteora">
   <autoFilter ref="A2:H61" xr:uid="{AD739091-30BD-4C30-BDDA-7504C0C4B6E2}"/>
   <tableColumns count="8">
-    <tableColumn id="7" xr3:uid="{5E8DE7C3-CDB6-4314-A5CC-C44D3C21973F}" name="Mês" dataDxfId="22">
+    <tableColumn id="7" xr3:uid="{5E8DE7C3-CDB6-4314-A5CC-C44D3C21973F}" name="Mês" dataDxfId="7">
       <calculatedColumnFormula>MONTH(TB_Vendas[[#This Row],[Data]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{43632F1F-6978-4CE7-BB13-7CCE587D6821}" name="Data" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{49DF5362-33BE-4541-BD47-0B512249381E}" name="Código" dataDxfId="20"/>
-    <tableColumn id="3" xr3:uid="{B3C718A1-FEFF-4C65-9CA1-DF94EF755918}" name="Tamanho" dataDxfId="19">
+    <tableColumn id="1" xr3:uid="{43632F1F-6978-4CE7-BB13-7CCE587D6821}" name="Data" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{49DF5362-33BE-4541-BD47-0B512249381E}" name="Código" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{B3C718A1-FEFF-4C65-9CA1-DF94EF755918}" name="Tamanho" dataDxfId="4">
       <calculatedColumnFormula>_xlfn.XLOOKUP(C3,TB_Produtos[Código],TB_Produtos[Tamanho])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{1F3EAF93-84E7-4086-BE54-3AB7D71B21A8}" name="Categoria" dataDxfId="18"/>
-    <tableColumn id="5" xr3:uid="{7DC2ADED-AF8A-4BC8-A38E-FEF676FE49C9}" name="Qtd" dataDxfId="17"/>
-    <tableColumn id="6" xr3:uid="{9459B662-6A4F-4486-82B1-12F67B8F842E}" name="Total" dataDxfId="16"/>
-    <tableColumn id="8" xr3:uid="{192FEBCA-1287-48A6-9BE6-69528F71C305}" name="Vendedor" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{1F3EAF93-84E7-4086-BE54-3AB7D71B21A8}" name="Categoria" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{7DC2ADED-AF8A-4BC8-A38E-FEF676FE49C9}" name="Qtd" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{9459B662-6A4F-4486-82B1-12F67B8F842E}" name="Total" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{192FEBCA-1287-48A6-9BE6-69528F71C305}" name="Vendedor" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3266,7 +3219,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8ADA2D8-DE9E-4ACF-B5A7-8907124C5CF1}">
   <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
@@ -4264,7 +4217,7 @@
     <mergeCell ref="A1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="F4:F42">
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="20" priority="3" operator="lessThan">
       <formula>3</formula>
     </cfRule>
     <cfRule type="iconSet" priority="2">
@@ -4314,6 +4267,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E00FC3C9-9397-44D3-9033-21F02904195D}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="2.140625" defaultRowHeight="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BF34D44-0E29-4A7F-B47B-66AF094D5F9D}">
   <dimension ref="A1:H61"/>
   <sheetViews>
@@ -6028,7 +5995,7 @@
     <mergeCell ref="A1:H1"/>
   </mergeCells>
   <conditionalFormatting sqref="F2">
-    <cfRule type="cellIs" dxfId="13" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6051,7 +6018,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87920B21-B994-41DD-BEC6-B8D0834CB666}">
   <dimension ref="A1:H4"/>
   <sheetViews>
@@ -6151,7 +6118,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BBE6E77-EBCD-448B-AB61-14EA4DC9C25B}">
   <dimension ref="B2:H14"/>
   <sheetViews>

</xml_diff>

<commit_message>
Arquivo:03 - Modelo Dashbord finalizado, anotações e planilha base
</commit_message>
<xml_diff>
--- a/03-Meteora_Ecommerce-Graficos-Formatos.xlsx
+++ b/03-Meteora_Ecommerce-Graficos-Formatos.xlsx
@@ -8,29 +8,31 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafae\Meu Drive (mz.tears.of.time@gmail.com)\Dev\Cursos\Curso-003\001 - Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36EF3DD9-40B9-4769-B864-2E012969786A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A2EA89A-C7EC-48C9-9E07-6BF607A3ACCA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="23070" windowHeight="11505" firstSheet="2" activeTab="3" xr2:uid="{F6D97A53-F63B-4272-A181-44B26E0B790F}"/>
+    <workbookView xWindow="3720" yWindow="0" windowWidth="23070" windowHeight="11505" firstSheet="2" activeTab="5" xr2:uid="{F6D97A53-F63B-4272-A181-44B26E0B790F}"/>
   </bookViews>
   <sheets>
     <sheet name="Meu Gráfico" sheetId="6" state="hidden" r:id="rId1"/>
     <sheet name="Planilha3" sheetId="5" state="hidden" r:id="rId2"/>
     <sheet name="Produtos" sheetId="17" r:id="rId3"/>
-    <sheet name="Dashboard" sheetId="18" r:id="rId4"/>
-    <sheet name="Vendas" sheetId="16" r:id="rId5"/>
-    <sheet name="Meus Números (Tabela)" sheetId="12" state="hidden" r:id="rId6"/>
-    <sheet name="Filtro Avançado" sheetId="9" state="hidden" r:id="rId7"/>
+    <sheet name="Vendas" sheetId="16" r:id="rId4"/>
+    <sheet name="Dashboard" sheetId="18" r:id="rId5"/>
+    <sheet name="Base de Dados Gráficos" sheetId="21" r:id="rId6"/>
+    <sheet name="Anotações" sheetId="20" r:id="rId7"/>
+    <sheet name="Meus Números (Tabela)" sheetId="12" state="hidden" r:id="rId8"/>
+    <sheet name="Filtro Avançado" sheetId="9" state="hidden" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Vendas!$B$2:$F$61</definedName>
-    <definedName name="_xlnm.Extract" localSheetId="6">'Filtro Avançado'!$B$6:$H$6</definedName>
-    <definedName name="_xlnm.Criteria" localSheetId="6">'Filtro Avançado'!$B$2:$C$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Vendas!$B$2:$F$61</definedName>
+    <definedName name="_xlnm.Extract" localSheetId="8">'Filtro Avançado'!$B$6:$H$6</definedName>
+    <definedName name="_xlnm.Criteria" localSheetId="8">'Filtro Avançado'!$B$2:$C$3</definedName>
     <definedName name="Int_Nome_Produtos">#REF!</definedName>
     <definedName name="Int_Quantidade">#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId8"/>
+    <pivotCache cacheId="0" r:id="rId10"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -41,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="98">
   <si>
     <t>Produtos</t>
   </si>
@@ -312,15 +314,198 @@
   <si>
     <t>Situação</t>
   </si>
+  <si>
+    <t>Total de Produtos</t>
+  </si>
+  <si>
+    <t>Produtos Vendidos</t>
+  </si>
+  <si>
+    <t>Total de Vendas</t>
+  </si>
+  <si>
+    <t>Vendas por Categorias</t>
+  </si>
+  <si>
+    <t>Ranking de Vendedores</t>
+  </si>
+  <si>
+    <t>=SOMASE(intervalo, critério, [intervalo_soma])</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">É usada para somar os valores de um intervalo que atendem a um critério específico.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Argumentos</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>intervalo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: O intervalo de células que você deseja avaliar com o critério.
+    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>critério</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: A condição que você deseja aplicar ao intervalo. Pode ser um número, uma expressão, uma referência de célula ou um texto que define quais células serão somadas.
+   </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> intervalo_soma (opcional)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: O intervalo de células que contém os valores a serem somados. Se omitido, o Excel somará os valores do intervalo.
+ Somar valores maiores que 50: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>=SOMASE(A1:A10, "&gt;50")</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+ Somar valores de uma coluna com base em um critério de outra coluna: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>=SOMASE(B1:B10, "Maçã", C1:C10)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+ Somar valores de acordo com um critério dinâmico: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>=SOMASE(A1:A10, E1)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+ </t>
+    </r>
+  </si>
+  <si>
+    <t>Vendedores</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="&quot;R$&quot;\ #,##0.00"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -387,6 +572,42 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="NSimSun"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FFDAFF01"/>
+      <name val="NSimSun"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="26"/>
+      <color theme="1"/>
+      <name val="NSimSun"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -425,7 +646,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -674,6 +895,86 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -685,7 +986,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -759,7 +1060,71 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -774,6 +1139,88 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="15" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Cabeçalho Meteora" xfId="3" xr:uid="{43DBFFA1-791E-423B-B2A6-377CC2810274}"/>
@@ -2127,6 +2574,49 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="3143250" cy="438150"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="image1.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7263EE6E-8E8D-4993-ADBD-B27E15270A79}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr preferRelativeResize="0"/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="276225"/>
+          <a:ext cx="3143250" cy="438150"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Office Resolve Testes" refreshedDate="45091.695904398148" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="39" xr:uid="{D9D057AD-0FAE-4908-B186-309A9CA94BEA}">
   <cacheSource type="worksheet">
@@ -3219,7 +3709,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8ADA2D8-DE9E-4ACF-B5A7-8907124C5CF1}">
   <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView topLeftCell="A20" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
@@ -3234,15 +3724,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
     </row>
     <row r="2" spans="1:7" ht="4.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2"/>
@@ -4267,24 +4757,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E00FC3C9-9397-44D3-9033-21F02904195D}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="2.140625" defaultRowHeight="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BF34D44-0E29-4A7F-B47B-66AF094D5F9D}">
   <dimension ref="A1:H61"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView topLeftCell="A35" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
@@ -4301,16 +4777,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
     </row>
     <row r="2" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="32" t="s">
@@ -6018,7 +6494,3772 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E00FC3C9-9397-44D3-9033-21F02904195D}">
+  <dimension ref="C1:CB46"/>
+  <sheetViews>
+    <sheetView showGridLines="0" showRowColHeaders="0" zoomScale="123" zoomScaleNormal="123" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28:AN46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="2.140625" defaultRowHeight="9.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="16384" width="2.140625" style="33"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:80" ht="9.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="3:80" ht="9.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="W2" s="35" t="s">
+        <v>90</v>
+      </c>
+      <c r="X2" s="36"/>
+      <c r="Y2" s="36"/>
+      <c r="Z2" s="36"/>
+      <c r="AA2" s="36"/>
+      <c r="AB2" s="36"/>
+      <c r="AC2" s="36"/>
+      <c r="AD2" s="36"/>
+      <c r="AE2" s="36"/>
+      <c r="AF2" s="36"/>
+      <c r="AG2" s="36"/>
+      <c r="AH2" s="36"/>
+      <c r="AI2" s="36"/>
+      <c r="AJ2" s="36"/>
+      <c r="AK2" s="36"/>
+      <c r="AL2" s="36"/>
+      <c r="AM2" s="36"/>
+      <c r="AN2" s="37"/>
+      <c r="AQ2" s="35" t="s">
+        <v>91</v>
+      </c>
+      <c r="AR2" s="36"/>
+      <c r="AS2" s="36"/>
+      <c r="AT2" s="36"/>
+      <c r="AU2" s="36"/>
+      <c r="AV2" s="36"/>
+      <c r="AW2" s="36"/>
+      <c r="AX2" s="36"/>
+      <c r="AY2" s="36"/>
+      <c r="AZ2" s="36"/>
+      <c r="BA2" s="36"/>
+      <c r="BB2" s="36"/>
+      <c r="BC2" s="36"/>
+      <c r="BD2" s="36"/>
+      <c r="BE2" s="36"/>
+      <c r="BF2" s="36"/>
+      <c r="BG2" s="36"/>
+      <c r="BH2" s="37"/>
+      <c r="BK2" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="BL2" s="36"/>
+      <c r="BM2" s="36"/>
+      <c r="BN2" s="36"/>
+      <c r="BO2" s="36"/>
+      <c r="BP2" s="36"/>
+      <c r="BQ2" s="36"/>
+      <c r="BR2" s="36"/>
+      <c r="BS2" s="36"/>
+      <c r="BT2" s="36"/>
+      <c r="BU2" s="36"/>
+      <c r="BV2" s="36"/>
+      <c r="BW2" s="36"/>
+      <c r="BX2" s="36"/>
+      <c r="BY2" s="36"/>
+      <c r="BZ2" s="36"/>
+      <c r="CA2" s="36"/>
+      <c r="CB2" s="37"/>
+    </row>
+    <row r="3" spans="3:80" ht="9.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="W3" s="38"/>
+      <c r="X3" s="39"/>
+      <c r="Y3" s="39"/>
+      <c r="Z3" s="39"/>
+      <c r="AA3" s="39"/>
+      <c r="AB3" s="39"/>
+      <c r="AC3" s="39"/>
+      <c r="AD3" s="39"/>
+      <c r="AE3" s="39"/>
+      <c r="AF3" s="39"/>
+      <c r="AG3" s="39"/>
+      <c r="AH3" s="39"/>
+      <c r="AI3" s="39"/>
+      <c r="AJ3" s="39"/>
+      <c r="AK3" s="39"/>
+      <c r="AL3" s="39"/>
+      <c r="AM3" s="39"/>
+      <c r="AN3" s="40"/>
+      <c r="AQ3" s="38"/>
+      <c r="AR3" s="39"/>
+      <c r="AS3" s="39"/>
+      <c r="AT3" s="39"/>
+      <c r="AU3" s="39"/>
+      <c r="AV3" s="39"/>
+      <c r="AW3" s="39"/>
+      <c r="AX3" s="39"/>
+      <c r="AY3" s="39"/>
+      <c r="AZ3" s="39"/>
+      <c r="BA3" s="39"/>
+      <c r="BB3" s="39"/>
+      <c r="BC3" s="39"/>
+      <c r="BD3" s="39"/>
+      <c r="BE3" s="39"/>
+      <c r="BF3" s="39"/>
+      <c r="BG3" s="39"/>
+      <c r="BH3" s="40"/>
+      <c r="BK3" s="38"/>
+      <c r="BL3" s="39"/>
+      <c r="BM3" s="39"/>
+      <c r="BN3" s="39"/>
+      <c r="BO3" s="39"/>
+      <c r="BP3" s="39"/>
+      <c r="BQ3" s="39"/>
+      <c r="BR3" s="39"/>
+      <c r="BS3" s="39"/>
+      <c r="BT3" s="39"/>
+      <c r="BU3" s="39"/>
+      <c r="BV3" s="39"/>
+      <c r="BW3" s="39"/>
+      <c r="BX3" s="39"/>
+      <c r="BY3" s="39"/>
+      <c r="BZ3" s="39"/>
+      <c r="CA3" s="39"/>
+      <c r="CB3" s="40"/>
+    </row>
+    <row r="4" spans="3:80" ht="9.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="W4" s="60">
+        <f>COUNTA(TB_Produtos[Código])</f>
+        <v>39</v>
+      </c>
+      <c r="X4" s="61"/>
+      <c r="Y4" s="61"/>
+      <c r="Z4" s="61"/>
+      <c r="AA4" s="61"/>
+      <c r="AB4" s="61"/>
+      <c r="AC4" s="61"/>
+      <c r="AD4" s="61"/>
+      <c r="AE4" s="61"/>
+      <c r="AF4" s="61"/>
+      <c r="AG4" s="61"/>
+      <c r="AH4" s="61"/>
+      <c r="AI4" s="61"/>
+      <c r="AJ4" s="61"/>
+      <c r="AK4" s="61"/>
+      <c r="AL4" s="61"/>
+      <c r="AM4" s="61"/>
+      <c r="AN4" s="62"/>
+      <c r="AQ4" s="60">
+        <f>SUM(TB_Vendas[Qtd])</f>
+        <v>131</v>
+      </c>
+      <c r="AR4" s="61"/>
+      <c r="AS4" s="61"/>
+      <c r="AT4" s="61"/>
+      <c r="AU4" s="61"/>
+      <c r="AV4" s="61"/>
+      <c r="AW4" s="61"/>
+      <c r="AX4" s="61"/>
+      <c r="AY4" s="61"/>
+      <c r="AZ4" s="61"/>
+      <c r="BA4" s="61"/>
+      <c r="BB4" s="61"/>
+      <c r="BC4" s="61"/>
+      <c r="BD4" s="61"/>
+      <c r="BE4" s="61"/>
+      <c r="BF4" s="61"/>
+      <c r="BG4" s="61"/>
+      <c r="BH4" s="62"/>
+      <c r="BK4" s="69">
+        <f>SUM(TB_Vendas[Total])</f>
+        <v>15963.659999999998</v>
+      </c>
+      <c r="BL4" s="70"/>
+      <c r="BM4" s="70"/>
+      <c r="BN4" s="70"/>
+      <c r="BO4" s="70"/>
+      <c r="BP4" s="70"/>
+      <c r="BQ4" s="70"/>
+      <c r="BR4" s="70"/>
+      <c r="BS4" s="70"/>
+      <c r="BT4" s="70"/>
+      <c r="BU4" s="70"/>
+      <c r="BV4" s="70"/>
+      <c r="BW4" s="70"/>
+      <c r="BX4" s="70"/>
+      <c r="BY4" s="70"/>
+      <c r="BZ4" s="70"/>
+      <c r="CA4" s="70"/>
+      <c r="CB4" s="71"/>
+    </row>
+    <row r="5" spans="3:80" ht="9.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="W5" s="63"/>
+      <c r="X5" s="64"/>
+      <c r="Y5" s="64"/>
+      <c r="Z5" s="64"/>
+      <c r="AA5" s="64"/>
+      <c r="AB5" s="64"/>
+      <c r="AC5" s="64"/>
+      <c r="AD5" s="64"/>
+      <c r="AE5" s="64"/>
+      <c r="AF5" s="64"/>
+      <c r="AG5" s="64"/>
+      <c r="AH5" s="64"/>
+      <c r="AI5" s="64"/>
+      <c r="AJ5" s="64"/>
+      <c r="AK5" s="64"/>
+      <c r="AL5" s="64"/>
+      <c r="AM5" s="64"/>
+      <c r="AN5" s="65"/>
+      <c r="AQ5" s="63"/>
+      <c r="AR5" s="64"/>
+      <c r="AS5" s="64"/>
+      <c r="AT5" s="64"/>
+      <c r="AU5" s="64"/>
+      <c r="AV5" s="64"/>
+      <c r="AW5" s="64"/>
+      <c r="AX5" s="64"/>
+      <c r="AY5" s="64"/>
+      <c r="AZ5" s="64"/>
+      <c r="BA5" s="64"/>
+      <c r="BB5" s="64"/>
+      <c r="BC5" s="64"/>
+      <c r="BD5" s="64"/>
+      <c r="BE5" s="64"/>
+      <c r="BF5" s="64"/>
+      <c r="BG5" s="64"/>
+      <c r="BH5" s="65"/>
+      <c r="BK5" s="72"/>
+      <c r="BL5" s="73"/>
+      <c r="BM5" s="73"/>
+      <c r="BN5" s="73"/>
+      <c r="BO5" s="73"/>
+      <c r="BP5" s="73"/>
+      <c r="BQ5" s="73"/>
+      <c r="BR5" s="73"/>
+      <c r="BS5" s="73"/>
+      <c r="BT5" s="73"/>
+      <c r="BU5" s="73"/>
+      <c r="BV5" s="73"/>
+      <c r="BW5" s="73"/>
+      <c r="BX5" s="73"/>
+      <c r="BY5" s="73"/>
+      <c r="BZ5" s="73"/>
+      <c r="CA5" s="73"/>
+      <c r="CB5" s="74"/>
+    </row>
+    <row r="6" spans="3:80" ht="9.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="W6" s="63"/>
+      <c r="X6" s="64"/>
+      <c r="Y6" s="64"/>
+      <c r="Z6" s="64"/>
+      <c r="AA6" s="64"/>
+      <c r="AB6" s="64"/>
+      <c r="AC6" s="64"/>
+      <c r="AD6" s="64"/>
+      <c r="AE6" s="64"/>
+      <c r="AF6" s="64"/>
+      <c r="AG6" s="64"/>
+      <c r="AH6" s="64"/>
+      <c r="AI6" s="64"/>
+      <c r="AJ6" s="64"/>
+      <c r="AK6" s="64"/>
+      <c r="AL6" s="64"/>
+      <c r="AM6" s="64"/>
+      <c r="AN6" s="65"/>
+      <c r="AQ6" s="63"/>
+      <c r="AR6" s="64"/>
+      <c r="AS6" s="64"/>
+      <c r="AT6" s="64"/>
+      <c r="AU6" s="64"/>
+      <c r="AV6" s="64"/>
+      <c r="AW6" s="64"/>
+      <c r="AX6" s="64"/>
+      <c r="AY6" s="64"/>
+      <c r="AZ6" s="64"/>
+      <c r="BA6" s="64"/>
+      <c r="BB6" s="64"/>
+      <c r="BC6" s="64"/>
+      <c r="BD6" s="64"/>
+      <c r="BE6" s="64"/>
+      <c r="BF6" s="64"/>
+      <c r="BG6" s="64"/>
+      <c r="BH6" s="65"/>
+      <c r="BK6" s="72"/>
+      <c r="BL6" s="73"/>
+      <c r="BM6" s="73"/>
+      <c r="BN6" s="73"/>
+      <c r="BO6" s="73"/>
+      <c r="BP6" s="73"/>
+      <c r="BQ6" s="73"/>
+      <c r="BR6" s="73"/>
+      <c r="BS6" s="73"/>
+      <c r="BT6" s="73"/>
+      <c r="BU6" s="73"/>
+      <c r="BV6" s="73"/>
+      <c r="BW6" s="73"/>
+      <c r="BX6" s="73"/>
+      <c r="BY6" s="73"/>
+      <c r="BZ6" s="73"/>
+      <c r="CA6" s="73"/>
+      <c r="CB6" s="74"/>
+    </row>
+    <row r="7" spans="3:80" ht="9.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="W7" s="66"/>
+      <c r="X7" s="67"/>
+      <c r="Y7" s="67"/>
+      <c r="Z7" s="67"/>
+      <c r="AA7" s="67"/>
+      <c r="AB7" s="67"/>
+      <c r="AC7" s="67"/>
+      <c r="AD7" s="67"/>
+      <c r="AE7" s="67"/>
+      <c r="AF7" s="67"/>
+      <c r="AG7" s="67"/>
+      <c r="AH7" s="67"/>
+      <c r="AI7" s="67"/>
+      <c r="AJ7" s="67"/>
+      <c r="AK7" s="67"/>
+      <c r="AL7" s="67"/>
+      <c r="AM7" s="67"/>
+      <c r="AN7" s="68"/>
+      <c r="AQ7" s="66"/>
+      <c r="AR7" s="67"/>
+      <c r="AS7" s="67"/>
+      <c r="AT7" s="67"/>
+      <c r="AU7" s="67"/>
+      <c r="AV7" s="67"/>
+      <c r="AW7" s="67"/>
+      <c r="AX7" s="67"/>
+      <c r="AY7" s="67"/>
+      <c r="AZ7" s="67"/>
+      <c r="BA7" s="67"/>
+      <c r="BB7" s="67"/>
+      <c r="BC7" s="67"/>
+      <c r="BD7" s="67"/>
+      <c r="BE7" s="67"/>
+      <c r="BF7" s="67"/>
+      <c r="BG7" s="67"/>
+      <c r="BH7" s="68"/>
+      <c r="BK7" s="75"/>
+      <c r="BL7" s="76"/>
+      <c r="BM7" s="76"/>
+      <c r="BN7" s="76"/>
+      <c r="BO7" s="76"/>
+      <c r="BP7" s="76"/>
+      <c r="BQ7" s="76"/>
+      <c r="BR7" s="76"/>
+      <c r="BS7" s="76"/>
+      <c r="BT7" s="76"/>
+      <c r="BU7" s="76"/>
+      <c r="BV7" s="76"/>
+      <c r="BW7" s="76"/>
+      <c r="BX7" s="76"/>
+      <c r="BY7" s="76"/>
+      <c r="BZ7" s="76"/>
+      <c r="CA7" s="76"/>
+      <c r="CB7" s="77"/>
+    </row>
+    <row r="8" spans="3:80" ht="9.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="3:80" ht="9.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C9" s="50"/>
+      <c r="D9" s="51"/>
+      <c r="E9" s="51"/>
+      <c r="F9" s="51"/>
+      <c r="G9" s="51"/>
+      <c r="H9" s="51"/>
+      <c r="I9" s="51"/>
+      <c r="J9" s="51"/>
+      <c r="K9" s="51"/>
+      <c r="L9" s="51"/>
+      <c r="M9" s="51"/>
+      <c r="N9" s="51"/>
+      <c r="O9" s="51"/>
+      <c r="P9" s="51"/>
+      <c r="Q9" s="51"/>
+      <c r="R9" s="51"/>
+      <c r="S9" s="51"/>
+      <c r="T9" s="51"/>
+      <c r="U9" s="51"/>
+      <c r="V9" s="51"/>
+      <c r="W9" s="51"/>
+      <c r="X9" s="51"/>
+      <c r="Y9" s="51"/>
+      <c r="Z9" s="51"/>
+      <c r="AA9" s="51"/>
+      <c r="AB9" s="51"/>
+      <c r="AC9" s="51"/>
+      <c r="AD9" s="51"/>
+      <c r="AE9" s="51"/>
+      <c r="AF9" s="51"/>
+      <c r="AG9" s="51"/>
+      <c r="AH9" s="51"/>
+      <c r="AI9" s="51"/>
+      <c r="AJ9" s="51"/>
+      <c r="AK9" s="51"/>
+      <c r="AL9" s="51"/>
+      <c r="AM9" s="51"/>
+      <c r="AN9" s="51"/>
+      <c r="AO9" s="51"/>
+      <c r="AP9" s="51"/>
+      <c r="AQ9" s="51"/>
+      <c r="AR9" s="51"/>
+      <c r="AS9" s="51"/>
+      <c r="AT9" s="51"/>
+      <c r="AU9" s="51"/>
+      <c r="AV9" s="51"/>
+      <c r="AW9" s="51"/>
+      <c r="AX9" s="51"/>
+      <c r="AY9" s="51"/>
+      <c r="AZ9" s="51"/>
+      <c r="BA9" s="51"/>
+      <c r="BB9" s="51"/>
+      <c r="BC9" s="51"/>
+      <c r="BD9" s="51"/>
+      <c r="BE9" s="51"/>
+      <c r="BF9" s="51"/>
+      <c r="BG9" s="51"/>
+      <c r="BH9" s="51"/>
+      <c r="BI9" s="51"/>
+      <c r="BJ9" s="51"/>
+      <c r="BK9" s="51"/>
+      <c r="BL9" s="51"/>
+      <c r="BM9" s="51"/>
+      <c r="BN9" s="51"/>
+      <c r="BO9" s="51"/>
+      <c r="BP9" s="51"/>
+      <c r="BQ9" s="51"/>
+      <c r="BR9" s="51"/>
+      <c r="BS9" s="51"/>
+      <c r="BT9" s="51"/>
+      <c r="BU9" s="51"/>
+      <c r="BV9" s="51"/>
+      <c r="BW9" s="51"/>
+      <c r="BX9" s="51"/>
+      <c r="BY9" s="51"/>
+      <c r="BZ9" s="51"/>
+      <c r="CA9" s="51"/>
+      <c r="CB9" s="52"/>
+    </row>
+    <row r="10" spans="3:80" ht="9.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="C10" s="53"/>
+      <c r="D10" s="54"/>
+      <c r="E10" s="54"/>
+      <c r="F10" s="54"/>
+      <c r="G10" s="54"/>
+      <c r="H10" s="54"/>
+      <c r="I10" s="54"/>
+      <c r="J10" s="54"/>
+      <c r="K10" s="54"/>
+      <c r="L10" s="54"/>
+      <c r="M10" s="54"/>
+      <c r="N10" s="54"/>
+      <c r="O10" s="54"/>
+      <c r="P10" s="54"/>
+      <c r="Q10" s="54"/>
+      <c r="R10" s="54"/>
+      <c r="S10" s="54"/>
+      <c r="T10" s="54"/>
+      <c r="U10" s="54"/>
+      <c r="V10" s="54"/>
+      <c r="W10" s="54"/>
+      <c r="X10" s="54"/>
+      <c r="Y10" s="54"/>
+      <c r="Z10" s="54"/>
+      <c r="AA10" s="54"/>
+      <c r="AB10" s="54"/>
+      <c r="AC10" s="54"/>
+      <c r="AD10" s="54"/>
+      <c r="AE10" s="54"/>
+      <c r="AF10" s="54"/>
+      <c r="AG10" s="54"/>
+      <c r="AH10" s="54"/>
+      <c r="AI10" s="54"/>
+      <c r="AJ10" s="54"/>
+      <c r="AK10" s="54"/>
+      <c r="AL10" s="54"/>
+      <c r="AM10" s="54"/>
+      <c r="AN10" s="54"/>
+      <c r="AO10" s="54"/>
+      <c r="AP10" s="54"/>
+      <c r="AQ10" s="54"/>
+      <c r="AR10" s="54"/>
+      <c r="AS10" s="54"/>
+      <c r="AT10" s="54"/>
+      <c r="AU10" s="54"/>
+      <c r="AV10" s="54"/>
+      <c r="AW10" s="54"/>
+      <c r="AX10" s="54"/>
+      <c r="AY10" s="54"/>
+      <c r="AZ10" s="54"/>
+      <c r="BA10" s="54"/>
+      <c r="BB10" s="54"/>
+      <c r="BC10" s="54"/>
+      <c r="BD10" s="54"/>
+      <c r="BE10" s="54"/>
+      <c r="BF10" s="54"/>
+      <c r="BG10" s="54"/>
+      <c r="BH10" s="54"/>
+      <c r="BI10" s="54"/>
+      <c r="BJ10" s="54"/>
+      <c r="BK10" s="54"/>
+      <c r="BL10" s="54"/>
+      <c r="BM10" s="54"/>
+      <c r="BN10" s="54"/>
+      <c r="BO10" s="54"/>
+      <c r="BP10" s="54"/>
+      <c r="BQ10" s="54"/>
+      <c r="BR10" s="54"/>
+      <c r="BS10" s="54"/>
+      <c r="BT10" s="54"/>
+      <c r="BU10" s="54"/>
+      <c r="BV10" s="54"/>
+      <c r="BW10" s="54"/>
+      <c r="BX10" s="54"/>
+      <c r="BY10" s="54"/>
+      <c r="BZ10" s="54"/>
+      <c r="CA10" s="54"/>
+      <c r="CB10" s="55"/>
+    </row>
+    <row r="11" spans="3:80" ht="9.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C11" s="41"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="42"/>
+      <c r="H11" s="42"/>
+      <c r="I11" s="42"/>
+      <c r="J11" s="42"/>
+      <c r="K11" s="42"/>
+      <c r="L11" s="42"/>
+      <c r="M11" s="42"/>
+      <c r="N11" s="42"/>
+      <c r="O11" s="42"/>
+      <c r="P11" s="42"/>
+      <c r="Q11" s="42"/>
+      <c r="R11" s="42"/>
+      <c r="S11" s="42"/>
+      <c r="T11" s="42"/>
+      <c r="U11" s="42"/>
+      <c r="V11" s="42"/>
+      <c r="W11" s="42"/>
+      <c r="X11" s="42"/>
+      <c r="Y11" s="42"/>
+      <c r="Z11" s="42"/>
+      <c r="AA11" s="42"/>
+      <c r="AB11" s="42"/>
+      <c r="AC11" s="42"/>
+      <c r="AD11" s="42"/>
+      <c r="AE11" s="42"/>
+      <c r="AF11" s="42"/>
+      <c r="AG11" s="42"/>
+      <c r="AH11" s="42"/>
+      <c r="AI11" s="42"/>
+      <c r="AJ11" s="42"/>
+      <c r="AK11" s="42"/>
+      <c r="AL11" s="42"/>
+      <c r="AM11" s="42"/>
+      <c r="AN11" s="42"/>
+      <c r="AO11" s="42"/>
+      <c r="AP11" s="42"/>
+      <c r="AQ11" s="42"/>
+      <c r="AR11" s="42"/>
+      <c r="AS11" s="42"/>
+      <c r="AT11" s="42"/>
+      <c r="AU11" s="42"/>
+      <c r="AV11" s="42"/>
+      <c r="AW11" s="42"/>
+      <c r="AX11" s="42"/>
+      <c r="AY11" s="42"/>
+      <c r="AZ11" s="42"/>
+      <c r="BA11" s="42"/>
+      <c r="BB11" s="42"/>
+      <c r="BC11" s="42"/>
+      <c r="BD11" s="42"/>
+      <c r="BE11" s="42"/>
+      <c r="BF11" s="42"/>
+      <c r="BG11" s="42"/>
+      <c r="BH11" s="42"/>
+      <c r="BI11" s="42"/>
+      <c r="BJ11" s="42"/>
+      <c r="BK11" s="42"/>
+      <c r="BL11" s="42"/>
+      <c r="BM11" s="42"/>
+      <c r="BN11" s="42"/>
+      <c r="BO11" s="42"/>
+      <c r="BP11" s="42"/>
+      <c r="BQ11" s="42"/>
+      <c r="BR11" s="42"/>
+      <c r="BS11" s="42"/>
+      <c r="BT11" s="42"/>
+      <c r="BU11" s="42"/>
+      <c r="BV11" s="42"/>
+      <c r="BW11" s="42"/>
+      <c r="BX11" s="42"/>
+      <c r="BY11" s="42"/>
+      <c r="BZ11" s="42"/>
+      <c r="CA11" s="42"/>
+      <c r="CB11" s="43"/>
+    </row>
+    <row r="12" spans="3:80" ht="9.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C12" s="44"/>
+      <c r="D12" s="45"/>
+      <c r="E12" s="45"/>
+      <c r="F12" s="45"/>
+      <c r="G12" s="45"/>
+      <c r="H12" s="45"/>
+      <c r="I12" s="45"/>
+      <c r="J12" s="45"/>
+      <c r="K12" s="45"/>
+      <c r="L12" s="45"/>
+      <c r="M12" s="45"/>
+      <c r="N12" s="45"/>
+      <c r="O12" s="45"/>
+      <c r="P12" s="45"/>
+      <c r="Q12" s="45"/>
+      <c r="R12" s="45"/>
+      <c r="S12" s="45"/>
+      <c r="T12" s="45"/>
+      <c r="U12" s="45"/>
+      <c r="V12" s="45"/>
+      <c r="W12" s="45"/>
+      <c r="X12" s="45"/>
+      <c r="Y12" s="45"/>
+      <c r="Z12" s="45"/>
+      <c r="AA12" s="45"/>
+      <c r="AB12" s="45"/>
+      <c r="AC12" s="45"/>
+      <c r="AD12" s="45"/>
+      <c r="AE12" s="45"/>
+      <c r="AF12" s="45"/>
+      <c r="AG12" s="45"/>
+      <c r="AH12" s="45"/>
+      <c r="AI12" s="45"/>
+      <c r="AJ12" s="45"/>
+      <c r="AK12" s="45"/>
+      <c r="AL12" s="45"/>
+      <c r="AM12" s="45"/>
+      <c r="AN12" s="45"/>
+      <c r="AO12" s="45"/>
+      <c r="AP12" s="45"/>
+      <c r="AQ12" s="45"/>
+      <c r="AR12" s="45"/>
+      <c r="AS12" s="45"/>
+      <c r="AT12" s="45"/>
+      <c r="AU12" s="45"/>
+      <c r="AV12" s="45"/>
+      <c r="AW12" s="45"/>
+      <c r="AX12" s="45"/>
+      <c r="AY12" s="45"/>
+      <c r="AZ12" s="45"/>
+      <c r="BA12" s="45"/>
+      <c r="BB12" s="45"/>
+      <c r="BC12" s="45"/>
+      <c r="BD12" s="45"/>
+      <c r="BE12" s="45"/>
+      <c r="BF12" s="45"/>
+      <c r="BG12" s="45"/>
+      <c r="BH12" s="45"/>
+      <c r="BI12" s="45"/>
+      <c r="BJ12" s="45"/>
+      <c r="BK12" s="45"/>
+      <c r="BL12" s="45"/>
+      <c r="BM12" s="45"/>
+      <c r="BN12" s="45"/>
+      <c r="BO12" s="45"/>
+      <c r="BP12" s="45"/>
+      <c r="BQ12" s="45"/>
+      <c r="BR12" s="45"/>
+      <c r="BS12" s="45"/>
+      <c r="BT12" s="45"/>
+      <c r="BU12" s="45"/>
+      <c r="BV12" s="45"/>
+      <c r="BW12" s="45"/>
+      <c r="BX12" s="45"/>
+      <c r="BY12" s="45"/>
+      <c r="BZ12" s="45"/>
+      <c r="CA12" s="45"/>
+      <c r="CB12" s="46"/>
+    </row>
+    <row r="13" spans="3:80" ht="9.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C13" s="44"/>
+      <c r="D13" s="45"/>
+      <c r="E13" s="45"/>
+      <c r="F13" s="45"/>
+      <c r="G13" s="45"/>
+      <c r="H13" s="45"/>
+      <c r="I13" s="45"/>
+      <c r="J13" s="45"/>
+      <c r="K13" s="45"/>
+      <c r="L13" s="45"/>
+      <c r="M13" s="45"/>
+      <c r="N13" s="45"/>
+      <c r="O13" s="45"/>
+      <c r="P13" s="45"/>
+      <c r="Q13" s="45"/>
+      <c r="R13" s="45"/>
+      <c r="S13" s="45"/>
+      <c r="T13" s="45"/>
+      <c r="U13" s="45"/>
+      <c r="V13" s="45"/>
+      <c r="W13" s="45"/>
+      <c r="X13" s="45"/>
+      <c r="Y13" s="45"/>
+      <c r="Z13" s="45"/>
+      <c r="AA13" s="45"/>
+      <c r="AB13" s="45"/>
+      <c r="AC13" s="45"/>
+      <c r="AD13" s="45"/>
+      <c r="AE13" s="45"/>
+      <c r="AF13" s="45"/>
+      <c r="AG13" s="45"/>
+      <c r="AH13" s="45"/>
+      <c r="AI13" s="45"/>
+      <c r="AJ13" s="45"/>
+      <c r="AK13" s="45"/>
+      <c r="AL13" s="45"/>
+      <c r="AM13" s="45"/>
+      <c r="AN13" s="45"/>
+      <c r="AO13" s="45"/>
+      <c r="AP13" s="45"/>
+      <c r="AQ13" s="45"/>
+      <c r="AR13" s="45"/>
+      <c r="AS13" s="45"/>
+      <c r="AT13" s="45"/>
+      <c r="AU13" s="45"/>
+      <c r="AV13" s="45"/>
+      <c r="AW13" s="45"/>
+      <c r="AX13" s="45"/>
+      <c r="AY13" s="45"/>
+      <c r="AZ13" s="45"/>
+      <c r="BA13" s="45"/>
+      <c r="BB13" s="45"/>
+      <c r="BC13" s="45"/>
+      <c r="BD13" s="45"/>
+      <c r="BE13" s="45"/>
+      <c r="BF13" s="45"/>
+      <c r="BG13" s="45"/>
+      <c r="BH13" s="45"/>
+      <c r="BI13" s="45"/>
+      <c r="BJ13" s="45"/>
+      <c r="BK13" s="45"/>
+      <c r="BL13" s="45"/>
+      <c r="BM13" s="45"/>
+      <c r="BN13" s="45"/>
+      <c r="BO13" s="45"/>
+      <c r="BP13" s="45"/>
+      <c r="BQ13" s="45"/>
+      <c r="BR13" s="45"/>
+      <c r="BS13" s="45"/>
+      <c r="BT13" s="45"/>
+      <c r="BU13" s="45"/>
+      <c r="BV13" s="45"/>
+      <c r="BW13" s="45"/>
+      <c r="BX13" s="45"/>
+      <c r="BY13" s="45"/>
+      <c r="BZ13" s="45"/>
+      <c r="CA13" s="45"/>
+      <c r="CB13" s="46"/>
+    </row>
+    <row r="14" spans="3:80" ht="9.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C14" s="44"/>
+      <c r="D14" s="45"/>
+      <c r="E14" s="45"/>
+      <c r="F14" s="45"/>
+      <c r="G14" s="45"/>
+      <c r="H14" s="45"/>
+      <c r="I14" s="45"/>
+      <c r="J14" s="45"/>
+      <c r="K14" s="45"/>
+      <c r="L14" s="45"/>
+      <c r="M14" s="45"/>
+      <c r="N14" s="45"/>
+      <c r="O14" s="45"/>
+      <c r="P14" s="45"/>
+      <c r="Q14" s="45"/>
+      <c r="R14" s="45"/>
+      <c r="S14" s="45"/>
+      <c r="T14" s="45"/>
+      <c r="U14" s="45"/>
+      <c r="V14" s="45"/>
+      <c r="W14" s="45"/>
+      <c r="X14" s="45"/>
+      <c r="Y14" s="45"/>
+      <c r="Z14" s="45"/>
+      <c r="AA14" s="45"/>
+      <c r="AB14" s="45"/>
+      <c r="AC14" s="45"/>
+      <c r="AD14" s="45"/>
+      <c r="AE14" s="45"/>
+      <c r="AF14" s="45"/>
+      <c r="AG14" s="45"/>
+      <c r="AH14" s="45"/>
+      <c r="AI14" s="45"/>
+      <c r="AJ14" s="45"/>
+      <c r="AK14" s="45"/>
+      <c r="AL14" s="45"/>
+      <c r="AM14" s="45"/>
+      <c r="AN14" s="45"/>
+      <c r="AO14" s="45"/>
+      <c r="AP14" s="45"/>
+      <c r="AQ14" s="45"/>
+      <c r="AR14" s="45"/>
+      <c r="AS14" s="45"/>
+      <c r="AT14" s="45"/>
+      <c r="AU14" s="45"/>
+      <c r="AV14" s="45"/>
+      <c r="AW14" s="45"/>
+      <c r="AX14" s="45"/>
+      <c r="AY14" s="45"/>
+      <c r="AZ14" s="45"/>
+      <c r="BA14" s="45"/>
+      <c r="BB14" s="45"/>
+      <c r="BC14" s="45"/>
+      <c r="BD14" s="45"/>
+      <c r="BE14" s="45"/>
+      <c r="BF14" s="45"/>
+      <c r="BG14" s="45"/>
+      <c r="BH14" s="45"/>
+      <c r="BI14" s="45"/>
+      <c r="BJ14" s="45"/>
+      <c r="BK14" s="45"/>
+      <c r="BL14" s="45"/>
+      <c r="BM14" s="45"/>
+      <c r="BN14" s="45"/>
+      <c r="BO14" s="45"/>
+      <c r="BP14" s="45"/>
+      <c r="BQ14" s="45"/>
+      <c r="BR14" s="45"/>
+      <c r="BS14" s="45"/>
+      <c r="BT14" s="45"/>
+      <c r="BU14" s="45"/>
+      <c r="BV14" s="45"/>
+      <c r="BW14" s="45"/>
+      <c r="BX14" s="45"/>
+      <c r="BY14" s="45"/>
+      <c r="BZ14" s="45"/>
+      <c r="CA14" s="45"/>
+      <c r="CB14" s="46"/>
+    </row>
+    <row r="15" spans="3:80" ht="9.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C15" s="44"/>
+      <c r="D15" s="45"/>
+      <c r="E15" s="45"/>
+      <c r="F15" s="45"/>
+      <c r="G15" s="45"/>
+      <c r="H15" s="45"/>
+      <c r="I15" s="45"/>
+      <c r="J15" s="45"/>
+      <c r="K15" s="45"/>
+      <c r="L15" s="45"/>
+      <c r="M15" s="45"/>
+      <c r="N15" s="45"/>
+      <c r="O15" s="45"/>
+      <c r="P15" s="45"/>
+      <c r="Q15" s="45"/>
+      <c r="R15" s="45"/>
+      <c r="S15" s="45"/>
+      <c r="T15" s="45"/>
+      <c r="U15" s="45"/>
+      <c r="V15" s="45"/>
+      <c r="W15" s="45"/>
+      <c r="X15" s="45"/>
+      <c r="Y15" s="45"/>
+      <c r="Z15" s="45"/>
+      <c r="AA15" s="45"/>
+      <c r="AB15" s="45"/>
+      <c r="AC15" s="45"/>
+      <c r="AD15" s="45"/>
+      <c r="AE15" s="45"/>
+      <c r="AF15" s="45"/>
+      <c r="AG15" s="45"/>
+      <c r="AH15" s="45"/>
+      <c r="AI15" s="45"/>
+      <c r="AJ15" s="45"/>
+      <c r="AK15" s="45"/>
+      <c r="AL15" s="45"/>
+      <c r="AM15" s="45"/>
+      <c r="AN15" s="45"/>
+      <c r="AO15" s="45"/>
+      <c r="AP15" s="45"/>
+      <c r="AQ15" s="45"/>
+      <c r="AR15" s="45"/>
+      <c r="AS15" s="45"/>
+      <c r="AT15" s="45"/>
+      <c r="AU15" s="45"/>
+      <c r="AV15" s="45"/>
+      <c r="AW15" s="45"/>
+      <c r="AX15" s="45"/>
+      <c r="AY15" s="45"/>
+      <c r="AZ15" s="45"/>
+      <c r="BA15" s="45"/>
+      <c r="BB15" s="45"/>
+      <c r="BC15" s="45"/>
+      <c r="BD15" s="45"/>
+      <c r="BE15" s="45"/>
+      <c r="BF15" s="45"/>
+      <c r="BG15" s="45"/>
+      <c r="BH15" s="45"/>
+      <c r="BI15" s="45"/>
+      <c r="BJ15" s="45"/>
+      <c r="BK15" s="45"/>
+      <c r="BL15" s="45"/>
+      <c r="BM15" s="45"/>
+      <c r="BN15" s="45"/>
+      <c r="BO15" s="45"/>
+      <c r="BP15" s="45"/>
+      <c r="BQ15" s="45"/>
+      <c r="BR15" s="45"/>
+      <c r="BS15" s="45"/>
+      <c r="BT15" s="45"/>
+      <c r="BU15" s="45"/>
+      <c r="BV15" s="45"/>
+      <c r="BW15" s="45"/>
+      <c r="BX15" s="45"/>
+      <c r="BY15" s="45"/>
+      <c r="BZ15" s="45"/>
+      <c r="CA15" s="45"/>
+      <c r="CB15" s="46"/>
+    </row>
+    <row r="16" spans="3:80" ht="9.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C16" s="44"/>
+      <c r="D16" s="45"/>
+      <c r="E16" s="45"/>
+      <c r="F16" s="45"/>
+      <c r="G16" s="45"/>
+      <c r="H16" s="45"/>
+      <c r="I16" s="45"/>
+      <c r="J16" s="45"/>
+      <c r="K16" s="45"/>
+      <c r="L16" s="45"/>
+      <c r="M16" s="45"/>
+      <c r="N16" s="45"/>
+      <c r="O16" s="45"/>
+      <c r="P16" s="45"/>
+      <c r="Q16" s="45"/>
+      <c r="R16" s="45"/>
+      <c r="S16" s="45"/>
+      <c r="T16" s="45"/>
+      <c r="U16" s="45"/>
+      <c r="V16" s="45"/>
+      <c r="W16" s="45"/>
+      <c r="X16" s="45"/>
+      <c r="Y16" s="45"/>
+      <c r="Z16" s="45"/>
+      <c r="AA16" s="45"/>
+      <c r="AB16" s="45"/>
+      <c r="AC16" s="45"/>
+      <c r="AD16" s="45"/>
+      <c r="AE16" s="45"/>
+      <c r="AF16" s="45"/>
+      <c r="AG16" s="45"/>
+      <c r="AH16" s="45"/>
+      <c r="AI16" s="45"/>
+      <c r="AJ16" s="45"/>
+      <c r="AK16" s="45"/>
+      <c r="AL16" s="45"/>
+      <c r="AM16" s="45"/>
+      <c r="AN16" s="45"/>
+      <c r="AO16" s="45"/>
+      <c r="AP16" s="45"/>
+      <c r="AQ16" s="45"/>
+      <c r="AR16" s="45"/>
+      <c r="AS16" s="45"/>
+      <c r="AT16" s="45"/>
+      <c r="AU16" s="45"/>
+      <c r="AV16" s="45"/>
+      <c r="AW16" s="45"/>
+      <c r="AX16" s="45"/>
+      <c r="AY16" s="45"/>
+      <c r="AZ16" s="45"/>
+      <c r="BA16" s="45"/>
+      <c r="BB16" s="45"/>
+      <c r="BC16" s="45"/>
+      <c r="BD16" s="45"/>
+      <c r="BE16" s="45"/>
+      <c r="BF16" s="45"/>
+      <c r="BG16" s="45"/>
+      <c r="BH16" s="45"/>
+      <c r="BI16" s="45"/>
+      <c r="BJ16" s="45"/>
+      <c r="BK16" s="45"/>
+      <c r="BL16" s="45"/>
+      <c r="BM16" s="45"/>
+      <c r="BN16" s="45"/>
+      <c r="BO16" s="45"/>
+      <c r="BP16" s="45"/>
+      <c r="BQ16" s="45"/>
+      <c r="BR16" s="45"/>
+      <c r="BS16" s="45"/>
+      <c r="BT16" s="45"/>
+      <c r="BU16" s="45"/>
+      <c r="BV16" s="45"/>
+      <c r="BW16" s="45"/>
+      <c r="BX16" s="45"/>
+      <c r="BY16" s="45"/>
+      <c r="BZ16" s="45"/>
+      <c r="CA16" s="45"/>
+      <c r="CB16" s="46"/>
+    </row>
+    <row r="17" spans="3:80" ht="9.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C17" s="44"/>
+      <c r="D17" s="45"/>
+      <c r="E17" s="45"/>
+      <c r="F17" s="45"/>
+      <c r="G17" s="45"/>
+      <c r="H17" s="45"/>
+      <c r="I17" s="45"/>
+      <c r="J17" s="45"/>
+      <c r="K17" s="45"/>
+      <c r="L17" s="45"/>
+      <c r="M17" s="45"/>
+      <c r="N17" s="45"/>
+      <c r="O17" s="45"/>
+      <c r="P17" s="45"/>
+      <c r="Q17" s="45"/>
+      <c r="R17" s="45"/>
+      <c r="S17" s="45"/>
+      <c r="T17" s="45"/>
+      <c r="U17" s="45"/>
+      <c r="V17" s="45"/>
+      <c r="W17" s="45"/>
+      <c r="X17" s="45"/>
+      <c r="Y17" s="45"/>
+      <c r="Z17" s="45"/>
+      <c r="AA17" s="45"/>
+      <c r="AB17" s="45"/>
+      <c r="AC17" s="45"/>
+      <c r="AD17" s="45"/>
+      <c r="AE17" s="45"/>
+      <c r="AF17" s="45"/>
+      <c r="AG17" s="45"/>
+      <c r="AH17" s="45"/>
+      <c r="AI17" s="45"/>
+      <c r="AJ17" s="45"/>
+      <c r="AK17" s="45"/>
+      <c r="AL17" s="45"/>
+      <c r="AM17" s="45"/>
+      <c r="AN17" s="45"/>
+      <c r="AO17" s="45"/>
+      <c r="AP17" s="45"/>
+      <c r="AQ17" s="45"/>
+      <c r="AR17" s="45"/>
+      <c r="AS17" s="45"/>
+      <c r="AT17" s="45"/>
+      <c r="AU17" s="45"/>
+      <c r="AV17" s="45"/>
+      <c r="AW17" s="45"/>
+      <c r="AX17" s="45"/>
+      <c r="AY17" s="45"/>
+      <c r="AZ17" s="45"/>
+      <c r="BA17" s="45"/>
+      <c r="BB17" s="45"/>
+      <c r="BC17" s="45"/>
+      <c r="BD17" s="45"/>
+      <c r="BE17" s="45"/>
+      <c r="BF17" s="45"/>
+      <c r="BG17" s="45"/>
+      <c r="BH17" s="45"/>
+      <c r="BI17" s="45"/>
+      <c r="BJ17" s="45"/>
+      <c r="BK17" s="45"/>
+      <c r="BL17" s="45"/>
+      <c r="BM17" s="45"/>
+      <c r="BN17" s="45"/>
+      <c r="BO17" s="45"/>
+      <c r="BP17" s="45"/>
+      <c r="BQ17" s="45"/>
+      <c r="BR17" s="45"/>
+      <c r="BS17" s="45"/>
+      <c r="BT17" s="45"/>
+      <c r="BU17" s="45"/>
+      <c r="BV17" s="45"/>
+      <c r="BW17" s="45"/>
+      <c r="BX17" s="45"/>
+      <c r="BY17" s="45"/>
+      <c r="BZ17" s="45"/>
+      <c r="CA17" s="45"/>
+      <c r="CB17" s="46"/>
+    </row>
+    <row r="18" spans="3:80" ht="9.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C18" s="44"/>
+      <c r="D18" s="45"/>
+      <c r="E18" s="45"/>
+      <c r="F18" s="45"/>
+      <c r="G18" s="45"/>
+      <c r="H18" s="45"/>
+      <c r="I18" s="45"/>
+      <c r="J18" s="45"/>
+      <c r="K18" s="45"/>
+      <c r="L18" s="45"/>
+      <c r="M18" s="45"/>
+      <c r="N18" s="45"/>
+      <c r="O18" s="45"/>
+      <c r="P18" s="45"/>
+      <c r="Q18" s="45"/>
+      <c r="R18" s="45"/>
+      <c r="S18" s="45"/>
+      <c r="T18" s="45"/>
+      <c r="U18" s="45"/>
+      <c r="V18" s="45"/>
+      <c r="W18" s="45"/>
+      <c r="X18" s="45"/>
+      <c r="Y18" s="45"/>
+      <c r="Z18" s="45"/>
+      <c r="AA18" s="45"/>
+      <c r="AB18" s="45"/>
+      <c r="AC18" s="45"/>
+      <c r="AD18" s="45"/>
+      <c r="AE18" s="45"/>
+      <c r="AF18" s="45"/>
+      <c r="AG18" s="45"/>
+      <c r="AH18" s="45"/>
+      <c r="AI18" s="45"/>
+      <c r="AJ18" s="45"/>
+      <c r="AK18" s="45"/>
+      <c r="AL18" s="45"/>
+      <c r="AM18" s="45"/>
+      <c r="AN18" s="45"/>
+      <c r="AO18" s="45"/>
+      <c r="AP18" s="45"/>
+      <c r="AQ18" s="45"/>
+      <c r="AR18" s="45"/>
+      <c r="AS18" s="45"/>
+      <c r="AT18" s="45"/>
+      <c r="AU18" s="45"/>
+      <c r="AV18" s="45"/>
+      <c r="AW18" s="45"/>
+      <c r="AX18" s="45"/>
+      <c r="AY18" s="45"/>
+      <c r="AZ18" s="45"/>
+      <c r="BA18" s="45"/>
+      <c r="BB18" s="45"/>
+      <c r="BC18" s="45"/>
+      <c r="BD18" s="45"/>
+      <c r="BE18" s="45"/>
+      <c r="BF18" s="45"/>
+      <c r="BG18" s="45"/>
+      <c r="BH18" s="45"/>
+      <c r="BI18" s="45"/>
+      <c r="BJ18" s="45"/>
+      <c r="BK18" s="45"/>
+      <c r="BL18" s="45"/>
+      <c r="BM18" s="45"/>
+      <c r="BN18" s="45"/>
+      <c r="BO18" s="45"/>
+      <c r="BP18" s="45"/>
+      <c r="BQ18" s="45"/>
+      <c r="BR18" s="45"/>
+      <c r="BS18" s="45"/>
+      <c r="BT18" s="45"/>
+      <c r="BU18" s="45"/>
+      <c r="BV18" s="45"/>
+      <c r="BW18" s="45"/>
+      <c r="BX18" s="45"/>
+      <c r="BY18" s="45"/>
+      <c r="BZ18" s="45"/>
+      <c r="CA18" s="45"/>
+      <c r="CB18" s="46"/>
+    </row>
+    <row r="19" spans="3:80" ht="9.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C19" s="44"/>
+      <c r="D19" s="45"/>
+      <c r="E19" s="45"/>
+      <c r="F19" s="45"/>
+      <c r="G19" s="45"/>
+      <c r="H19" s="45"/>
+      <c r="I19" s="45"/>
+      <c r="J19" s="45"/>
+      <c r="K19" s="45"/>
+      <c r="L19" s="45"/>
+      <c r="M19" s="45"/>
+      <c r="N19" s="45"/>
+      <c r="O19" s="45"/>
+      <c r="P19" s="45"/>
+      <c r="Q19" s="45"/>
+      <c r="R19" s="45"/>
+      <c r="S19" s="45"/>
+      <c r="T19" s="45"/>
+      <c r="U19" s="45"/>
+      <c r="V19" s="45"/>
+      <c r="W19" s="45"/>
+      <c r="X19" s="45"/>
+      <c r="Y19" s="45"/>
+      <c r="Z19" s="45"/>
+      <c r="AA19" s="45"/>
+      <c r="AB19" s="45"/>
+      <c r="AC19" s="45"/>
+      <c r="AD19" s="45"/>
+      <c r="AE19" s="45"/>
+      <c r="AF19" s="45"/>
+      <c r="AG19" s="45"/>
+      <c r="AH19" s="45"/>
+      <c r="AI19" s="45"/>
+      <c r="AJ19" s="45"/>
+      <c r="AK19" s="45"/>
+      <c r="AL19" s="45"/>
+      <c r="AM19" s="45"/>
+      <c r="AN19" s="45"/>
+      <c r="AO19" s="45"/>
+      <c r="AP19" s="45"/>
+      <c r="AQ19" s="45"/>
+      <c r="AR19" s="45"/>
+      <c r="AS19" s="45"/>
+      <c r="AT19" s="45"/>
+      <c r="AU19" s="45"/>
+      <c r="AV19" s="45"/>
+      <c r="AW19" s="45"/>
+      <c r="AX19" s="45"/>
+      <c r="AY19" s="45"/>
+      <c r="AZ19" s="45"/>
+      <c r="BA19" s="45"/>
+      <c r="BB19" s="45"/>
+      <c r="BC19" s="45"/>
+      <c r="BD19" s="45"/>
+      <c r="BE19" s="45"/>
+      <c r="BF19" s="45"/>
+      <c r="BG19" s="45"/>
+      <c r="BH19" s="45"/>
+      <c r="BI19" s="45"/>
+      <c r="BJ19" s="45"/>
+      <c r="BK19" s="45"/>
+      <c r="BL19" s="45"/>
+      <c r="BM19" s="45"/>
+      <c r="BN19" s="45"/>
+      <c r="BO19" s="45"/>
+      <c r="BP19" s="45"/>
+      <c r="BQ19" s="45"/>
+      <c r="BR19" s="45"/>
+      <c r="BS19" s="45"/>
+      <c r="BT19" s="45"/>
+      <c r="BU19" s="45"/>
+      <c r="BV19" s="45"/>
+      <c r="BW19" s="45"/>
+      <c r="BX19" s="45"/>
+      <c r="BY19" s="45"/>
+      <c r="BZ19" s="45"/>
+      <c r="CA19" s="45"/>
+      <c r="CB19" s="46"/>
+    </row>
+    <row r="20" spans="3:80" ht="9.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C20" s="44"/>
+      <c r="D20" s="45"/>
+      <c r="E20" s="45"/>
+      <c r="F20" s="45"/>
+      <c r="G20" s="45"/>
+      <c r="H20" s="45"/>
+      <c r="I20" s="45"/>
+      <c r="J20" s="45"/>
+      <c r="K20" s="45"/>
+      <c r="L20" s="45"/>
+      <c r="M20" s="45"/>
+      <c r="N20" s="45"/>
+      <c r="O20" s="45"/>
+      <c r="P20" s="45"/>
+      <c r="Q20" s="45"/>
+      <c r="R20" s="45"/>
+      <c r="S20" s="45"/>
+      <c r="T20" s="45"/>
+      <c r="U20" s="45"/>
+      <c r="V20" s="45"/>
+      <c r="W20" s="45"/>
+      <c r="X20" s="45"/>
+      <c r="Y20" s="45"/>
+      <c r="Z20" s="45"/>
+      <c r="AA20" s="45"/>
+      <c r="AB20" s="45"/>
+      <c r="AC20" s="45"/>
+      <c r="AD20" s="45"/>
+      <c r="AE20" s="45"/>
+      <c r="AF20" s="45"/>
+      <c r="AG20" s="45"/>
+      <c r="AH20" s="45"/>
+      <c r="AI20" s="45"/>
+      <c r="AJ20" s="45"/>
+      <c r="AK20" s="45"/>
+      <c r="AL20" s="45"/>
+      <c r="AM20" s="45"/>
+      <c r="AN20" s="45"/>
+      <c r="AO20" s="45"/>
+      <c r="AP20" s="45"/>
+      <c r="AQ20" s="45"/>
+      <c r="AR20" s="45"/>
+      <c r="AS20" s="45"/>
+      <c r="AT20" s="45"/>
+      <c r="AU20" s="45"/>
+      <c r="AV20" s="45"/>
+      <c r="AW20" s="45"/>
+      <c r="AX20" s="45"/>
+      <c r="AY20" s="45"/>
+      <c r="AZ20" s="45"/>
+      <c r="BA20" s="45"/>
+      <c r="BB20" s="45"/>
+      <c r="BC20" s="45"/>
+      <c r="BD20" s="45"/>
+      <c r="BE20" s="45"/>
+      <c r="BF20" s="45"/>
+      <c r="BG20" s="45"/>
+      <c r="BH20" s="45"/>
+      <c r="BI20" s="45"/>
+      <c r="BJ20" s="45"/>
+      <c r="BK20" s="45"/>
+      <c r="BL20" s="45"/>
+      <c r="BM20" s="45"/>
+      <c r="BN20" s="45"/>
+      <c r="BO20" s="45"/>
+      <c r="BP20" s="45"/>
+      <c r="BQ20" s="45"/>
+      <c r="BR20" s="45"/>
+      <c r="BS20" s="45"/>
+      <c r="BT20" s="45"/>
+      <c r="BU20" s="45"/>
+      <c r="BV20" s="45"/>
+      <c r="BW20" s="45"/>
+      <c r="BX20" s="45"/>
+      <c r="BY20" s="45"/>
+      <c r="BZ20" s="45"/>
+      <c r="CA20" s="45"/>
+      <c r="CB20" s="46"/>
+    </row>
+    <row r="21" spans="3:80" ht="9.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C21" s="44"/>
+      <c r="D21" s="45"/>
+      <c r="E21" s="45"/>
+      <c r="F21" s="45"/>
+      <c r="G21" s="45"/>
+      <c r="H21" s="45"/>
+      <c r="I21" s="45"/>
+      <c r="J21" s="45"/>
+      <c r="K21" s="45"/>
+      <c r="L21" s="45"/>
+      <c r="M21" s="45"/>
+      <c r="N21" s="45"/>
+      <c r="O21" s="45"/>
+      <c r="P21" s="45"/>
+      <c r="Q21" s="45"/>
+      <c r="R21" s="45"/>
+      <c r="S21" s="45"/>
+      <c r="T21" s="45"/>
+      <c r="U21" s="45"/>
+      <c r="V21" s="45"/>
+      <c r="W21" s="45"/>
+      <c r="X21" s="45"/>
+      <c r="Y21" s="45"/>
+      <c r="Z21" s="45"/>
+      <c r="AA21" s="45"/>
+      <c r="AB21" s="45"/>
+      <c r="AC21" s="45"/>
+      <c r="AD21" s="45"/>
+      <c r="AE21" s="45"/>
+      <c r="AF21" s="45"/>
+      <c r="AG21" s="45"/>
+      <c r="AH21" s="45"/>
+      <c r="AI21" s="45"/>
+      <c r="AJ21" s="45"/>
+      <c r="AK21" s="45"/>
+      <c r="AL21" s="45"/>
+      <c r="AM21" s="45"/>
+      <c r="AN21" s="45"/>
+      <c r="AO21" s="45"/>
+      <c r="AP21" s="45"/>
+      <c r="AQ21" s="45"/>
+      <c r="AR21" s="45"/>
+      <c r="AS21" s="45"/>
+      <c r="AT21" s="45"/>
+      <c r="AU21" s="45"/>
+      <c r="AV21" s="45"/>
+      <c r="AW21" s="45"/>
+      <c r="AX21" s="45"/>
+      <c r="AY21" s="45"/>
+      <c r="AZ21" s="45"/>
+      <c r="BA21" s="45"/>
+      <c r="BB21" s="45"/>
+      <c r="BC21" s="45"/>
+      <c r="BD21" s="45"/>
+      <c r="BE21" s="45"/>
+      <c r="BF21" s="45"/>
+      <c r="BG21" s="45"/>
+      <c r="BH21" s="45"/>
+      <c r="BI21" s="45"/>
+      <c r="BJ21" s="45"/>
+      <c r="BK21" s="45"/>
+      <c r="BL21" s="45"/>
+      <c r="BM21" s="45"/>
+      <c r="BN21" s="45"/>
+      <c r="BO21" s="45"/>
+      <c r="BP21" s="45"/>
+      <c r="BQ21" s="45"/>
+      <c r="BR21" s="45"/>
+      <c r="BS21" s="45"/>
+      <c r="BT21" s="45"/>
+      <c r="BU21" s="45"/>
+      <c r="BV21" s="45"/>
+      <c r="BW21" s="45"/>
+      <c r="BX21" s="45"/>
+      <c r="BY21" s="45"/>
+      <c r="BZ21" s="45"/>
+      <c r="CA21" s="45"/>
+      <c r="CB21" s="46"/>
+    </row>
+    <row r="22" spans="3:80" ht="9.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C22" s="44"/>
+      <c r="D22" s="45"/>
+      <c r="E22" s="45"/>
+      <c r="F22" s="45"/>
+      <c r="G22" s="45"/>
+      <c r="H22" s="45"/>
+      <c r="I22" s="45"/>
+      <c r="J22" s="45"/>
+      <c r="K22" s="45"/>
+      <c r="L22" s="45"/>
+      <c r="M22" s="45"/>
+      <c r="N22" s="45"/>
+      <c r="O22" s="45"/>
+      <c r="P22" s="45"/>
+      <c r="Q22" s="45"/>
+      <c r="R22" s="45"/>
+      <c r="S22" s="45"/>
+      <c r="T22" s="45"/>
+      <c r="U22" s="45"/>
+      <c r="V22" s="45"/>
+      <c r="W22" s="45"/>
+      <c r="X22" s="45"/>
+      <c r="Y22" s="45"/>
+      <c r="Z22" s="45"/>
+      <c r="AA22" s="45"/>
+      <c r="AB22" s="45"/>
+      <c r="AC22" s="45"/>
+      <c r="AD22" s="45"/>
+      <c r="AE22" s="45"/>
+      <c r="AF22" s="45"/>
+      <c r="AG22" s="45"/>
+      <c r="AH22" s="45"/>
+      <c r="AI22" s="45"/>
+      <c r="AJ22" s="45"/>
+      <c r="AK22" s="45"/>
+      <c r="AL22" s="45"/>
+      <c r="AM22" s="45"/>
+      <c r="AN22" s="45"/>
+      <c r="AO22" s="45"/>
+      <c r="AP22" s="45"/>
+      <c r="AQ22" s="45"/>
+      <c r="AR22" s="45"/>
+      <c r="AS22" s="45"/>
+      <c r="AT22" s="45"/>
+      <c r="AU22" s="45"/>
+      <c r="AV22" s="45"/>
+      <c r="AW22" s="45"/>
+      <c r="AX22" s="45"/>
+      <c r="AY22" s="45"/>
+      <c r="AZ22" s="45"/>
+      <c r="BA22" s="45"/>
+      <c r="BB22" s="45"/>
+      <c r="BC22" s="45"/>
+      <c r="BD22" s="45"/>
+      <c r="BE22" s="45"/>
+      <c r="BF22" s="45"/>
+      <c r="BG22" s="45"/>
+      <c r="BH22" s="45"/>
+      <c r="BI22" s="45"/>
+      <c r="BJ22" s="45"/>
+      <c r="BK22" s="45"/>
+      <c r="BL22" s="45"/>
+      <c r="BM22" s="45"/>
+      <c r="BN22" s="45"/>
+      <c r="BO22" s="45"/>
+      <c r="BP22" s="45"/>
+      <c r="BQ22" s="45"/>
+      <c r="BR22" s="45"/>
+      <c r="BS22" s="45"/>
+      <c r="BT22" s="45"/>
+      <c r="BU22" s="45"/>
+      <c r="BV22" s="45"/>
+      <c r="BW22" s="45"/>
+      <c r="BX22" s="45"/>
+      <c r="BY22" s="45"/>
+      <c r="BZ22" s="45"/>
+      <c r="CA22" s="45"/>
+      <c r="CB22" s="46"/>
+    </row>
+    <row r="23" spans="3:80" ht="9.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C23" s="44"/>
+      <c r="D23" s="45"/>
+      <c r="E23" s="45"/>
+      <c r="F23" s="45"/>
+      <c r="G23" s="45"/>
+      <c r="H23" s="45"/>
+      <c r="I23" s="45"/>
+      <c r="J23" s="45"/>
+      <c r="K23" s="45"/>
+      <c r="L23" s="45"/>
+      <c r="M23" s="45"/>
+      <c r="N23" s="45"/>
+      <c r="O23" s="45"/>
+      <c r="P23" s="45"/>
+      <c r="Q23" s="45"/>
+      <c r="R23" s="45"/>
+      <c r="S23" s="45"/>
+      <c r="T23" s="45"/>
+      <c r="U23" s="45"/>
+      <c r="V23" s="45"/>
+      <c r="W23" s="45"/>
+      <c r="X23" s="45"/>
+      <c r="Y23" s="45"/>
+      <c r="Z23" s="45"/>
+      <c r="AA23" s="45"/>
+      <c r="AB23" s="45"/>
+      <c r="AC23" s="45"/>
+      <c r="AD23" s="45"/>
+      <c r="AE23" s="45"/>
+      <c r="AF23" s="45"/>
+      <c r="AG23" s="45"/>
+      <c r="AH23" s="45"/>
+      <c r="AI23" s="45"/>
+      <c r="AJ23" s="45"/>
+      <c r="AK23" s="45"/>
+      <c r="AL23" s="45"/>
+      <c r="AM23" s="45"/>
+      <c r="AN23" s="45"/>
+      <c r="AO23" s="45"/>
+      <c r="AP23" s="45"/>
+      <c r="AQ23" s="45"/>
+      <c r="AR23" s="45"/>
+      <c r="AS23" s="45"/>
+      <c r="AT23" s="45"/>
+      <c r="AU23" s="45"/>
+      <c r="AV23" s="45"/>
+      <c r="AW23" s="45"/>
+      <c r="AX23" s="45"/>
+      <c r="AY23" s="45"/>
+      <c r="AZ23" s="45"/>
+      <c r="BA23" s="45"/>
+      <c r="BB23" s="45"/>
+      <c r="BC23" s="45"/>
+      <c r="BD23" s="45"/>
+      <c r="BE23" s="45"/>
+      <c r="BF23" s="45"/>
+      <c r="BG23" s="45"/>
+      <c r="BH23" s="45"/>
+      <c r="BI23" s="45"/>
+      <c r="BJ23" s="45"/>
+      <c r="BK23" s="45"/>
+      <c r="BL23" s="45"/>
+      <c r="BM23" s="45"/>
+      <c r="BN23" s="45"/>
+      <c r="BO23" s="45"/>
+      <c r="BP23" s="45"/>
+      <c r="BQ23" s="45"/>
+      <c r="BR23" s="45"/>
+      <c r="BS23" s="45"/>
+      <c r="BT23" s="45"/>
+      <c r="BU23" s="45"/>
+      <c r="BV23" s="45"/>
+      <c r="BW23" s="45"/>
+      <c r="BX23" s="45"/>
+      <c r="BY23" s="45"/>
+      <c r="BZ23" s="45"/>
+      <c r="CA23" s="45"/>
+      <c r="CB23" s="46"/>
+    </row>
+    <row r="24" spans="3:80" ht="9.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="C24" s="47"/>
+      <c r="D24" s="48"/>
+      <c r="E24" s="48"/>
+      <c r="F24" s="48"/>
+      <c r="G24" s="48"/>
+      <c r="H24" s="48"/>
+      <c r="I24" s="48"/>
+      <c r="J24" s="48"/>
+      <c r="K24" s="48"/>
+      <c r="L24" s="48"/>
+      <c r="M24" s="48"/>
+      <c r="N24" s="48"/>
+      <c r="O24" s="48"/>
+      <c r="P24" s="48"/>
+      <c r="Q24" s="48"/>
+      <c r="R24" s="48"/>
+      <c r="S24" s="48"/>
+      <c r="T24" s="48"/>
+      <c r="U24" s="48"/>
+      <c r="V24" s="48"/>
+      <c r="W24" s="48"/>
+      <c r="X24" s="48"/>
+      <c r="Y24" s="48"/>
+      <c r="Z24" s="48"/>
+      <c r="AA24" s="48"/>
+      <c r="AB24" s="48"/>
+      <c r="AC24" s="48"/>
+      <c r="AD24" s="48"/>
+      <c r="AE24" s="48"/>
+      <c r="AF24" s="48"/>
+      <c r="AG24" s="48"/>
+      <c r="AH24" s="48"/>
+      <c r="AI24" s="48"/>
+      <c r="AJ24" s="48"/>
+      <c r="AK24" s="48"/>
+      <c r="AL24" s="48"/>
+      <c r="AM24" s="48"/>
+      <c r="AN24" s="48"/>
+      <c r="AO24" s="48"/>
+      <c r="AP24" s="48"/>
+      <c r="AQ24" s="48"/>
+      <c r="AR24" s="48"/>
+      <c r="AS24" s="48"/>
+      <c r="AT24" s="48"/>
+      <c r="AU24" s="48"/>
+      <c r="AV24" s="48"/>
+      <c r="AW24" s="48"/>
+      <c r="AX24" s="48"/>
+      <c r="AY24" s="48"/>
+      <c r="AZ24" s="48"/>
+      <c r="BA24" s="48"/>
+      <c r="BB24" s="48"/>
+      <c r="BC24" s="48"/>
+      <c r="BD24" s="48"/>
+      <c r="BE24" s="48"/>
+      <c r="BF24" s="48"/>
+      <c r="BG24" s="48"/>
+      <c r="BH24" s="48"/>
+      <c r="BI24" s="48"/>
+      <c r="BJ24" s="48"/>
+      <c r="BK24" s="48"/>
+      <c r="BL24" s="48"/>
+      <c r="BM24" s="48"/>
+      <c r="BN24" s="48"/>
+      <c r="BO24" s="48"/>
+      <c r="BP24" s="48"/>
+      <c r="BQ24" s="48"/>
+      <c r="BR24" s="48"/>
+      <c r="BS24" s="48"/>
+      <c r="BT24" s="48"/>
+      <c r="BU24" s="48"/>
+      <c r="BV24" s="48"/>
+      <c r="BW24" s="48"/>
+      <c r="BX24" s="48"/>
+      <c r="BY24" s="48"/>
+      <c r="BZ24" s="48"/>
+      <c r="CA24" s="48"/>
+      <c r="CB24" s="49"/>
+    </row>
+    <row r="25" spans="3:80" ht="9.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="3:80" ht="9.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C26" s="35" t="s">
+        <v>93</v>
+      </c>
+      <c r="D26" s="36"/>
+      <c r="E26" s="36"/>
+      <c r="F26" s="36"/>
+      <c r="G26" s="36"/>
+      <c r="H26" s="36"/>
+      <c r="I26" s="36"/>
+      <c r="J26" s="36"/>
+      <c r="K26" s="36"/>
+      <c r="L26" s="36"/>
+      <c r="M26" s="36"/>
+      <c r="N26" s="36"/>
+      <c r="O26" s="36"/>
+      <c r="P26" s="36"/>
+      <c r="Q26" s="36"/>
+      <c r="R26" s="36"/>
+      <c r="S26" s="36"/>
+      <c r="T26" s="36"/>
+      <c r="U26" s="36"/>
+      <c r="V26" s="36"/>
+      <c r="W26" s="36"/>
+      <c r="X26" s="36"/>
+      <c r="Y26" s="36"/>
+      <c r="Z26" s="36"/>
+      <c r="AA26" s="36"/>
+      <c r="AB26" s="36"/>
+      <c r="AC26" s="36"/>
+      <c r="AD26" s="36"/>
+      <c r="AE26" s="36"/>
+      <c r="AF26" s="36"/>
+      <c r="AG26" s="36"/>
+      <c r="AH26" s="36"/>
+      <c r="AI26" s="36"/>
+      <c r="AJ26" s="36"/>
+      <c r="AK26" s="36"/>
+      <c r="AL26" s="36"/>
+      <c r="AM26" s="36"/>
+      <c r="AN26" s="36"/>
+      <c r="AQ26" s="35" t="s">
+        <v>94</v>
+      </c>
+      <c r="AR26" s="36"/>
+      <c r="AS26" s="36"/>
+      <c r="AT26" s="36"/>
+      <c r="AU26" s="36"/>
+      <c r="AV26" s="36"/>
+      <c r="AW26" s="36"/>
+      <c r="AX26" s="36"/>
+      <c r="AY26" s="36"/>
+      <c r="AZ26" s="36"/>
+      <c r="BA26" s="36"/>
+      <c r="BB26" s="36"/>
+      <c r="BC26" s="36"/>
+      <c r="BD26" s="36"/>
+      <c r="BE26" s="36"/>
+      <c r="BF26" s="36"/>
+      <c r="BG26" s="36"/>
+      <c r="BH26" s="36"/>
+      <c r="BI26" s="36"/>
+      <c r="BJ26" s="36"/>
+      <c r="BK26" s="36"/>
+      <c r="BL26" s="36"/>
+      <c r="BM26" s="36"/>
+      <c r="BN26" s="36"/>
+      <c r="BO26" s="36"/>
+      <c r="BP26" s="36"/>
+      <c r="BQ26" s="36"/>
+      <c r="BR26" s="36"/>
+      <c r="BS26" s="36"/>
+      <c r="BT26" s="36"/>
+      <c r="BU26" s="36"/>
+      <c r="BV26" s="36"/>
+      <c r="BW26" s="36"/>
+      <c r="BX26" s="36"/>
+      <c r="BY26" s="36"/>
+      <c r="BZ26" s="36"/>
+      <c r="CA26" s="36"/>
+      <c r="CB26" s="36"/>
+    </row>
+    <row r="27" spans="3:80" ht="9.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="C27" s="38"/>
+      <c r="D27" s="39"/>
+      <c r="E27" s="39"/>
+      <c r="F27" s="39"/>
+      <c r="G27" s="39"/>
+      <c r="H27" s="39"/>
+      <c r="I27" s="39"/>
+      <c r="J27" s="39"/>
+      <c r="K27" s="39"/>
+      <c r="L27" s="39"/>
+      <c r="M27" s="39"/>
+      <c r="N27" s="39"/>
+      <c r="O27" s="39"/>
+      <c r="P27" s="39"/>
+      <c r="Q27" s="39"/>
+      <c r="R27" s="39"/>
+      <c r="S27" s="39"/>
+      <c r="T27" s="39"/>
+      <c r="U27" s="39"/>
+      <c r="V27" s="39"/>
+      <c r="W27" s="39"/>
+      <c r="X27" s="39"/>
+      <c r="Y27" s="39"/>
+      <c r="Z27" s="39"/>
+      <c r="AA27" s="39"/>
+      <c r="AB27" s="39"/>
+      <c r="AC27" s="39"/>
+      <c r="AD27" s="39"/>
+      <c r="AE27" s="39"/>
+      <c r="AF27" s="39"/>
+      <c r="AG27" s="39"/>
+      <c r="AH27" s="39"/>
+      <c r="AI27" s="39"/>
+      <c r="AJ27" s="39"/>
+      <c r="AK27" s="39"/>
+      <c r="AL27" s="39"/>
+      <c r="AM27" s="39"/>
+      <c r="AN27" s="39"/>
+      <c r="AQ27" s="38"/>
+      <c r="AR27" s="39"/>
+      <c r="AS27" s="39"/>
+      <c r="AT27" s="39"/>
+      <c r="AU27" s="39"/>
+      <c r="AV27" s="39"/>
+      <c r="AW27" s="39"/>
+      <c r="AX27" s="39"/>
+      <c r="AY27" s="39"/>
+      <c r="AZ27" s="39"/>
+      <c r="BA27" s="39"/>
+      <c r="BB27" s="39"/>
+      <c r="BC27" s="39"/>
+      <c r="BD27" s="39"/>
+      <c r="BE27" s="39"/>
+      <c r="BF27" s="39"/>
+      <c r="BG27" s="39"/>
+      <c r="BH27" s="39"/>
+      <c r="BI27" s="39"/>
+      <c r="BJ27" s="39"/>
+      <c r="BK27" s="39"/>
+      <c r="BL27" s="39"/>
+      <c r="BM27" s="39"/>
+      <c r="BN27" s="39"/>
+      <c r="BO27" s="39"/>
+      <c r="BP27" s="39"/>
+      <c r="BQ27" s="39"/>
+      <c r="BR27" s="39"/>
+      <c r="BS27" s="39"/>
+      <c r="BT27" s="39"/>
+      <c r="BU27" s="39"/>
+      <c r="BV27" s="39"/>
+      <c r="BW27" s="39"/>
+      <c r="BX27" s="39"/>
+      <c r="BY27" s="39"/>
+      <c r="BZ27" s="39"/>
+      <c r="CA27" s="39"/>
+      <c r="CB27" s="39"/>
+    </row>
+    <row r="28" spans="3:80" ht="9.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C28" s="41"/>
+      <c r="D28" s="42"/>
+      <c r="E28" s="42"/>
+      <c r="F28" s="42"/>
+      <c r="G28" s="42"/>
+      <c r="H28" s="42"/>
+      <c r="I28" s="42"/>
+      <c r="J28" s="42"/>
+      <c r="K28" s="42"/>
+      <c r="L28" s="42"/>
+      <c r="M28" s="42"/>
+      <c r="N28" s="42"/>
+      <c r="O28" s="42"/>
+      <c r="P28" s="42"/>
+      <c r="Q28" s="42"/>
+      <c r="R28" s="42"/>
+      <c r="S28" s="42"/>
+      <c r="T28" s="42"/>
+      <c r="U28" s="42"/>
+      <c r="V28" s="42"/>
+      <c r="W28" s="42"/>
+      <c r="X28" s="42"/>
+      <c r="Y28" s="42"/>
+      <c r="Z28" s="42"/>
+      <c r="AA28" s="42"/>
+      <c r="AB28" s="42"/>
+      <c r="AC28" s="42"/>
+      <c r="AD28" s="42"/>
+      <c r="AE28" s="42"/>
+      <c r="AF28" s="42"/>
+      <c r="AG28" s="42"/>
+      <c r="AH28" s="42"/>
+      <c r="AI28" s="42"/>
+      <c r="AJ28" s="42"/>
+      <c r="AK28" s="42"/>
+      <c r="AL28" s="42"/>
+      <c r="AM28" s="42"/>
+      <c r="AN28" s="43"/>
+      <c r="AQ28" s="41"/>
+      <c r="AR28" s="42"/>
+      <c r="AS28" s="42"/>
+      <c r="AT28" s="42"/>
+      <c r="AU28" s="42"/>
+      <c r="AV28" s="42"/>
+      <c r="AW28" s="42"/>
+      <c r="AX28" s="42"/>
+      <c r="AY28" s="42"/>
+      <c r="AZ28" s="42"/>
+      <c r="BA28" s="42"/>
+      <c r="BB28" s="42"/>
+      <c r="BC28" s="42"/>
+      <c r="BD28" s="42"/>
+      <c r="BE28" s="42"/>
+      <c r="BF28" s="42"/>
+      <c r="BG28" s="42"/>
+      <c r="BH28" s="42"/>
+      <c r="BI28" s="42"/>
+      <c r="BJ28" s="42"/>
+      <c r="BK28" s="42"/>
+      <c r="BL28" s="42"/>
+      <c r="BM28" s="42"/>
+      <c r="BN28" s="42"/>
+      <c r="BO28" s="42"/>
+      <c r="BP28" s="42"/>
+      <c r="BQ28" s="42"/>
+      <c r="BR28" s="42"/>
+      <c r="BS28" s="42"/>
+      <c r="BT28" s="42"/>
+      <c r="BU28" s="42"/>
+      <c r="BV28" s="42"/>
+      <c r="BW28" s="42"/>
+      <c r="BX28" s="42"/>
+      <c r="BY28" s="42"/>
+      <c r="BZ28" s="42"/>
+      <c r="CA28" s="42"/>
+      <c r="CB28" s="43"/>
+    </row>
+    <row r="29" spans="3:80" ht="9.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C29" s="44"/>
+      <c r="D29" s="45"/>
+      <c r="E29" s="45"/>
+      <c r="F29" s="45"/>
+      <c r="G29" s="45"/>
+      <c r="H29" s="45"/>
+      <c r="I29" s="45"/>
+      <c r="J29" s="45"/>
+      <c r="K29" s="45"/>
+      <c r="L29" s="45"/>
+      <c r="M29" s="45"/>
+      <c r="N29" s="45"/>
+      <c r="O29" s="45"/>
+      <c r="P29" s="45"/>
+      <c r="Q29" s="45"/>
+      <c r="R29" s="45"/>
+      <c r="S29" s="45"/>
+      <c r="T29" s="45"/>
+      <c r="U29" s="45"/>
+      <c r="V29" s="45"/>
+      <c r="W29" s="45"/>
+      <c r="X29" s="45"/>
+      <c r="Y29" s="45"/>
+      <c r="Z29" s="45"/>
+      <c r="AA29" s="45"/>
+      <c r="AB29" s="45"/>
+      <c r="AC29" s="45"/>
+      <c r="AD29" s="45"/>
+      <c r="AE29" s="45"/>
+      <c r="AF29" s="45"/>
+      <c r="AG29" s="45"/>
+      <c r="AH29" s="45"/>
+      <c r="AI29" s="45"/>
+      <c r="AJ29" s="45"/>
+      <c r="AK29" s="45"/>
+      <c r="AL29" s="45"/>
+      <c r="AM29" s="45"/>
+      <c r="AN29" s="46"/>
+      <c r="AQ29" s="44"/>
+      <c r="AR29" s="45"/>
+      <c r="AS29" s="45"/>
+      <c r="AT29" s="45"/>
+      <c r="AU29" s="45"/>
+      <c r="AV29" s="45"/>
+      <c r="AW29" s="45"/>
+      <c r="AX29" s="45"/>
+      <c r="AY29" s="45"/>
+      <c r="AZ29" s="45"/>
+      <c r="BA29" s="45"/>
+      <c r="BB29" s="45"/>
+      <c r="BC29" s="45"/>
+      <c r="BD29" s="45"/>
+      <c r="BE29" s="45"/>
+      <c r="BF29" s="45"/>
+      <c r="BG29" s="45"/>
+      <c r="BH29" s="45"/>
+      <c r="BI29" s="45"/>
+      <c r="BJ29" s="45"/>
+      <c r="BK29" s="45"/>
+      <c r="BL29" s="45"/>
+      <c r="BM29" s="45"/>
+      <c r="BN29" s="45"/>
+      <c r="BO29" s="45"/>
+      <c r="BP29" s="45"/>
+      <c r="BQ29" s="45"/>
+      <c r="BR29" s="45"/>
+      <c r="BS29" s="45"/>
+      <c r="BT29" s="45"/>
+      <c r="BU29" s="45"/>
+      <c r="BV29" s="45"/>
+      <c r="BW29" s="45"/>
+      <c r="BX29" s="45"/>
+      <c r="BY29" s="45"/>
+      <c r="BZ29" s="45"/>
+      <c r="CA29" s="45"/>
+      <c r="CB29" s="46"/>
+    </row>
+    <row r="30" spans="3:80" ht="9.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C30" s="44"/>
+      <c r="D30" s="45"/>
+      <c r="E30" s="45"/>
+      <c r="F30" s="45"/>
+      <c r="G30" s="45"/>
+      <c r="H30" s="45"/>
+      <c r="I30" s="45"/>
+      <c r="J30" s="45"/>
+      <c r="K30" s="45"/>
+      <c r="L30" s="45"/>
+      <c r="M30" s="45"/>
+      <c r="N30" s="45"/>
+      <c r="O30" s="45"/>
+      <c r="P30" s="45"/>
+      <c r="Q30" s="45"/>
+      <c r="R30" s="45"/>
+      <c r="S30" s="45"/>
+      <c r="T30" s="45"/>
+      <c r="U30" s="45"/>
+      <c r="V30" s="45"/>
+      <c r="W30" s="45"/>
+      <c r="X30" s="45"/>
+      <c r="Y30" s="45"/>
+      <c r="Z30" s="45"/>
+      <c r="AA30" s="45"/>
+      <c r="AB30" s="45"/>
+      <c r="AC30" s="45"/>
+      <c r="AD30" s="45"/>
+      <c r="AE30" s="45"/>
+      <c r="AF30" s="45"/>
+      <c r="AG30" s="45"/>
+      <c r="AH30" s="45"/>
+      <c r="AI30" s="45"/>
+      <c r="AJ30" s="45"/>
+      <c r="AK30" s="45"/>
+      <c r="AL30" s="45"/>
+      <c r="AM30" s="45"/>
+      <c r="AN30" s="46"/>
+      <c r="AQ30" s="44"/>
+      <c r="AR30" s="45"/>
+      <c r="AS30" s="45"/>
+      <c r="AT30" s="45"/>
+      <c r="AU30" s="45"/>
+      <c r="AV30" s="45"/>
+      <c r="AW30" s="45"/>
+      <c r="AX30" s="45"/>
+      <c r="AY30" s="45"/>
+      <c r="AZ30" s="45"/>
+      <c r="BA30" s="45"/>
+      <c r="BB30" s="45"/>
+      <c r="BC30" s="45"/>
+      <c r="BD30" s="45"/>
+      <c r="BE30" s="45"/>
+      <c r="BF30" s="45"/>
+      <c r="BG30" s="45"/>
+      <c r="BH30" s="45"/>
+      <c r="BI30" s="45"/>
+      <c r="BJ30" s="45"/>
+      <c r="BK30" s="45"/>
+      <c r="BL30" s="45"/>
+      <c r="BM30" s="45"/>
+      <c r="BN30" s="45"/>
+      <c r="BO30" s="45"/>
+      <c r="BP30" s="45"/>
+      <c r="BQ30" s="45"/>
+      <c r="BR30" s="45"/>
+      <c r="BS30" s="45"/>
+      <c r="BT30" s="45"/>
+      <c r="BU30" s="45"/>
+      <c r="BV30" s="45"/>
+      <c r="BW30" s="45"/>
+      <c r="BX30" s="45"/>
+      <c r="BY30" s="45"/>
+      <c r="BZ30" s="45"/>
+      <c r="CA30" s="45"/>
+      <c r="CB30" s="46"/>
+    </row>
+    <row r="31" spans="3:80" ht="9.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C31" s="44"/>
+      <c r="D31" s="45"/>
+      <c r="E31" s="45"/>
+      <c r="F31" s="45"/>
+      <c r="G31" s="45"/>
+      <c r="H31" s="45"/>
+      <c r="I31" s="45"/>
+      <c r="J31" s="45"/>
+      <c r="K31" s="45"/>
+      <c r="L31" s="45"/>
+      <c r="M31" s="45"/>
+      <c r="N31" s="45"/>
+      <c r="O31" s="45"/>
+      <c r="P31" s="45"/>
+      <c r="Q31" s="45"/>
+      <c r="R31" s="45"/>
+      <c r="S31" s="45"/>
+      <c r="T31" s="45"/>
+      <c r="U31" s="45"/>
+      <c r="V31" s="45"/>
+      <c r="W31" s="45"/>
+      <c r="X31" s="45"/>
+      <c r="Y31" s="45"/>
+      <c r="Z31" s="45"/>
+      <c r="AA31" s="45"/>
+      <c r="AB31" s="45"/>
+      <c r="AC31" s="45"/>
+      <c r="AD31" s="45"/>
+      <c r="AE31" s="45"/>
+      <c r="AF31" s="45"/>
+      <c r="AG31" s="45"/>
+      <c r="AH31" s="45"/>
+      <c r="AI31" s="45"/>
+      <c r="AJ31" s="45"/>
+      <c r="AK31" s="45"/>
+      <c r="AL31" s="45"/>
+      <c r="AM31" s="45"/>
+      <c r="AN31" s="46"/>
+      <c r="AQ31" s="44"/>
+      <c r="AR31" s="45"/>
+      <c r="AS31" s="45"/>
+      <c r="AT31" s="45"/>
+      <c r="AU31" s="45"/>
+      <c r="AV31" s="45"/>
+      <c r="AW31" s="45"/>
+      <c r="AX31" s="45"/>
+      <c r="AY31" s="45"/>
+      <c r="AZ31" s="45"/>
+      <c r="BA31" s="45"/>
+      <c r="BB31" s="45"/>
+      <c r="BC31" s="45"/>
+      <c r="BD31" s="45"/>
+      <c r="BE31" s="45"/>
+      <c r="BF31" s="45"/>
+      <c r="BG31" s="45"/>
+      <c r="BH31" s="45"/>
+      <c r="BI31" s="45"/>
+      <c r="BJ31" s="45"/>
+      <c r="BK31" s="45"/>
+      <c r="BL31" s="45"/>
+      <c r="BM31" s="45"/>
+      <c r="BN31" s="45"/>
+      <c r="BO31" s="45"/>
+      <c r="BP31" s="45"/>
+      <c r="BQ31" s="45"/>
+      <c r="BR31" s="45"/>
+      <c r="BS31" s="45"/>
+      <c r="BT31" s="45"/>
+      <c r="BU31" s="45"/>
+      <c r="BV31" s="45"/>
+      <c r="BW31" s="45"/>
+      <c r="BX31" s="45"/>
+      <c r="BY31" s="45"/>
+      <c r="BZ31" s="45"/>
+      <c r="CA31" s="45"/>
+      <c r="CB31" s="46"/>
+    </row>
+    <row r="32" spans="3:80" ht="9.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C32" s="44"/>
+      <c r="D32" s="45"/>
+      <c r="E32" s="45"/>
+      <c r="F32" s="45"/>
+      <c r="G32" s="45"/>
+      <c r="H32" s="45"/>
+      <c r="I32" s="45"/>
+      <c r="J32" s="45"/>
+      <c r="K32" s="45"/>
+      <c r="L32" s="45"/>
+      <c r="M32" s="45"/>
+      <c r="N32" s="45"/>
+      <c r="O32" s="45"/>
+      <c r="P32" s="45"/>
+      <c r="Q32" s="45"/>
+      <c r="R32" s="45"/>
+      <c r="S32" s="45"/>
+      <c r="T32" s="45"/>
+      <c r="U32" s="45"/>
+      <c r="V32" s="45"/>
+      <c r="W32" s="45"/>
+      <c r="X32" s="45"/>
+      <c r="Y32" s="45"/>
+      <c r="Z32" s="45"/>
+      <c r="AA32" s="45"/>
+      <c r="AB32" s="45"/>
+      <c r="AC32" s="45"/>
+      <c r="AD32" s="45"/>
+      <c r="AE32" s="45"/>
+      <c r="AF32" s="45"/>
+      <c r="AG32" s="45"/>
+      <c r="AH32" s="45"/>
+      <c r="AI32" s="45"/>
+      <c r="AJ32" s="45"/>
+      <c r="AK32" s="45"/>
+      <c r="AL32" s="45"/>
+      <c r="AM32" s="45"/>
+      <c r="AN32" s="46"/>
+      <c r="AQ32" s="44"/>
+      <c r="AR32" s="45"/>
+      <c r="AS32" s="45"/>
+      <c r="AT32" s="45"/>
+      <c r="AU32" s="45"/>
+      <c r="AV32" s="45"/>
+      <c r="AW32" s="45"/>
+      <c r="AX32" s="45"/>
+      <c r="AY32" s="45"/>
+      <c r="AZ32" s="45"/>
+      <c r="BA32" s="45"/>
+      <c r="BB32" s="45"/>
+      <c r="BC32" s="45"/>
+      <c r="BD32" s="45"/>
+      <c r="BE32" s="45"/>
+      <c r="BF32" s="45"/>
+      <c r="BG32" s="45"/>
+      <c r="BH32" s="45"/>
+      <c r="BI32" s="45"/>
+      <c r="BJ32" s="45"/>
+      <c r="BK32" s="45"/>
+      <c r="BL32" s="45"/>
+      <c r="BM32" s="45"/>
+      <c r="BN32" s="45"/>
+      <c r="BO32" s="45"/>
+      <c r="BP32" s="45"/>
+      <c r="BQ32" s="45"/>
+      <c r="BR32" s="45"/>
+      <c r="BS32" s="45"/>
+      <c r="BT32" s="45"/>
+      <c r="BU32" s="45"/>
+      <c r="BV32" s="45"/>
+      <c r="BW32" s="45"/>
+      <c r="BX32" s="45"/>
+      <c r="BY32" s="45"/>
+      <c r="BZ32" s="45"/>
+      <c r="CA32" s="45"/>
+      <c r="CB32" s="46"/>
+    </row>
+    <row r="33" spans="3:80" ht="9.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C33" s="44"/>
+      <c r="D33" s="45"/>
+      <c r="E33" s="45"/>
+      <c r="F33" s="45"/>
+      <c r="G33" s="45"/>
+      <c r="H33" s="45"/>
+      <c r="I33" s="45"/>
+      <c r="J33" s="45"/>
+      <c r="K33" s="45"/>
+      <c r="L33" s="45"/>
+      <c r="M33" s="45"/>
+      <c r="N33" s="45"/>
+      <c r="O33" s="45"/>
+      <c r="P33" s="45"/>
+      <c r="Q33" s="45"/>
+      <c r="R33" s="45"/>
+      <c r="S33" s="45"/>
+      <c r="T33" s="45"/>
+      <c r="U33" s="45"/>
+      <c r="V33" s="45"/>
+      <c r="W33" s="45"/>
+      <c r="X33" s="45"/>
+      <c r="Y33" s="45"/>
+      <c r="Z33" s="45"/>
+      <c r="AA33" s="45"/>
+      <c r="AB33" s="45"/>
+      <c r="AC33" s="45"/>
+      <c r="AD33" s="45"/>
+      <c r="AE33" s="45"/>
+      <c r="AF33" s="45"/>
+      <c r="AG33" s="45"/>
+      <c r="AH33" s="45"/>
+      <c r="AI33" s="45"/>
+      <c r="AJ33" s="45"/>
+      <c r="AK33" s="45"/>
+      <c r="AL33" s="45"/>
+      <c r="AM33" s="45"/>
+      <c r="AN33" s="46"/>
+      <c r="AQ33" s="44"/>
+      <c r="AR33" s="45"/>
+      <c r="AS33" s="45"/>
+      <c r="AT33" s="45"/>
+      <c r="AU33" s="45"/>
+      <c r="AV33" s="45"/>
+      <c r="AW33" s="45"/>
+      <c r="AX33" s="45"/>
+      <c r="AY33" s="45"/>
+      <c r="AZ33" s="45"/>
+      <c r="BA33" s="45"/>
+      <c r="BB33" s="45"/>
+      <c r="BC33" s="45"/>
+      <c r="BD33" s="45"/>
+      <c r="BE33" s="45"/>
+      <c r="BF33" s="45"/>
+      <c r="BG33" s="45"/>
+      <c r="BH33" s="45"/>
+      <c r="BI33" s="45"/>
+      <c r="BJ33" s="45"/>
+      <c r="BK33" s="45"/>
+      <c r="BL33" s="45"/>
+      <c r="BM33" s="45"/>
+      <c r="BN33" s="45"/>
+      <c r="BO33" s="45"/>
+      <c r="BP33" s="45"/>
+      <c r="BQ33" s="45"/>
+      <c r="BR33" s="45"/>
+      <c r="BS33" s="45"/>
+      <c r="BT33" s="45"/>
+      <c r="BU33" s="45"/>
+      <c r="BV33" s="45"/>
+      <c r="BW33" s="45"/>
+      <c r="BX33" s="45"/>
+      <c r="BY33" s="45"/>
+      <c r="BZ33" s="45"/>
+      <c r="CA33" s="45"/>
+      <c r="CB33" s="46"/>
+    </row>
+    <row r="34" spans="3:80" ht="9.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C34" s="44"/>
+      <c r="D34" s="45"/>
+      <c r="E34" s="45"/>
+      <c r="F34" s="45"/>
+      <c r="G34" s="45"/>
+      <c r="H34" s="45"/>
+      <c r="I34" s="45"/>
+      <c r="J34" s="45"/>
+      <c r="K34" s="45"/>
+      <c r="L34" s="45"/>
+      <c r="M34" s="45"/>
+      <c r="N34" s="45"/>
+      <c r="O34" s="45"/>
+      <c r="P34" s="45"/>
+      <c r="Q34" s="45"/>
+      <c r="R34" s="45"/>
+      <c r="S34" s="45"/>
+      <c r="T34" s="45"/>
+      <c r="U34" s="45"/>
+      <c r="V34" s="45"/>
+      <c r="W34" s="45"/>
+      <c r="X34" s="45"/>
+      <c r="Y34" s="45"/>
+      <c r="Z34" s="45"/>
+      <c r="AA34" s="45"/>
+      <c r="AB34" s="45"/>
+      <c r="AC34" s="45"/>
+      <c r="AD34" s="45"/>
+      <c r="AE34" s="45"/>
+      <c r="AF34" s="45"/>
+      <c r="AG34" s="45"/>
+      <c r="AH34" s="45"/>
+      <c r="AI34" s="45"/>
+      <c r="AJ34" s="45"/>
+      <c r="AK34" s="45"/>
+      <c r="AL34" s="45"/>
+      <c r="AM34" s="45"/>
+      <c r="AN34" s="46"/>
+      <c r="AQ34" s="44"/>
+      <c r="AR34" s="45"/>
+      <c r="AS34" s="45"/>
+      <c r="AT34" s="45"/>
+      <c r="AU34" s="45"/>
+      <c r="AV34" s="45"/>
+      <c r="AW34" s="45"/>
+      <c r="AX34" s="45"/>
+      <c r="AY34" s="45"/>
+      <c r="AZ34" s="45"/>
+      <c r="BA34" s="45"/>
+      <c r="BB34" s="45"/>
+      <c r="BC34" s="45"/>
+      <c r="BD34" s="45"/>
+      <c r="BE34" s="45"/>
+      <c r="BF34" s="45"/>
+      <c r="BG34" s="45"/>
+      <c r="BH34" s="45"/>
+      <c r="BI34" s="45"/>
+      <c r="BJ34" s="45"/>
+      <c r="BK34" s="45"/>
+      <c r="BL34" s="45"/>
+      <c r="BM34" s="45"/>
+      <c r="BN34" s="45"/>
+      <c r="BO34" s="45"/>
+      <c r="BP34" s="45"/>
+      <c r="BQ34" s="45"/>
+      <c r="BR34" s="45"/>
+      <c r="BS34" s="45"/>
+      <c r="BT34" s="45"/>
+      <c r="BU34" s="45"/>
+      <c r="BV34" s="45"/>
+      <c r="BW34" s="45"/>
+      <c r="BX34" s="45"/>
+      <c r="BY34" s="45"/>
+      <c r="BZ34" s="45"/>
+      <c r="CA34" s="45"/>
+      <c r="CB34" s="46"/>
+    </row>
+    <row r="35" spans="3:80" ht="9.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C35" s="44"/>
+      <c r="D35" s="45"/>
+      <c r="E35" s="45"/>
+      <c r="F35" s="45"/>
+      <c r="G35" s="45"/>
+      <c r="H35" s="45"/>
+      <c r="I35" s="45"/>
+      <c r="J35" s="45"/>
+      <c r="K35" s="45"/>
+      <c r="L35" s="45"/>
+      <c r="M35" s="45"/>
+      <c r="N35" s="45"/>
+      <c r="O35" s="45"/>
+      <c r="P35" s="45"/>
+      <c r="Q35" s="45"/>
+      <c r="R35" s="45"/>
+      <c r="S35" s="45"/>
+      <c r="T35" s="45"/>
+      <c r="U35" s="45"/>
+      <c r="V35" s="45"/>
+      <c r="W35" s="45"/>
+      <c r="X35" s="45"/>
+      <c r="Y35" s="45"/>
+      <c r="Z35" s="45"/>
+      <c r="AA35" s="45"/>
+      <c r="AB35" s="45"/>
+      <c r="AC35" s="45"/>
+      <c r="AD35" s="45"/>
+      <c r="AE35" s="45"/>
+      <c r="AF35" s="45"/>
+      <c r="AG35" s="45"/>
+      <c r="AH35" s="45"/>
+      <c r="AI35" s="45"/>
+      <c r="AJ35" s="45"/>
+      <c r="AK35" s="45"/>
+      <c r="AL35" s="45"/>
+      <c r="AM35" s="45"/>
+      <c r="AN35" s="46"/>
+      <c r="AQ35" s="44"/>
+      <c r="AR35" s="45"/>
+      <c r="AS35" s="45"/>
+      <c r="AT35" s="45"/>
+      <c r="AU35" s="45"/>
+      <c r="AV35" s="45"/>
+      <c r="AW35" s="45"/>
+      <c r="AX35" s="45"/>
+      <c r="AY35" s="45"/>
+      <c r="AZ35" s="45"/>
+      <c r="BA35" s="45"/>
+      <c r="BB35" s="45"/>
+      <c r="BC35" s="45"/>
+      <c r="BD35" s="45"/>
+      <c r="BE35" s="45"/>
+      <c r="BF35" s="45"/>
+      <c r="BG35" s="45"/>
+      <c r="BH35" s="45"/>
+      <c r="BI35" s="45"/>
+      <c r="BJ35" s="45"/>
+      <c r="BK35" s="45"/>
+      <c r="BL35" s="45"/>
+      <c r="BM35" s="45"/>
+      <c r="BN35" s="45"/>
+      <c r="BO35" s="45"/>
+      <c r="BP35" s="45"/>
+      <c r="BQ35" s="45"/>
+      <c r="BR35" s="45"/>
+      <c r="BS35" s="45"/>
+      <c r="BT35" s="45"/>
+      <c r="BU35" s="45"/>
+      <c r="BV35" s="45"/>
+      <c r="BW35" s="45"/>
+      <c r="BX35" s="45"/>
+      <c r="BY35" s="45"/>
+      <c r="BZ35" s="45"/>
+      <c r="CA35" s="45"/>
+      <c r="CB35" s="46"/>
+    </row>
+    <row r="36" spans="3:80" ht="9.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C36" s="44"/>
+      <c r="D36" s="45"/>
+      <c r="E36" s="45"/>
+      <c r="F36" s="45"/>
+      <c r="G36" s="45"/>
+      <c r="H36" s="45"/>
+      <c r="I36" s="45"/>
+      <c r="J36" s="45"/>
+      <c r="K36" s="45"/>
+      <c r="L36" s="45"/>
+      <c r="M36" s="45"/>
+      <c r="N36" s="45"/>
+      <c r="O36" s="45"/>
+      <c r="P36" s="45"/>
+      <c r="Q36" s="45"/>
+      <c r="R36" s="45"/>
+      <c r="S36" s="45"/>
+      <c r="T36" s="45"/>
+      <c r="U36" s="45"/>
+      <c r="V36" s="45"/>
+      <c r="W36" s="45"/>
+      <c r="X36" s="45"/>
+      <c r="Y36" s="45"/>
+      <c r="Z36" s="45"/>
+      <c r="AA36" s="45"/>
+      <c r="AB36" s="45"/>
+      <c r="AC36" s="45"/>
+      <c r="AD36" s="45"/>
+      <c r="AE36" s="45"/>
+      <c r="AF36" s="45"/>
+      <c r="AG36" s="45"/>
+      <c r="AH36" s="45"/>
+      <c r="AI36" s="45"/>
+      <c r="AJ36" s="45"/>
+      <c r="AK36" s="45"/>
+      <c r="AL36" s="45"/>
+      <c r="AM36" s="45"/>
+      <c r="AN36" s="46"/>
+      <c r="AQ36" s="44"/>
+      <c r="AR36" s="45"/>
+      <c r="AS36" s="45"/>
+      <c r="AT36" s="45"/>
+      <c r="AU36" s="45"/>
+      <c r="AV36" s="45"/>
+      <c r="AW36" s="45"/>
+      <c r="AX36" s="45"/>
+      <c r="AY36" s="45"/>
+      <c r="AZ36" s="45"/>
+      <c r="BA36" s="45"/>
+      <c r="BB36" s="45"/>
+      <c r="BC36" s="45"/>
+      <c r="BD36" s="45"/>
+      <c r="BE36" s="45"/>
+      <c r="BF36" s="45"/>
+      <c r="BG36" s="45"/>
+      <c r="BH36" s="45"/>
+      <c r="BI36" s="45"/>
+      <c r="BJ36" s="45"/>
+      <c r="BK36" s="45"/>
+      <c r="BL36" s="45"/>
+      <c r="BM36" s="45"/>
+      <c r="BN36" s="45"/>
+      <c r="BO36" s="45"/>
+      <c r="BP36" s="45"/>
+      <c r="BQ36" s="45"/>
+      <c r="BR36" s="45"/>
+      <c r="BS36" s="45"/>
+      <c r="BT36" s="45"/>
+      <c r="BU36" s="45"/>
+      <c r="BV36" s="45"/>
+      <c r="BW36" s="45"/>
+      <c r="BX36" s="45"/>
+      <c r="BY36" s="45"/>
+      <c r="BZ36" s="45"/>
+      <c r="CA36" s="45"/>
+      <c r="CB36" s="46"/>
+    </row>
+    <row r="37" spans="3:80" ht="9.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C37" s="44"/>
+      <c r="D37" s="45"/>
+      <c r="E37" s="45"/>
+      <c r="F37" s="45"/>
+      <c r="G37" s="45"/>
+      <c r="H37" s="45"/>
+      <c r="I37" s="45"/>
+      <c r="J37" s="45"/>
+      <c r="K37" s="45"/>
+      <c r="L37" s="45"/>
+      <c r="M37" s="45"/>
+      <c r="N37" s="45"/>
+      <c r="O37" s="45"/>
+      <c r="P37" s="45"/>
+      <c r="Q37" s="45"/>
+      <c r="R37" s="45"/>
+      <c r="S37" s="45"/>
+      <c r="T37" s="45"/>
+      <c r="U37" s="45"/>
+      <c r="V37" s="45"/>
+      <c r="W37" s="45"/>
+      <c r="X37" s="45"/>
+      <c r="Y37" s="45"/>
+      <c r="Z37" s="45"/>
+      <c r="AA37" s="45"/>
+      <c r="AB37" s="45"/>
+      <c r="AC37" s="45"/>
+      <c r="AD37" s="45"/>
+      <c r="AE37" s="45"/>
+      <c r="AF37" s="45"/>
+      <c r="AG37" s="45"/>
+      <c r="AH37" s="45"/>
+      <c r="AI37" s="45"/>
+      <c r="AJ37" s="45"/>
+      <c r="AK37" s="45"/>
+      <c r="AL37" s="45"/>
+      <c r="AM37" s="45"/>
+      <c r="AN37" s="46"/>
+      <c r="AQ37" s="44"/>
+      <c r="AR37" s="45"/>
+      <c r="AS37" s="45"/>
+      <c r="AT37" s="45"/>
+      <c r="AU37" s="45"/>
+      <c r="AV37" s="45"/>
+      <c r="AW37" s="45"/>
+      <c r="AX37" s="45"/>
+      <c r="AY37" s="45"/>
+      <c r="AZ37" s="45"/>
+      <c r="BA37" s="45"/>
+      <c r="BB37" s="45"/>
+      <c r="BC37" s="45"/>
+      <c r="BD37" s="45"/>
+      <c r="BE37" s="45"/>
+      <c r="BF37" s="45"/>
+      <c r="BG37" s="45"/>
+      <c r="BH37" s="45"/>
+      <c r="BI37" s="45"/>
+      <c r="BJ37" s="45"/>
+      <c r="BK37" s="45"/>
+      <c r="BL37" s="45"/>
+      <c r="BM37" s="45"/>
+      <c r="BN37" s="45"/>
+      <c r="BO37" s="45"/>
+      <c r="BP37" s="45"/>
+      <c r="BQ37" s="45"/>
+      <c r="BR37" s="45"/>
+      <c r="BS37" s="45"/>
+      <c r="BT37" s="45"/>
+      <c r="BU37" s="45"/>
+      <c r="BV37" s="45"/>
+      <c r="BW37" s="45"/>
+      <c r="BX37" s="45"/>
+      <c r="BY37" s="45"/>
+      <c r="BZ37" s="45"/>
+      <c r="CA37" s="45"/>
+      <c r="CB37" s="46"/>
+    </row>
+    <row r="38" spans="3:80" ht="9.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C38" s="44"/>
+      <c r="D38" s="45"/>
+      <c r="E38" s="45"/>
+      <c r="F38" s="45"/>
+      <c r="G38" s="45"/>
+      <c r="H38" s="45"/>
+      <c r="I38" s="45"/>
+      <c r="J38" s="45"/>
+      <c r="K38" s="45"/>
+      <c r="L38" s="45"/>
+      <c r="M38" s="45"/>
+      <c r="N38" s="45"/>
+      <c r="O38" s="45"/>
+      <c r="P38" s="45"/>
+      <c r="Q38" s="45"/>
+      <c r="R38" s="45"/>
+      <c r="S38" s="45"/>
+      <c r="T38" s="45"/>
+      <c r="U38" s="45"/>
+      <c r="V38" s="45"/>
+      <c r="W38" s="45"/>
+      <c r="X38" s="45"/>
+      <c r="Y38" s="45"/>
+      <c r="Z38" s="45"/>
+      <c r="AA38" s="45"/>
+      <c r="AB38" s="45"/>
+      <c r="AC38" s="45"/>
+      <c r="AD38" s="45"/>
+      <c r="AE38" s="45"/>
+      <c r="AF38" s="45"/>
+      <c r="AG38" s="45"/>
+      <c r="AH38" s="45"/>
+      <c r="AI38" s="45"/>
+      <c r="AJ38" s="45"/>
+      <c r="AK38" s="45"/>
+      <c r="AL38" s="45"/>
+      <c r="AM38" s="45"/>
+      <c r="AN38" s="46"/>
+      <c r="AQ38" s="44"/>
+      <c r="AR38" s="45"/>
+      <c r="AS38" s="45"/>
+      <c r="AT38" s="45"/>
+      <c r="AU38" s="45"/>
+      <c r="AV38" s="45"/>
+      <c r="AW38" s="45"/>
+      <c r="AX38" s="45"/>
+      <c r="AY38" s="45"/>
+      <c r="AZ38" s="45"/>
+      <c r="BA38" s="45"/>
+      <c r="BB38" s="45"/>
+      <c r="BC38" s="45"/>
+      <c r="BD38" s="45"/>
+      <c r="BE38" s="45"/>
+      <c r="BF38" s="45"/>
+      <c r="BG38" s="45"/>
+      <c r="BH38" s="45"/>
+      <c r="BI38" s="45"/>
+      <c r="BJ38" s="45"/>
+      <c r="BK38" s="45"/>
+      <c r="BL38" s="45"/>
+      <c r="BM38" s="45"/>
+      <c r="BN38" s="45"/>
+      <c r="BO38" s="45"/>
+      <c r="BP38" s="45"/>
+      <c r="BQ38" s="45"/>
+      <c r="BR38" s="45"/>
+      <c r="BS38" s="45"/>
+      <c r="BT38" s="45"/>
+      <c r="BU38" s="45"/>
+      <c r="BV38" s="45"/>
+      <c r="BW38" s="45"/>
+      <c r="BX38" s="45"/>
+      <c r="BY38" s="45"/>
+      <c r="BZ38" s="45"/>
+      <c r="CA38" s="45"/>
+      <c r="CB38" s="46"/>
+    </row>
+    <row r="39" spans="3:80" ht="9.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C39" s="44"/>
+      <c r="D39" s="45"/>
+      <c r="E39" s="45"/>
+      <c r="F39" s="45"/>
+      <c r="G39" s="45"/>
+      <c r="H39" s="45"/>
+      <c r="I39" s="45"/>
+      <c r="J39" s="45"/>
+      <c r="K39" s="45"/>
+      <c r="L39" s="45"/>
+      <c r="M39" s="45"/>
+      <c r="N39" s="45"/>
+      <c r="O39" s="45"/>
+      <c r="P39" s="45"/>
+      <c r="Q39" s="45"/>
+      <c r="R39" s="45"/>
+      <c r="S39" s="45"/>
+      <c r="T39" s="45"/>
+      <c r="U39" s="45"/>
+      <c r="V39" s="45"/>
+      <c r="W39" s="45"/>
+      <c r="X39" s="45"/>
+      <c r="Y39" s="45"/>
+      <c r="Z39" s="45"/>
+      <c r="AA39" s="45"/>
+      <c r="AB39" s="45"/>
+      <c r="AC39" s="45"/>
+      <c r="AD39" s="45"/>
+      <c r="AE39" s="45"/>
+      <c r="AF39" s="45"/>
+      <c r="AG39" s="45"/>
+      <c r="AH39" s="45"/>
+      <c r="AI39" s="45"/>
+      <c r="AJ39" s="45"/>
+      <c r="AK39" s="45"/>
+      <c r="AL39" s="45"/>
+      <c r="AM39" s="45"/>
+      <c r="AN39" s="46"/>
+      <c r="AQ39" s="44"/>
+      <c r="AR39" s="45"/>
+      <c r="AS39" s="45"/>
+      <c r="AT39" s="45"/>
+      <c r="AU39" s="45"/>
+      <c r="AV39" s="45"/>
+      <c r="AW39" s="45"/>
+      <c r="AX39" s="45"/>
+      <c r="AY39" s="45"/>
+      <c r="AZ39" s="45"/>
+      <c r="BA39" s="45"/>
+      <c r="BB39" s="45"/>
+      <c r="BC39" s="45"/>
+      <c r="BD39" s="45"/>
+      <c r="BE39" s="45"/>
+      <c r="BF39" s="45"/>
+      <c r="BG39" s="45"/>
+      <c r="BH39" s="45"/>
+      <c r="BI39" s="45"/>
+      <c r="BJ39" s="45"/>
+      <c r="BK39" s="45"/>
+      <c r="BL39" s="45"/>
+      <c r="BM39" s="45"/>
+      <c r="BN39" s="45"/>
+      <c r="BO39" s="45"/>
+      <c r="BP39" s="45"/>
+      <c r="BQ39" s="45"/>
+      <c r="BR39" s="45"/>
+      <c r="BS39" s="45"/>
+      <c r="BT39" s="45"/>
+      <c r="BU39" s="45"/>
+      <c r="BV39" s="45"/>
+      <c r="BW39" s="45"/>
+      <c r="BX39" s="45"/>
+      <c r="BY39" s="45"/>
+      <c r="BZ39" s="45"/>
+      <c r="CA39" s="45"/>
+      <c r="CB39" s="46"/>
+    </row>
+    <row r="40" spans="3:80" ht="9.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C40" s="44"/>
+      <c r="D40" s="45"/>
+      <c r="E40" s="45"/>
+      <c r="F40" s="45"/>
+      <c r="G40" s="45"/>
+      <c r="H40" s="45"/>
+      <c r="I40" s="45"/>
+      <c r="J40" s="45"/>
+      <c r="K40" s="45"/>
+      <c r="L40" s="45"/>
+      <c r="M40" s="45"/>
+      <c r="N40" s="45"/>
+      <c r="O40" s="45"/>
+      <c r="P40" s="45"/>
+      <c r="Q40" s="45"/>
+      <c r="R40" s="45"/>
+      <c r="S40" s="45"/>
+      <c r="T40" s="45"/>
+      <c r="U40" s="45"/>
+      <c r="V40" s="45"/>
+      <c r="W40" s="45"/>
+      <c r="X40" s="45"/>
+      <c r="Y40" s="45"/>
+      <c r="Z40" s="45"/>
+      <c r="AA40" s="45"/>
+      <c r="AB40" s="45"/>
+      <c r="AC40" s="45"/>
+      <c r="AD40" s="45"/>
+      <c r="AE40" s="45"/>
+      <c r="AF40" s="45"/>
+      <c r="AG40" s="45"/>
+      <c r="AH40" s="45"/>
+      <c r="AI40" s="45"/>
+      <c r="AJ40" s="45"/>
+      <c r="AK40" s="45"/>
+      <c r="AL40" s="45"/>
+      <c r="AM40" s="45"/>
+      <c r="AN40" s="46"/>
+      <c r="AQ40" s="44"/>
+      <c r="AR40" s="45"/>
+      <c r="AS40" s="45"/>
+      <c r="AT40" s="45"/>
+      <c r="AU40" s="45"/>
+      <c r="AV40" s="45"/>
+      <c r="AW40" s="45"/>
+      <c r="AX40" s="45"/>
+      <c r="AY40" s="45"/>
+      <c r="AZ40" s="45"/>
+      <c r="BA40" s="45"/>
+      <c r="BB40" s="45"/>
+      <c r="BC40" s="45"/>
+      <c r="BD40" s="45"/>
+      <c r="BE40" s="45"/>
+      <c r="BF40" s="45"/>
+      <c r="BG40" s="45"/>
+      <c r="BH40" s="45"/>
+      <c r="BI40" s="45"/>
+      <c r="BJ40" s="45"/>
+      <c r="BK40" s="45"/>
+      <c r="BL40" s="45"/>
+      <c r="BM40" s="45"/>
+      <c r="BN40" s="45"/>
+      <c r="BO40" s="45"/>
+      <c r="BP40" s="45"/>
+      <c r="BQ40" s="45"/>
+      <c r="BR40" s="45"/>
+      <c r="BS40" s="45"/>
+      <c r="BT40" s="45"/>
+      <c r="BU40" s="45"/>
+      <c r="BV40" s="45"/>
+      <c r="BW40" s="45"/>
+      <c r="BX40" s="45"/>
+      <c r="BY40" s="45"/>
+      <c r="BZ40" s="45"/>
+      <c r="CA40" s="45"/>
+      <c r="CB40" s="46"/>
+    </row>
+    <row r="41" spans="3:80" ht="9.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C41" s="44"/>
+      <c r="D41" s="45"/>
+      <c r="E41" s="45"/>
+      <c r="F41" s="45"/>
+      <c r="G41" s="45"/>
+      <c r="H41" s="45"/>
+      <c r="I41" s="45"/>
+      <c r="J41" s="45"/>
+      <c r="K41" s="45"/>
+      <c r="L41" s="45"/>
+      <c r="M41" s="45"/>
+      <c r="N41" s="45"/>
+      <c r="O41" s="45"/>
+      <c r="P41" s="45"/>
+      <c r="Q41" s="45"/>
+      <c r="R41" s="45"/>
+      <c r="S41" s="45"/>
+      <c r="T41" s="45"/>
+      <c r="U41" s="45"/>
+      <c r="V41" s="45"/>
+      <c r="W41" s="45"/>
+      <c r="X41" s="45"/>
+      <c r="Y41" s="45"/>
+      <c r="Z41" s="45"/>
+      <c r="AA41" s="45"/>
+      <c r="AB41" s="45"/>
+      <c r="AC41" s="45"/>
+      <c r="AD41" s="45"/>
+      <c r="AE41" s="45"/>
+      <c r="AF41" s="45"/>
+      <c r="AG41" s="45"/>
+      <c r="AH41" s="45"/>
+      <c r="AI41" s="45"/>
+      <c r="AJ41" s="45"/>
+      <c r="AK41" s="45"/>
+      <c r="AL41" s="45"/>
+      <c r="AM41" s="45"/>
+      <c r="AN41" s="46"/>
+      <c r="AQ41" s="44"/>
+      <c r="AR41" s="45"/>
+      <c r="AS41" s="45"/>
+      <c r="AT41" s="45"/>
+      <c r="AU41" s="45"/>
+      <c r="AV41" s="45"/>
+      <c r="AW41" s="45"/>
+      <c r="AX41" s="45"/>
+      <c r="AY41" s="45"/>
+      <c r="AZ41" s="45"/>
+      <c r="BA41" s="45"/>
+      <c r="BB41" s="45"/>
+      <c r="BC41" s="45"/>
+      <c r="BD41" s="45"/>
+      <c r="BE41" s="45"/>
+      <c r="BF41" s="45"/>
+      <c r="BG41" s="45"/>
+      <c r="BH41" s="45"/>
+      <c r="BI41" s="45"/>
+      <c r="BJ41" s="45"/>
+      <c r="BK41" s="45"/>
+      <c r="BL41" s="45"/>
+      <c r="BM41" s="45"/>
+      <c r="BN41" s="45"/>
+      <c r="BO41" s="45"/>
+      <c r="BP41" s="45"/>
+      <c r="BQ41" s="45"/>
+      <c r="BR41" s="45"/>
+      <c r="BS41" s="45"/>
+      <c r="BT41" s="45"/>
+      <c r="BU41" s="45"/>
+      <c r="BV41" s="45"/>
+      <c r="BW41" s="45"/>
+      <c r="BX41" s="45"/>
+      <c r="BY41" s="45"/>
+      <c r="BZ41" s="45"/>
+      <c r="CA41" s="45"/>
+      <c r="CB41" s="46"/>
+    </row>
+    <row r="42" spans="3:80" ht="9.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C42" s="44"/>
+      <c r="D42" s="45"/>
+      <c r="E42" s="45"/>
+      <c r="F42" s="45"/>
+      <c r="G42" s="45"/>
+      <c r="H42" s="45"/>
+      <c r="I42" s="45"/>
+      <c r="J42" s="45"/>
+      <c r="K42" s="45"/>
+      <c r="L42" s="45"/>
+      <c r="M42" s="45"/>
+      <c r="N42" s="45"/>
+      <c r="O42" s="45"/>
+      <c r="P42" s="45"/>
+      <c r="Q42" s="45"/>
+      <c r="R42" s="45"/>
+      <c r="S42" s="45"/>
+      <c r="T42" s="45"/>
+      <c r="U42" s="45"/>
+      <c r="V42" s="45"/>
+      <c r="W42" s="45"/>
+      <c r="X42" s="45"/>
+      <c r="Y42" s="45"/>
+      <c r="Z42" s="45"/>
+      <c r="AA42" s="45"/>
+      <c r="AB42" s="45"/>
+      <c r="AC42" s="45"/>
+      <c r="AD42" s="45"/>
+      <c r="AE42" s="45"/>
+      <c r="AF42" s="45"/>
+      <c r="AG42" s="45"/>
+      <c r="AH42" s="45"/>
+      <c r="AI42" s="45"/>
+      <c r="AJ42" s="45"/>
+      <c r="AK42" s="45"/>
+      <c r="AL42" s="45"/>
+      <c r="AM42" s="45"/>
+      <c r="AN42" s="46"/>
+      <c r="AQ42" s="44"/>
+      <c r="AR42" s="45"/>
+      <c r="AS42" s="45"/>
+      <c r="AT42" s="45"/>
+      <c r="AU42" s="45"/>
+      <c r="AV42" s="45"/>
+      <c r="AW42" s="45"/>
+      <c r="AX42" s="45"/>
+      <c r="AY42" s="45"/>
+      <c r="AZ42" s="45"/>
+      <c r="BA42" s="45"/>
+      <c r="BB42" s="45"/>
+      <c r="BC42" s="45"/>
+      <c r="BD42" s="45"/>
+      <c r="BE42" s="45"/>
+      <c r="BF42" s="45"/>
+      <c r="BG42" s="45"/>
+      <c r="BH42" s="45"/>
+      <c r="BI42" s="45"/>
+      <c r="BJ42" s="45"/>
+      <c r="BK42" s="45"/>
+      <c r="BL42" s="45"/>
+      <c r="BM42" s="45"/>
+      <c r="BN42" s="45"/>
+      <c r="BO42" s="45"/>
+      <c r="BP42" s="45"/>
+      <c r="BQ42" s="45"/>
+      <c r="BR42" s="45"/>
+      <c r="BS42" s="45"/>
+      <c r="BT42" s="45"/>
+      <c r="BU42" s="45"/>
+      <c r="BV42" s="45"/>
+      <c r="BW42" s="45"/>
+      <c r="BX42" s="45"/>
+      <c r="BY42" s="45"/>
+      <c r="BZ42" s="45"/>
+      <c r="CA42" s="45"/>
+      <c r="CB42" s="46"/>
+    </row>
+    <row r="43" spans="3:80" ht="9.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C43" s="44"/>
+      <c r="D43" s="45"/>
+      <c r="E43" s="45"/>
+      <c r="F43" s="45"/>
+      <c r="G43" s="45"/>
+      <c r="H43" s="45"/>
+      <c r="I43" s="45"/>
+      <c r="J43" s="45"/>
+      <c r="K43" s="45"/>
+      <c r="L43" s="45"/>
+      <c r="M43" s="45"/>
+      <c r="N43" s="45"/>
+      <c r="O43" s="45"/>
+      <c r="P43" s="45"/>
+      <c r="Q43" s="45"/>
+      <c r="R43" s="45"/>
+      <c r="S43" s="45"/>
+      <c r="T43" s="45"/>
+      <c r="U43" s="45"/>
+      <c r="V43" s="45"/>
+      <c r="W43" s="45"/>
+      <c r="X43" s="45"/>
+      <c r="Y43" s="45"/>
+      <c r="Z43" s="45"/>
+      <c r="AA43" s="45"/>
+      <c r="AB43" s="45"/>
+      <c r="AC43" s="45"/>
+      <c r="AD43" s="45"/>
+      <c r="AE43" s="45"/>
+      <c r="AF43" s="45"/>
+      <c r="AG43" s="45"/>
+      <c r="AH43" s="45"/>
+      <c r="AI43" s="45"/>
+      <c r="AJ43" s="45"/>
+      <c r="AK43" s="45"/>
+      <c r="AL43" s="45"/>
+      <c r="AM43" s="45"/>
+      <c r="AN43" s="46"/>
+      <c r="AQ43" s="44"/>
+      <c r="AR43" s="45"/>
+      <c r="AS43" s="45"/>
+      <c r="AT43" s="45"/>
+      <c r="AU43" s="45"/>
+      <c r="AV43" s="45"/>
+      <c r="AW43" s="45"/>
+      <c r="AX43" s="45"/>
+      <c r="AY43" s="45"/>
+      <c r="AZ43" s="45"/>
+      <c r="BA43" s="45"/>
+      <c r="BB43" s="45"/>
+      <c r="BC43" s="45"/>
+      <c r="BD43" s="45"/>
+      <c r="BE43" s="45"/>
+      <c r="BF43" s="45"/>
+      <c r="BG43" s="45"/>
+      <c r="BH43" s="45"/>
+      <c r="BI43" s="45"/>
+      <c r="BJ43" s="45"/>
+      <c r="BK43" s="45"/>
+      <c r="BL43" s="45"/>
+      <c r="BM43" s="45"/>
+      <c r="BN43" s="45"/>
+      <c r="BO43" s="45"/>
+      <c r="BP43" s="45"/>
+      <c r="BQ43" s="45"/>
+      <c r="BR43" s="45"/>
+      <c r="BS43" s="45"/>
+      <c r="BT43" s="45"/>
+      <c r="BU43" s="45"/>
+      <c r="BV43" s="45"/>
+      <c r="BW43" s="45"/>
+      <c r="BX43" s="45"/>
+      <c r="BY43" s="45"/>
+      <c r="BZ43" s="45"/>
+      <c r="CA43" s="45"/>
+      <c r="CB43" s="46"/>
+    </row>
+    <row r="44" spans="3:80" ht="9.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C44" s="44"/>
+      <c r="D44" s="45"/>
+      <c r="E44" s="45"/>
+      <c r="F44" s="45"/>
+      <c r="G44" s="45"/>
+      <c r="H44" s="45"/>
+      <c r="I44" s="45"/>
+      <c r="J44" s="45"/>
+      <c r="K44" s="45"/>
+      <c r="L44" s="45"/>
+      <c r="M44" s="45"/>
+      <c r="N44" s="45"/>
+      <c r="O44" s="45"/>
+      <c r="P44" s="45"/>
+      <c r="Q44" s="45"/>
+      <c r="R44" s="45"/>
+      <c r="S44" s="45"/>
+      <c r="T44" s="45"/>
+      <c r="U44" s="45"/>
+      <c r="V44" s="45"/>
+      <c r="W44" s="45"/>
+      <c r="X44" s="45"/>
+      <c r="Y44" s="45"/>
+      <c r="Z44" s="45"/>
+      <c r="AA44" s="45"/>
+      <c r="AB44" s="45"/>
+      <c r="AC44" s="45"/>
+      <c r="AD44" s="45"/>
+      <c r="AE44" s="45"/>
+      <c r="AF44" s="45"/>
+      <c r="AG44" s="45"/>
+      <c r="AH44" s="45"/>
+      <c r="AI44" s="45"/>
+      <c r="AJ44" s="45"/>
+      <c r="AK44" s="45"/>
+      <c r="AL44" s="45"/>
+      <c r="AM44" s="45"/>
+      <c r="AN44" s="46"/>
+      <c r="AQ44" s="44"/>
+      <c r="AR44" s="45"/>
+      <c r="AS44" s="45"/>
+      <c r="AT44" s="45"/>
+      <c r="AU44" s="45"/>
+      <c r="AV44" s="45"/>
+      <c r="AW44" s="45"/>
+      <c r="AX44" s="45"/>
+      <c r="AY44" s="45"/>
+      <c r="AZ44" s="45"/>
+      <c r="BA44" s="45"/>
+      <c r="BB44" s="45"/>
+      <c r="BC44" s="45"/>
+      <c r="BD44" s="45"/>
+      <c r="BE44" s="45"/>
+      <c r="BF44" s="45"/>
+      <c r="BG44" s="45"/>
+      <c r="BH44" s="45"/>
+      <c r="BI44" s="45"/>
+      <c r="BJ44" s="45"/>
+      <c r="BK44" s="45"/>
+      <c r="BL44" s="45"/>
+      <c r="BM44" s="45"/>
+      <c r="BN44" s="45"/>
+      <c r="BO44" s="45"/>
+      <c r="BP44" s="45"/>
+      <c r="BQ44" s="45"/>
+      <c r="BR44" s="45"/>
+      <c r="BS44" s="45"/>
+      <c r="BT44" s="45"/>
+      <c r="BU44" s="45"/>
+      <c r="BV44" s="45"/>
+      <c r="BW44" s="45"/>
+      <c r="BX44" s="45"/>
+      <c r="BY44" s="45"/>
+      <c r="BZ44" s="45"/>
+      <c r="CA44" s="45"/>
+      <c r="CB44" s="46"/>
+    </row>
+    <row r="45" spans="3:80" ht="9.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C45" s="44"/>
+      <c r="D45" s="45"/>
+      <c r="E45" s="45"/>
+      <c r="F45" s="45"/>
+      <c r="G45" s="45"/>
+      <c r="H45" s="45"/>
+      <c r="I45" s="45"/>
+      <c r="J45" s="45"/>
+      <c r="K45" s="45"/>
+      <c r="L45" s="45"/>
+      <c r="M45" s="45"/>
+      <c r="N45" s="45"/>
+      <c r="O45" s="45"/>
+      <c r="P45" s="45"/>
+      <c r="Q45" s="45"/>
+      <c r="R45" s="45"/>
+      <c r="S45" s="45"/>
+      <c r="T45" s="45"/>
+      <c r="U45" s="45"/>
+      <c r="V45" s="45"/>
+      <c r="W45" s="45"/>
+      <c r="X45" s="45"/>
+      <c r="Y45" s="45"/>
+      <c r="Z45" s="45"/>
+      <c r="AA45" s="45"/>
+      <c r="AB45" s="45"/>
+      <c r="AC45" s="45"/>
+      <c r="AD45" s="45"/>
+      <c r="AE45" s="45"/>
+      <c r="AF45" s="45"/>
+      <c r="AG45" s="45"/>
+      <c r="AH45" s="45"/>
+      <c r="AI45" s="45"/>
+      <c r="AJ45" s="45"/>
+      <c r="AK45" s="45"/>
+      <c r="AL45" s="45"/>
+      <c r="AM45" s="45"/>
+      <c r="AN45" s="46"/>
+      <c r="AQ45" s="44"/>
+      <c r="AR45" s="45"/>
+      <c r="AS45" s="45"/>
+      <c r="AT45" s="45"/>
+      <c r="AU45" s="45"/>
+      <c r="AV45" s="45"/>
+      <c r="AW45" s="45"/>
+      <c r="AX45" s="45"/>
+      <c r="AY45" s="45"/>
+      <c r="AZ45" s="45"/>
+      <c r="BA45" s="45"/>
+      <c r="BB45" s="45"/>
+      <c r="BC45" s="45"/>
+      <c r="BD45" s="45"/>
+      <c r="BE45" s="45"/>
+      <c r="BF45" s="45"/>
+      <c r="BG45" s="45"/>
+      <c r="BH45" s="45"/>
+      <c r="BI45" s="45"/>
+      <c r="BJ45" s="45"/>
+      <c r="BK45" s="45"/>
+      <c r="BL45" s="45"/>
+      <c r="BM45" s="45"/>
+      <c r="BN45" s="45"/>
+      <c r="BO45" s="45"/>
+      <c r="BP45" s="45"/>
+      <c r="BQ45" s="45"/>
+      <c r="BR45" s="45"/>
+      <c r="BS45" s="45"/>
+      <c r="BT45" s="45"/>
+      <c r="BU45" s="45"/>
+      <c r="BV45" s="45"/>
+      <c r="BW45" s="45"/>
+      <c r="BX45" s="45"/>
+      <c r="BY45" s="45"/>
+      <c r="BZ45" s="45"/>
+      <c r="CA45" s="45"/>
+      <c r="CB45" s="46"/>
+    </row>
+    <row r="46" spans="3:80" ht="9.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="C46" s="47"/>
+      <c r="D46" s="48"/>
+      <c r="E46" s="48"/>
+      <c r="F46" s="48"/>
+      <c r="G46" s="48"/>
+      <c r="H46" s="48"/>
+      <c r="I46" s="48"/>
+      <c r="J46" s="48"/>
+      <c r="K46" s="48"/>
+      <c r="L46" s="48"/>
+      <c r="M46" s="48"/>
+      <c r="N46" s="48"/>
+      <c r="O46" s="48"/>
+      <c r="P46" s="48"/>
+      <c r="Q46" s="48"/>
+      <c r="R46" s="48"/>
+      <c r="S46" s="48"/>
+      <c r="T46" s="48"/>
+      <c r="U46" s="48"/>
+      <c r="V46" s="48"/>
+      <c r="W46" s="48"/>
+      <c r="X46" s="48"/>
+      <c r="Y46" s="48"/>
+      <c r="Z46" s="48"/>
+      <c r="AA46" s="48"/>
+      <c r="AB46" s="48"/>
+      <c r="AC46" s="48"/>
+      <c r="AD46" s="48"/>
+      <c r="AE46" s="48"/>
+      <c r="AF46" s="48"/>
+      <c r="AG46" s="48"/>
+      <c r="AH46" s="48"/>
+      <c r="AI46" s="48"/>
+      <c r="AJ46" s="48"/>
+      <c r="AK46" s="48"/>
+      <c r="AL46" s="48"/>
+      <c r="AM46" s="48"/>
+      <c r="AN46" s="49"/>
+      <c r="AQ46" s="47"/>
+      <c r="AR46" s="48"/>
+      <c r="AS46" s="48"/>
+      <c r="AT46" s="48"/>
+      <c r="AU46" s="48"/>
+      <c r="AV46" s="48"/>
+      <c r="AW46" s="48"/>
+      <c r="AX46" s="48"/>
+      <c r="AY46" s="48"/>
+      <c r="AZ46" s="48"/>
+      <c r="BA46" s="48"/>
+      <c r="BB46" s="48"/>
+      <c r="BC46" s="48"/>
+      <c r="BD46" s="48"/>
+      <c r="BE46" s="48"/>
+      <c r="BF46" s="48"/>
+      <c r="BG46" s="48"/>
+      <c r="BH46" s="48"/>
+      <c r="BI46" s="48"/>
+      <c r="BJ46" s="48"/>
+      <c r="BK46" s="48"/>
+      <c r="BL46" s="48"/>
+      <c r="BM46" s="48"/>
+      <c r="BN46" s="48"/>
+      <c r="BO46" s="48"/>
+      <c r="BP46" s="48"/>
+      <c r="BQ46" s="48"/>
+      <c r="BR46" s="48"/>
+      <c r="BS46" s="48"/>
+      <c r="BT46" s="48"/>
+      <c r="BU46" s="48"/>
+      <c r="BV46" s="48"/>
+      <c r="BW46" s="48"/>
+      <c r="BX46" s="48"/>
+      <c r="BY46" s="48"/>
+      <c r="BZ46" s="48"/>
+      <c r="CA46" s="48"/>
+      <c r="CB46" s="49"/>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="C26:AN27"/>
+    <mergeCell ref="AQ26:CB27"/>
+    <mergeCell ref="C28:AN46"/>
+    <mergeCell ref="AQ28:CB46"/>
+    <mergeCell ref="BK2:CB3"/>
+    <mergeCell ref="BK4:CB7"/>
+    <mergeCell ref="C9:CB10"/>
+    <mergeCell ref="C11:CB24"/>
+    <mergeCell ref="W2:AN3"/>
+    <mergeCell ref="W4:AN7"/>
+    <mergeCell ref="AQ2:BH3"/>
+    <mergeCell ref="AQ4:BH7"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76A61A88-938B-4AD6-9405-2203B020D104}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.28515625" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B2" s="28">
+        <f>SUMIF(TB_Vendas[Vendedor],A2,TB_Vendas[Total])</f>
+        <v>6102.4499999999989</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" s="28">
+        <f>SUMIF(TB_Vendas[Vendedor],A3,TB_Vendas[Total])</f>
+        <v>4567.68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B4" s="28">
+        <f>SUMIF(TB_Vendas[Vendedor],A4,TB_Vendas[Total])</f>
+        <v>5293.5299999999988</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC7E0810-0AF5-486C-BF0B-FA2CB7F55421}">
+  <dimension ref="B3:Q26"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="2:17" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B3" s="87" t="s">
+        <v>95</v>
+      </c>
+      <c r="C3" s="87"/>
+      <c r="D3" s="87"/>
+      <c r="E3" s="87"/>
+      <c r="F3" s="87"/>
+    </row>
+    <row r="4" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="78" t="s">
+        <v>96</v>
+      </c>
+      <c r="D5" s="79"/>
+      <c r="E5" s="79"/>
+      <c r="F5" s="79"/>
+      <c r="G5" s="79"/>
+      <c r="H5" s="79"/>
+      <c r="I5" s="79"/>
+      <c r="J5" s="79"/>
+      <c r="K5" s="79"/>
+      <c r="L5" s="79"/>
+      <c r="M5" s="79"/>
+      <c r="N5" s="79"/>
+      <c r="O5" s="79"/>
+      <c r="P5" s="79"/>
+      <c r="Q5" s="81"/>
+    </row>
+    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C6" s="82"/>
+      <c r="D6" s="80"/>
+      <c r="E6" s="80"/>
+      <c r="F6" s="80"/>
+      <c r="G6" s="80"/>
+      <c r="H6" s="80"/>
+      <c r="I6" s="80"/>
+      <c r="J6" s="80"/>
+      <c r="K6" s="80"/>
+      <c r="L6" s="80"/>
+      <c r="M6" s="80"/>
+      <c r="N6" s="80"/>
+      <c r="O6" s="80"/>
+      <c r="P6" s="80"/>
+      <c r="Q6" s="83"/>
+    </row>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C7" s="82"/>
+      <c r="D7" s="80"/>
+      <c r="E7" s="80"/>
+      <c r="F7" s="80"/>
+      <c r="G7" s="80"/>
+      <c r="H7" s="80"/>
+      <c r="I7" s="80"/>
+      <c r="J7" s="80"/>
+      <c r="K7" s="80"/>
+      <c r="L7" s="80"/>
+      <c r="M7" s="80"/>
+      <c r="N7" s="80"/>
+      <c r="O7" s="80"/>
+      <c r="P7" s="80"/>
+      <c r="Q7" s="83"/>
+    </row>
+    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C8" s="82"/>
+      <c r="D8" s="80"/>
+      <c r="E8" s="80"/>
+      <c r="F8" s="80"/>
+      <c r="G8" s="80"/>
+      <c r="H8" s="80"/>
+      <c r="I8" s="80"/>
+      <c r="J8" s="80"/>
+      <c r="K8" s="80"/>
+      <c r="L8" s="80"/>
+      <c r="M8" s="80"/>
+      <c r="N8" s="80"/>
+      <c r="O8" s="80"/>
+      <c r="P8" s="80"/>
+      <c r="Q8" s="83"/>
+    </row>
+    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C9" s="82"/>
+      <c r="D9" s="80"/>
+      <c r="E9" s="80"/>
+      <c r="F9" s="80"/>
+      <c r="G9" s="80"/>
+      <c r="H9" s="80"/>
+      <c r="I9" s="80"/>
+      <c r="J9" s="80"/>
+      <c r="K9" s="80"/>
+      <c r="L9" s="80"/>
+      <c r="M9" s="80"/>
+      <c r="N9" s="80"/>
+      <c r="O9" s="80"/>
+      <c r="P9" s="80"/>
+      <c r="Q9" s="83"/>
+    </row>
+    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C10" s="82"/>
+      <c r="D10" s="80"/>
+      <c r="E10" s="80"/>
+      <c r="F10" s="80"/>
+      <c r="G10" s="80"/>
+      <c r="H10" s="80"/>
+      <c r="I10" s="80"/>
+      <c r="J10" s="80"/>
+      <c r="K10" s="80"/>
+      <c r="L10" s="80"/>
+      <c r="M10" s="80"/>
+      <c r="N10" s="80"/>
+      <c r="O10" s="80"/>
+      <c r="P10" s="80"/>
+      <c r="Q10" s="83"/>
+    </row>
+    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C11" s="82"/>
+      <c r="D11" s="80"/>
+      <c r="E11" s="80"/>
+      <c r="F11" s="80"/>
+      <c r="G11" s="80"/>
+      <c r="H11" s="80"/>
+      <c r="I11" s="80"/>
+      <c r="J11" s="80"/>
+      <c r="K11" s="80"/>
+      <c r="L11" s="80"/>
+      <c r="M11" s="80"/>
+      <c r="N11" s="80"/>
+      <c r="O11" s="80"/>
+      <c r="P11" s="80"/>
+      <c r="Q11" s="83"/>
+    </row>
+    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C12" s="82"/>
+      <c r="D12" s="80"/>
+      <c r="E12" s="80"/>
+      <c r="F12" s="80"/>
+      <c r="G12" s="80"/>
+      <c r="H12" s="80"/>
+      <c r="I12" s="80"/>
+      <c r="J12" s="80"/>
+      <c r="K12" s="80"/>
+      <c r="L12" s="80"/>
+      <c r="M12" s="80"/>
+      <c r="N12" s="80"/>
+      <c r="O12" s="80"/>
+      <c r="P12" s="80"/>
+      <c r="Q12" s="83"/>
+    </row>
+    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C13" s="82"/>
+      <c r="D13" s="80"/>
+      <c r="E13" s="80"/>
+      <c r="F13" s="80"/>
+      <c r="G13" s="80"/>
+      <c r="H13" s="80"/>
+      <c r="I13" s="80"/>
+      <c r="J13" s="80"/>
+      <c r="K13" s="80"/>
+      <c r="L13" s="80"/>
+      <c r="M13" s="80"/>
+      <c r="N13" s="80"/>
+      <c r="O13" s="80"/>
+      <c r="P13" s="80"/>
+      <c r="Q13" s="83"/>
+    </row>
+    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C14" s="82"/>
+      <c r="D14" s="80"/>
+      <c r="E14" s="80"/>
+      <c r="F14" s="80"/>
+      <c r="G14" s="80"/>
+      <c r="H14" s="80"/>
+      <c r="I14" s="80"/>
+      <c r="J14" s="80"/>
+      <c r="K14" s="80"/>
+      <c r="L14" s="80"/>
+      <c r="M14" s="80"/>
+      <c r="N14" s="80"/>
+      <c r="O14" s="80"/>
+      <c r="P14" s="80"/>
+      <c r="Q14" s="83"/>
+    </row>
+    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C15" s="82"/>
+      <c r="D15" s="80"/>
+      <c r="E15" s="80"/>
+      <c r="F15" s="80"/>
+      <c r="G15" s="80"/>
+      <c r="H15" s="80"/>
+      <c r="I15" s="80"/>
+      <c r="J15" s="80"/>
+      <c r="K15" s="80"/>
+      <c r="L15" s="80"/>
+      <c r="M15" s="80"/>
+      <c r="N15" s="80"/>
+      <c r="O15" s="80"/>
+      <c r="P15" s="80"/>
+      <c r="Q15" s="83"/>
+    </row>
+    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C16" s="82"/>
+      <c r="D16" s="80"/>
+      <c r="E16" s="80"/>
+      <c r="F16" s="80"/>
+      <c r="G16" s="80"/>
+      <c r="H16" s="80"/>
+      <c r="I16" s="80"/>
+      <c r="J16" s="80"/>
+      <c r="K16" s="80"/>
+      <c r="L16" s="80"/>
+      <c r="M16" s="80"/>
+      <c r="N16" s="80"/>
+      <c r="O16" s="80"/>
+      <c r="P16" s="80"/>
+      <c r="Q16" s="83"/>
+    </row>
+    <row r="17" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C17" s="82"/>
+      <c r="D17" s="80"/>
+      <c r="E17" s="80"/>
+      <c r="F17" s="80"/>
+      <c r="G17" s="80"/>
+      <c r="H17" s="80"/>
+      <c r="I17" s="80"/>
+      <c r="J17" s="80"/>
+      <c r="K17" s="80"/>
+      <c r="L17" s="80"/>
+      <c r="M17" s="80"/>
+      <c r="N17" s="80"/>
+      <c r="O17" s="80"/>
+      <c r="P17" s="80"/>
+      <c r="Q17" s="83"/>
+    </row>
+    <row r="18" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C18" s="82"/>
+      <c r="D18" s="80"/>
+      <c r="E18" s="80"/>
+      <c r="F18" s="80"/>
+      <c r="G18" s="80"/>
+      <c r="H18" s="80"/>
+      <c r="I18" s="80"/>
+      <c r="J18" s="80"/>
+      <c r="K18" s="80"/>
+      <c r="L18" s="80"/>
+      <c r="M18" s="80"/>
+      <c r="N18" s="80"/>
+      <c r="O18" s="80"/>
+      <c r="P18" s="80"/>
+      <c r="Q18" s="83"/>
+    </row>
+    <row r="19" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C19" s="82"/>
+      <c r="D19" s="80"/>
+      <c r="E19" s="80"/>
+      <c r="F19" s="80"/>
+      <c r="G19" s="80"/>
+      <c r="H19" s="80"/>
+      <c r="I19" s="80"/>
+      <c r="J19" s="80"/>
+      <c r="K19" s="80"/>
+      <c r="L19" s="80"/>
+      <c r="M19" s="80"/>
+      <c r="N19" s="80"/>
+      <c r="O19" s="80"/>
+      <c r="P19" s="80"/>
+      <c r="Q19" s="83"/>
+    </row>
+    <row r="20" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C20" s="82"/>
+      <c r="D20" s="80"/>
+      <c r="E20" s="80"/>
+      <c r="F20" s="80"/>
+      <c r="G20" s="80"/>
+      <c r="H20" s="80"/>
+      <c r="I20" s="80"/>
+      <c r="J20" s="80"/>
+      <c r="K20" s="80"/>
+      <c r="L20" s="80"/>
+      <c r="M20" s="80"/>
+      <c r="N20" s="80"/>
+      <c r="O20" s="80"/>
+      <c r="P20" s="80"/>
+      <c r="Q20" s="83"/>
+    </row>
+    <row r="21" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C21" s="82"/>
+      <c r="D21" s="80"/>
+      <c r="E21" s="80"/>
+      <c r="F21" s="80"/>
+      <c r="G21" s="80"/>
+      <c r="H21" s="80"/>
+      <c r="I21" s="80"/>
+      <c r="J21" s="80"/>
+      <c r="K21" s="80"/>
+      <c r="L21" s="80"/>
+      <c r="M21" s="80"/>
+      <c r="N21" s="80"/>
+      <c r="O21" s="80"/>
+      <c r="P21" s="80"/>
+      <c r="Q21" s="83"/>
+    </row>
+    <row r="22" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C22" s="82"/>
+      <c r="D22" s="80"/>
+      <c r="E22" s="80"/>
+      <c r="F22" s="80"/>
+      <c r="G22" s="80"/>
+      <c r="H22" s="80"/>
+      <c r="I22" s="80"/>
+      <c r="J22" s="80"/>
+      <c r="K22" s="80"/>
+      <c r="L22" s="80"/>
+      <c r="M22" s="80"/>
+      <c r="N22" s="80"/>
+      <c r="O22" s="80"/>
+      <c r="P22" s="80"/>
+      <c r="Q22" s="83"/>
+    </row>
+    <row r="23" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C23" s="82"/>
+      <c r="D23" s="80"/>
+      <c r="E23" s="80"/>
+      <c r="F23" s="80"/>
+      <c r="G23" s="80"/>
+      <c r="H23" s="80"/>
+      <c r="I23" s="80"/>
+      <c r="J23" s="80"/>
+      <c r="K23" s="80"/>
+      <c r="L23" s="80"/>
+      <c r="M23" s="80"/>
+      <c r="N23" s="80"/>
+      <c r="O23" s="80"/>
+      <c r="P23" s="80"/>
+      <c r="Q23" s="83"/>
+    </row>
+    <row r="24" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C24" s="82"/>
+      <c r="D24" s="80"/>
+      <c r="E24" s="80"/>
+      <c r="F24" s="80"/>
+      <c r="G24" s="80"/>
+      <c r="H24" s="80"/>
+      <c r="I24" s="80"/>
+      <c r="J24" s="80"/>
+      <c r="K24" s="80"/>
+      <c r="L24" s="80"/>
+      <c r="M24" s="80"/>
+      <c r="N24" s="80"/>
+      <c r="O24" s="80"/>
+      <c r="P24" s="80"/>
+      <c r="Q24" s="83"/>
+    </row>
+    <row r="25" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C25" s="82"/>
+      <c r="D25" s="80"/>
+      <c r="E25" s="80"/>
+      <c r="F25" s="80"/>
+      <c r="G25" s="80"/>
+      <c r="H25" s="80"/>
+      <c r="I25" s="80"/>
+      <c r="J25" s="80"/>
+      <c r="K25" s="80"/>
+      <c r="L25" s="80"/>
+      <c r="M25" s="80"/>
+      <c r="N25" s="80"/>
+      <c r="O25" s="80"/>
+      <c r="P25" s="80"/>
+      <c r="Q25" s="83"/>
+    </row>
+    <row r="26" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C26" s="84"/>
+      <c r="D26" s="85"/>
+      <c r="E26" s="85"/>
+      <c r="F26" s="85"/>
+      <c r="G26" s="85"/>
+      <c r="H26" s="85"/>
+      <c r="I26" s="85"/>
+      <c r="J26" s="85"/>
+      <c r="K26" s="85"/>
+      <c r="L26" s="85"/>
+      <c r="M26" s="85"/>
+      <c r="N26" s="85"/>
+      <c r="O26" s="85"/>
+      <c r="P26" s="85"/>
+      <c r="Q26" s="86"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C5:Q26"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87920B21-B994-41DD-BEC6-B8D0834CB666}">
   <dimension ref="A1:H4"/>
   <sheetViews>
@@ -6034,28 +10275,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="23" customFormat="1" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="56" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
     </row>
     <row r="2" spans="1:8" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="57" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="36"/>
-      <c r="D2" s="37"/>
-      <c r="F2" s="35" t="s">
+      <c r="C2" s="58"/>
+      <c r="D2" s="59"/>
+      <c r="F2" s="57" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="36"/>
-      <c r="H2" s="37"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="59"/>
     </row>
     <row r="3" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="25" t="s">
@@ -6118,7 +10359,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BBE6E77-EBCD-448B-AB61-14EA4DC9C25B}">
   <dimension ref="B2:H14"/>
   <sheetViews>

</xml_diff>

<commit_message>
Arquivo:03 - Gráfico 'Vendas e Qtde.' Dashboard
</commit_message>
<xml_diff>
--- a/03-Meteora_Ecommerce-Graficos-Formatos.xlsx
+++ b/03-Meteora_Ecommerce-Graficos-Formatos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafae\Meu Drive (mz.tears.of.time@gmail.com)\Dev\Cursos\Curso-003\001 - Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91A1AC75-43AB-41CB-A9B6-AAF157DDF92E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FF39844-8B4E-4DE2-A6D3-9475FE650E74}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4650" yWindow="0" windowWidth="23070" windowHeight="11505" firstSheet="2" activeTab="5" xr2:uid="{F6D97A53-F63B-4272-A181-44B26E0B790F}"/>
+    <workbookView xWindow="5580" yWindow="0" windowWidth="23070" windowHeight="11505" firstSheet="2" activeTab="5" xr2:uid="{F6D97A53-F63B-4272-A181-44B26E0B790F}"/>
   </bookViews>
   <sheets>
     <sheet name="Meu Gráfico" sheetId="6" state="hidden" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="109">
   <si>
     <t>Produtos</t>
   </si>
@@ -499,16 +499,47 @@
   <si>
     <t>Totais</t>
   </si>
+  <si>
+    <t>N.Mês</t>
+  </si>
+  <si>
+    <t>Meses</t>
+  </si>
+  <si>
+    <t>Jan</t>
+  </si>
+  <si>
+    <t>Fev</t>
+  </si>
+  <si>
+    <t>Mar</t>
+  </si>
+  <si>
+    <t>Abr</t>
+  </si>
+  <si>
+    <t>Mai</t>
+  </si>
+  <si>
+    <t>Jun</t>
+  </si>
+  <si>
+    <t>Qtde</t>
+  </si>
+  <si>
+    <t>COMBINAÇÃO Total e Qtde</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
+    <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="&quot;R$&quot;\ #,##0.00"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -606,6 +637,13 @@
     <font>
       <b/>
       <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -979,7 +1017,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -988,8 +1026,9 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="10" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="44" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1224,14 +1263,39 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="15" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="4" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Cabeçalho Meteora" xfId="3" xr:uid="{43DBFFA1-791E-423B-B2A6-377CC2810274}"/>
     <cellStyle name="Ênfase4" xfId="1" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Moeda" xfId="4" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Título Meteora" xfId="2" xr:uid="{52F1EA3C-B23E-4AE6-AE73-27AD9F7C9021}"/>
   </cellStyles>
   <dxfs count="21">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1267,16 +1331,6 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
@@ -1317,28 +1371,18 @@
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF4472C4"/>
+      <color rgb="FFA2B9DA"/>
+      <color rgb="FF000000"/>
       <color rgb="FFDAFF01"/>
       <color rgb="FFCCCCCC"/>
       <color rgb="FFF87F46"/>
       <color rgb="FFEE6471"/>
       <color rgb="FF9353FF"/>
-      <color rgb="FF4472C4"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1940,7 +1984,43 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="1"/>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -1951,41 +2031,42 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:gradFill flip="none" rotWithShape="1">
+            <a:gradFill rotWithShape="1">
               <a:gsLst>
                 <a:gs pos="0">
-                  <a:srgbClr val="DAFF01">
-                    <a:shade val="30000"/>
-                    <a:satMod val="115000"/>
-                  </a:srgbClr>
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
                 </a:gs>
                 <a:gs pos="50000">
-                  <a:srgbClr val="DAFF01">
-                    <a:shade val="67500"/>
-                    <a:satMod val="115000"/>
-                  </a:srgbClr>
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
                 </a:gs>
                 <a:gs pos="100000">
-                  <a:srgbClr val="DAFF01">
-                    <a:shade val="100000"/>
-                    <a:satMod val="115000"/>
-                  </a:srgbClr>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
                 </a:gs>
               </a:gsLst>
-              <a:path path="circle">
-                <a:fillToRect l="100000" b="100000"/>
-              </a:path>
-              <a:tileRect t="-100000" r="-100000"/>
+              <a:lin ang="5400000" scaled="0"/>
             </a:gradFill>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:alpha val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
@@ -2003,18 +2084,12 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" baseline="0">
-                    <a:ln w="0"/>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1"/>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
                     </a:solidFill>
-                    <a:effectLst>
-                      <a:outerShdw blurRad="38100" dist="19050" dir="2700000" algn="tl" rotWithShape="0">
-                        <a:schemeClr val="dk1">
-                          <a:alpha val="40000"/>
-                        </a:schemeClr>
-                      </a:outerShdw>
-                    </a:effectLst>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
                     <a:cs typeface="+mn-cs"/>
@@ -2038,9 +2113,9 @@
                   <c:spPr>
                     <a:ln w="9525">
                       <a:solidFill>
-                        <a:schemeClr val="dk1">
-                          <a:lumMod val="50000"/>
-                          <a:lumOff val="50000"/>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="95000"/>
+                          <a:alpha val="54000"/>
                         </a:schemeClr>
                       </a:solidFill>
                     </a:ln>
@@ -2100,7 +2175,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="65"/>
+        <c:gapWidth val="115"/>
+        <c:overlap val="-20"/>
         <c:axId val="2128186495"/>
         <c:axId val="2128678047"/>
       </c:barChart>
@@ -2117,11 +2193,11 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="dk1">
-                <a:lumMod val="75000"/>
-                <a:lumOff val="25000"/>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="54000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -2133,11 +2209,10 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="dk1">
-                    <a:lumMod val="75000"/>
-                    <a:lumOff val="25000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -2160,29 +2235,17 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="1"/>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:gradFill>
-                <a:gsLst>
-                  <a:gs pos="100000">
-                    <a:schemeClr val="dk1">
-                      <a:lumMod val="95000"/>
-                      <a:lumOff val="5000"/>
-                      <a:alpha val="42000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="0">
-                    <a:schemeClr val="lt1">
-                      <a:lumMod val="75000"/>
-                      <a:alpha val="36000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                </a:gsLst>
-                <a:lin ang="5400000" scaled="0"/>
-              </a:gradFill>
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -2192,6 +2255,32 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
         <c:crossAx val="2128186495"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
@@ -2212,30 +2301,487 @@
     <a:gradFill flip="none" rotWithShape="1">
       <a:gsLst>
         <a:gs pos="0">
-          <a:schemeClr val="lt1"/>
-        </a:gs>
-        <a:gs pos="39000">
-          <a:schemeClr val="lt1"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
         </a:gs>
         <a:gs pos="100000">
-          <a:schemeClr val="lt1">
-            <a:lumMod val="75000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
           </a:schemeClr>
         </a:gs>
       </a:gsLst>
       <a:path path="circle">
-        <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
       </a:path>
       <a:tileRect/>
     </a:gradFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="25000"/>
-          <a:lumOff val="75000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:gradFill flip="none" rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:srgbClr val="A2B9DA">
+                    <a:shade val="30000"/>
+                    <a:satMod val="115000"/>
+                  </a:srgbClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:srgbClr val="A2B9DA">
+                    <a:shade val="67500"/>
+                    <a:satMod val="115000"/>
+                  </a:srgbClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:srgbClr val="A2B9DA">
+                    <a:shade val="100000"/>
+                    <a:satMod val="115000"/>
+                  </a:srgbClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="8100000" scaled="1"/>
+              <a:tileRect/>
+            </a:gradFill>
+            <a:ln w="19050">
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="40000"/>
+                  <a:lumOff val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Base de Dados - Gráficos'!$E$3:$E$8</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Jan</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Fev</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Mar</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Abr</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Mai</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Jun</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Base de Dados - Gráficos'!$F$3:$F$8</c:f>
+              <c:numCache>
+                <c:formatCode>_("R$"* #,##0.00_);_("R$"* \(#,##0.00\);_("R$"* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2017.2600000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2336.13</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3099.24</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3649.1399999999994</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1727.1899999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3134.7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D264-4492-954F-4DC7351CEC28}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="422691439"/>
+        <c:axId val="335917215"/>
+      </c:barChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Base de Dados - Gráficos'!$E$3:$E$8</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Jan</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Fev</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Mar</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Abr</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Mai</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Jun</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Base de Dados - Gráficos'!$G$3:$G$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>31</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-D264-4492-954F-4DC7351CEC28}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="422697039"/>
+        <c:axId val="335916799"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="422691439"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="54000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="335917215"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="335917215"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="422691439"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="335916799"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="422697039"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="422697039"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="335916799"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
     </a:ln>
     <a:effectLst/>
   </c:spPr>
@@ -2298,6 +2844,46 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -2905,41 +3491,39 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="218">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="222">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" b="1" kern="1200"/>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200" cap="all" baseline="0"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
   <cs:chartArea>
     <cs:lnRef idx="0"/>
@@ -2952,160 +3536,124 @@
       <a:gradFill flip="none" rotWithShape="1">
         <a:gsLst>
           <a:gs pos="0">
-            <a:schemeClr val="lt1"/>
-          </a:gs>
-          <a:gs pos="39000">
-            <a:schemeClr val="lt1"/>
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
           </a:gs>
           <a:gs pos="100000">
-            <a:schemeClr val="lt1">
-              <a:lumMod val="75000"/>
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
             </a:schemeClr>
           </a:gs>
         </a:gsLst>
         <a:path path="circle">
-          <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
         </a:path>
         <a:tileRect/>
       </a:gradFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:dataLabel>
   <cs:dataLabelCallout>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-          <a:alpha val="75000"/>
-        </a:schemeClr>
+        <a:schemeClr val="lt1"/>
       </a:solidFill>
     </cs:spPr>
-    <cs:defRPr sz="900" b="1" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
       <a:spAutoFit/>
     </cs:bodyPr>
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr">
-          <a:alpha val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:alpha val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr">
-          <a:alpha val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:alpha val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="31750" cap="rnd">
+      <a:ln w="34925" cap="rnd">
         <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:alpha val="85000"/>
-          </a:schemeClr>
+          <a:schemeClr val="phClr"/>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointLine>
   <cs:dataPointMarker>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr">
-          <a:alpha val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointMarkerLayout size="5"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -3121,17 +3669,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -3143,20 +3690,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="50000"/>
-          <a:lumOff val="50000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -3167,14 +3714,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:prstDash val="dash"/>
@@ -3186,14 +3733,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -3205,7 +3751,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:floor>
   <cs:gridlineMajor>
@@ -3213,28 +3759,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="100000">
-              <a:schemeClr val="dk1">
-                <a:lumMod val="95000"/>
-                <a:lumOff val="5000"/>
-                <a:alpha val="42000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="0">
-              <a:schemeClr val="lt1">
-                <a:lumMod val="75000"/>
-                <a:alpha val="36000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
@@ -3244,28 +3778,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="100000">
-              <a:schemeClr val="dk1">
-                <a:lumMod val="95000"/>
-                <a:lumOff val="5000"/>
-                <a:alpha val="42000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="0">
-              <a:schemeClr val="lt1">
-                <a:lumMod val="75000"/>
-                <a:alpha val="36000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
       </a:ln>
     </cs:spPr>
   </cs:gridlineMinor>
@@ -3274,14 +3796,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:prstDash val="dash"/>
@@ -3293,14 +3815,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -3311,19 +3833,10 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1">
-          <a:lumMod val="95000"/>
-          <a:alpha val="39000"/>
-        </a:schemeClr>
-      </a:solidFill>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:legend>
   <cs:plotArea>
@@ -3331,7 +3844,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:plotArea>
   <cs:plotArea3D>
@@ -3339,7 +3852,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:plotArea3D>
   <cs:seriesAxis>
@@ -3347,17 +3860,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="31750" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -3370,14 +3882,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -3389,12 +3901,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1800" b="1" kern="1200" baseline="0"/>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -3403,7 +3922,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="19050" cap="rnd">
@@ -3418,9 +3937,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -3430,7 +3948,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -3438,9 +3956,9 @@
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -3451,16 +3969,10 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -3468,7 +3980,520 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="328">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
       <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill>
+        <a:gsLst>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="95000"/>
+              <a:lumOff val="5000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="75000"/>
+              <a:lumOff val="25000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+      </a:gradFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill>
+        <a:gsLst>
+          <a:gs pos="100000">
+            <a:schemeClr val="lt1">
+              <a:lumMod val="85000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="0">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+      </a:gradFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
@@ -3589,6 +4614,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>13142</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>6218</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>79</xdr:col>
+      <xdr:colOff>131646</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>108415</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C22A6C5C-4014-4499-98B5-6BA5F5BF9B55}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4183,37 +5244,37 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{40AC111B-A369-4C0B-9503-7C5B9442DAEA}" name="TB_Produtos" displayName="TB_Produtos" ref="A3:G42" headerRowDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{40AC111B-A369-4C0B-9503-7C5B9442DAEA}" name="TB_Produtos" displayName="TB_Produtos" ref="A3:G42" headerRowDxfId="20">
   <autoFilter ref="A3:G42" xr:uid="{40AC111B-A369-4C0B-9503-7C5B9442DAEA}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{2F8ED5FF-48A1-488E-9DF1-FE060F71A415}" name="Código" totalsRowLabel="Total"/>
     <tableColumn id="2" xr3:uid="{E100D4E2-C3A0-43FF-A1D9-90A4BC2A9918}" name="Produtos"/>
-    <tableColumn id="3" xr3:uid="{2EF7FEE0-6B6F-4534-86A0-46B6555B7BEF}" name="Tamanho" dataDxfId="18" totalsRowDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{2EF7FEE0-6B6F-4534-86A0-46B6555B7BEF}" name="Tamanho" dataDxfId="19" totalsRowDxfId="18"/>
     <tableColumn id="4" xr3:uid="{4435A4B8-E7F0-4D66-A4F8-6A9FEAA36D5A}" name="Categoria"/>
-    <tableColumn id="6" xr3:uid="{15F9CACC-A558-4A20-80CF-C2ADA2603221}" name="Estoque" dataDxfId="16" totalsRowDxfId="15"/>
-    <tableColumn id="7" xr3:uid="{3D723964-A53C-4456-A86F-04BE235E4F0C}" name="Situação" dataDxfId="14" totalsRowDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{CA8AD0DE-58EC-4839-85FB-1DD75DA28087}" name="Preço Unitário" totalsRowFunction="sum" dataDxfId="12" totalsRowDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{15F9CACC-A558-4A20-80CF-C2ADA2603221}" name="Estoque" dataDxfId="17" totalsRowDxfId="16"/>
+    <tableColumn id="7" xr3:uid="{3D723964-A53C-4456-A86F-04BE235E4F0C}" name="Situação" dataDxfId="15" totalsRowDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{CA8AD0DE-58EC-4839-85FB-1DD75DA28087}" name="Preço Unitário" totalsRowFunction="sum" dataDxfId="13" totalsRowDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{AD739091-30BD-4C30-BDDA-7504C0C4B6E2}" name="TB_Vendas" displayName="TB_Vendas" ref="A2:H61" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8" headerRowCellStyle="Cabeçalho Meteora">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{AD739091-30BD-4C30-BDDA-7504C0C4B6E2}" name="TB_Vendas" displayName="TB_Vendas" ref="A2:H61" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10" headerRowCellStyle="Cabeçalho Meteora">
   <autoFilter ref="A2:H61" xr:uid="{AD739091-30BD-4C30-BDDA-7504C0C4B6E2}"/>
   <tableColumns count="8">
-    <tableColumn id="7" xr3:uid="{5E8DE7C3-CDB6-4314-A5CC-C44D3C21973F}" name="Mês" dataDxfId="7">
+    <tableColumn id="7" xr3:uid="{5E8DE7C3-CDB6-4314-A5CC-C44D3C21973F}" name="Mês" dataDxfId="9">
       <calculatedColumnFormula>MONTH(TB_Vendas[[#This Row],[Data]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{43632F1F-6978-4CE7-BB13-7CCE587D6821}" name="Data" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{49DF5362-33BE-4541-BD47-0B512249381E}" name="Código" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{B3C718A1-FEFF-4C65-9CA1-DF94EF755918}" name="Tamanho" dataDxfId="4">
+    <tableColumn id="1" xr3:uid="{43632F1F-6978-4CE7-BB13-7CCE587D6821}" name="Data" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{49DF5362-33BE-4541-BD47-0B512249381E}" name="Código" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{B3C718A1-FEFF-4C65-9CA1-DF94EF755918}" name="Tamanho" dataDxfId="6">
       <calculatedColumnFormula>_xlfn.XLOOKUP(C3,TB_Produtos[Código],TB_Produtos[Tamanho])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{1F3EAF93-84E7-4086-BE54-3AB7D71B21A8}" name="Categoria" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{7DC2ADED-AF8A-4BC8-A38E-FEF676FE49C9}" name="Qtd" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{9459B662-6A4F-4486-82B1-12F67B8F842E}" name="Total" dataDxfId="1"/>
-    <tableColumn id="8" xr3:uid="{192FEBCA-1287-48A6-9BE6-69528F71C305}" name="Vendedor" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{1F3EAF93-84E7-4086-BE54-3AB7D71B21A8}" name="Categoria" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{7DC2ADED-AF8A-4BC8-A38E-FEF676FE49C9}" name="Qtd" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{9459B662-6A4F-4486-82B1-12F67B8F842E}" name="Total" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{192FEBCA-1287-48A6-9BE6-69528F71C305}" name="Vendedor" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5687,15 +6748,15 @@
     <mergeCell ref="A1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="F4:F42">
-    <cfRule type="cellIs" dxfId="20" priority="3" operator="lessThan">
-      <formula>3</formula>
-    </cfRule>
     <cfRule type="iconSet" priority="2">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="3"/>
         <cfvo type="num" val="10" gte="0"/>
       </iconSet>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="lessThan">
+      <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4:G42">
@@ -5740,8 +6801,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BF34D44-0E29-4A7F-B47B-66AF094D5F9D}">
   <dimension ref="A1:H61"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7451,7 +8512,7 @@
     <mergeCell ref="A1:H1"/>
   </mergeCells>
   <conditionalFormatting sqref="F2">
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7479,7 +8540,7 @@
   <dimension ref="C1:CB46"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" zoomScale="123" zoomScaleNormal="123" workbookViewId="0">
-      <selection activeCell="AO25" sqref="AO25"/>
+      <selection activeCell="C9" sqref="C9:CB10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.140625" defaultRowHeight="9.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -10785,28 +11846,32 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76A61A88-938B-4AD6-9405-2203B020D104}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.28515625" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>97</v>
       </c>
       <c r="B1" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>83</v>
       </c>
@@ -10814,8 +11879,20 @@
         <f>SUMIF(TB_Vendas[Vendedor],A2,TB_Vendas[Total])</f>
         <v>6102.4499999999989</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D2" s="88" t="s">
+        <v>99</v>
+      </c>
+      <c r="E2" s="88" t="s">
+        <v>100</v>
+      </c>
+      <c r="F2" s="88" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="88" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>84</v>
       </c>
@@ -10823,14 +11900,106 @@
         <f>SUMIF(TB_Vendas[Vendedor],A3,TB_Vendas[Total])</f>
         <v>4567.68</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F3" s="89">
+        <f>SUMIF(TB_Vendas[Mês],D3,TB_Vendas[Total])</f>
+        <v>2017.2600000000002</v>
+      </c>
+      <c r="G3">
+        <f>SUMIF(TB_Vendas[Mês],D3,TB_Vendas[Qtd])</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>86</v>
       </c>
       <c r="B4" s="28">
         <f>SUMIF(TB_Vendas[Vendedor],A4,TB_Vendas[Total])</f>
         <v>5293.5299999999988</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>102</v>
+      </c>
+      <c r="F4" s="89">
+        <f>SUMIF(TB_Vendas[Mês],D4,TB_Vendas[Total])</f>
+        <v>2336.13</v>
+      </c>
+      <c r="G4">
+        <f>SUMIF(TB_Vendas[Mês],D4,TB_Vendas[Qtd])</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>103</v>
+      </c>
+      <c r="F5" s="89">
+        <f>SUMIF(TB_Vendas[Mês],D5,TB_Vendas[Total])</f>
+        <v>3099.24</v>
+      </c>
+      <c r="G5">
+        <f>SUMIF(TB_Vendas[Mês],D5,TB_Vendas[Qtd])</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6" t="s">
+        <v>104</v>
+      </c>
+      <c r="F6" s="89">
+        <f>SUMIF(TB_Vendas[Mês],D6,TB_Vendas[Total])</f>
+        <v>3649.1399999999994</v>
+      </c>
+      <c r="G6">
+        <f>SUMIF(TB_Vendas[Mês],D6,TB_Vendas[Qtd])</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <v>5</v>
+      </c>
+      <c r="E7" t="s">
+        <v>105</v>
+      </c>
+      <c r="F7" s="89">
+        <f>SUMIF(TB_Vendas[Mês],D7,TB_Vendas[Total])</f>
+        <v>1727.1899999999998</v>
+      </c>
+      <c r="G7">
+        <f>SUMIF(TB_Vendas[Mês],D7,TB_Vendas[Qtd])</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <v>6</v>
+      </c>
+      <c r="E8" t="s">
+        <v>106</v>
+      </c>
+      <c r="F8" s="89">
+        <f>SUMIF(TB_Vendas[Mês],D8,TB_Vendas[Total])</f>
+        <v>3134.7</v>
+      </c>
+      <c r="G8">
+        <f>SUMIF(TB_Vendas[Mês],D8,TB_Vendas[Qtd])</f>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>